<commit_message>
Added scripts for BT and TopUp Product
</commit_message>
<xml_diff>
--- a/KMBAutomation/TestData/TestData_LeadDetails.xlsx
+++ b/KMBAutomation/TestData/TestData_LeadDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="7470" tabRatio="847" firstSheet="5" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="7470" tabRatio="847" firstSheet="8" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="TestScenario" sheetId="3" r:id="rId1"/>
@@ -16,15 +16,17 @@
     <sheet name="HLDAPSelfEmpIndividualHomeLoan" sheetId="9" r:id="rId7"/>
     <sheet name="HLDAPSelfEmpNonIndividualHomeLo" sheetId="10" r:id="rId8"/>
     <sheet name="HLDAPSalariedBalanceTransferInd" sheetId="11" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId10"/>
-    <sheet name="Output" sheetId="2" r:id="rId11"/>
+    <sheet name="HLDAPSalariedBalanceTransferNRI" sheetId="13" r:id="rId10"/>
+    <sheet name="HLDAPSalariedOnlyTopUpIndian" sheetId="14" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId12"/>
+    <sheet name="Output" sheetId="2" r:id="rId13"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="338">
   <si>
     <t>Username</t>
   </si>
@@ -1015,6 +1017,30 @@
   </si>
   <si>
     <t>20/06/2022 5:40 PM</t>
+  </si>
+  <si>
+    <t>HLDAPSalariedBalanceTransferNRI</t>
+  </si>
+  <si>
+    <t>TC08</t>
+  </si>
+  <si>
+    <t>TC09</t>
+  </si>
+  <si>
+    <t>HLDAPSalariedOnlyTopUpIndian</t>
+  </si>
+  <si>
+    <t>Only Top up</t>
+  </si>
+  <si>
+    <t>100000</t>
+  </si>
+  <si>
+    <t>9879879817</t>
+  </si>
+  <si>
+    <t xml:space="preserve">July </t>
   </si>
 </sst>
 </file>
@@ -1080,7 +1106,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1090,6 +1116,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1133,7 +1171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1168,11 +1206,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1489,10 +1529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1586,7 @@
       <c r="A4" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="31" t="s">
         <v>273</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -1558,7 +1598,7 @@
       <c r="A5" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="32" t="s">
         <v>272</v>
       </c>
       <c r="C5" s="22" t="s">
@@ -1570,7 +1610,7 @@
       <c r="A6" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="32" t="s">
         <v>286</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -1582,7 +1622,7 @@
       <c r="A7" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="32" t="s">
         <v>293</v>
       </c>
       <c r="C7" s="22" t="s">
@@ -1594,10 +1634,32 @@
       <c r="A8" s="25" t="s">
         <v>317</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="30" t="s">
         <v>318</v>
       </c>
       <c r="C8" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>333</v>
+      </c>
+      <c r="C10" s="25" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1619,6 +1681,1164 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CJ2"/>
+  <sheetViews>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AI2" sqref="AI2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="12.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="34.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="12" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="25" style="4" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" style="4" customWidth="1"/>
+    <col min="18" max="22" width="24" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="20.85546875" style="4" customWidth="1"/>
+    <col min="25" max="25" width="36.28515625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="29.140625" style="4" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="22.42578125" style="4" customWidth="1"/>
+    <col min="30" max="30" width="25.42578125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="17.85546875" style="4" customWidth="1"/>
+    <col min="32" max="32" width="16.7109375" style="4" customWidth="1"/>
+    <col min="33" max="34" width="27.5703125" style="4" customWidth="1"/>
+    <col min="35" max="35" width="16.7109375" style="4" customWidth="1"/>
+    <col min="36" max="36" width="11.140625" style="4" customWidth="1"/>
+    <col min="37" max="37" width="24.5703125" style="4" customWidth="1"/>
+    <col min="38" max="38" width="17.7109375" style="4" customWidth="1"/>
+    <col min="39" max="40" width="19.42578125" style="4" customWidth="1"/>
+    <col min="41" max="42" width="34.42578125" style="5" customWidth="1"/>
+    <col min="43" max="43" width="21.7109375" style="4" customWidth="1"/>
+    <col min="44" max="44" width="24.140625" style="4" customWidth="1"/>
+    <col min="45" max="45" width="26.7109375" style="4" customWidth="1"/>
+    <col min="46" max="47" width="19.140625" style="4" customWidth="1"/>
+    <col min="48" max="48" width="16.5703125" style="4" customWidth="1"/>
+    <col min="49" max="49" width="21.42578125" style="4" customWidth="1"/>
+    <col min="50" max="50" width="12.85546875" style="4" customWidth="1"/>
+    <col min="51" max="51" width="30.7109375" style="4" customWidth="1"/>
+    <col min="52" max="52" width="91.42578125" style="4" customWidth="1"/>
+    <col min="53" max="53" width="10.5703125" style="4" customWidth="1"/>
+    <col min="54" max="54" width="13" style="4" customWidth="1"/>
+    <col min="55" max="55" width="13.28515625" style="4" customWidth="1"/>
+    <col min="56" max="56" width="15.28515625" style="4" customWidth="1"/>
+    <col min="57" max="57" width="12.42578125" style="4" customWidth="1"/>
+    <col min="58" max="58" width="9.140625" style="4"/>
+    <col min="59" max="59" width="19.85546875" style="4" customWidth="1"/>
+    <col min="60" max="60" width="25.7109375" style="4" customWidth="1"/>
+    <col min="61" max="61" width="13.42578125" style="4" customWidth="1"/>
+    <col min="62" max="62" width="15" style="4" customWidth="1"/>
+    <col min="63" max="63" width="20.140625" style="4" customWidth="1"/>
+    <col min="64" max="64" width="21.7109375" style="4" customWidth="1"/>
+    <col min="65" max="65" width="17.28515625" style="4" customWidth="1"/>
+    <col min="66" max="66" width="17.85546875" style="4" customWidth="1"/>
+    <col min="67" max="67" width="32.5703125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="24.7109375" style="4" customWidth="1"/>
+    <col min="69" max="69" width="26.5703125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="32.7109375" style="4" customWidth="1"/>
+    <col min="71" max="71" width="18.42578125" style="4" customWidth="1"/>
+    <col min="72" max="72" width="17.85546875" style="4" customWidth="1"/>
+    <col min="73" max="73" width="17.140625" style="4" customWidth="1"/>
+    <col min="74" max="74" width="18.5703125" style="4" customWidth="1"/>
+    <col min="75" max="75" width="18.42578125" style="4" customWidth="1"/>
+    <col min="76" max="77" width="17.85546875" style="4" customWidth="1"/>
+    <col min="78" max="80" width="25.28515625" style="4" customWidth="1"/>
+    <col min="81" max="81" width="17.28515625" style="4" customWidth="1"/>
+    <col min="82" max="82" width="19.28515625" style="4" customWidth="1"/>
+    <col min="83" max="83" width="24.140625" style="4" customWidth="1"/>
+    <col min="84" max="84" width="16.28515625" style="4" customWidth="1"/>
+    <col min="85" max="85" width="16" style="4" customWidth="1"/>
+    <col min="86" max="86" width="19.42578125" style="4" customWidth="1"/>
+    <col min="87" max="87" width="19.85546875" style="4" customWidth="1"/>
+    <col min="88" max="88" width="17.5703125" style="4" customWidth="1"/>
+    <col min="89" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:88" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AO1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AP1" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AT1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AU1" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="AV1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AW1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AX1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AY1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AZ1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="BM1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BN1" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="CA1" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="CB1" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="CC1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="CD1" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="CE1" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>265</v>
+      </c>
+      <c r="CG1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CI1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:88" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="S2" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="T2" s="23">
+        <v>4200000</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>325</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AI2" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="AL2" s="17"/>
+      <c r="AM2" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="AN2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AO2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AP2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AQ2" s="17"/>
+      <c r="AR2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AS2" s="17"/>
+      <c r="AT2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AU2" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AW2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AX2" s="17"/>
+      <c r="AY2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AZ2" s="17"/>
+      <c r="BA2" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="BB2" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="BD2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BE2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="BF2" s="17"/>
+      <c r="BG2" s="17"/>
+      <c r="BH2" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="BI2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BJ2" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="BK2" s="17"/>
+      <c r="BL2" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="BM2" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="BN2" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="BX2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BY2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BZ2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="CA2" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="CB2" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="CC2" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="CD2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="CE2" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="CF2"/>
+      <c r="CG2"/>
+      <c r="CH2"/>
+      <c r="CI2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Y2">
+      <formula1>"Just Balance Transfer,Balance Transfer Plus TopUp"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2">
+      <formula1>"Residential,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S2">
+      <formula1>"BANK OF MAHARASHTRA,BANK OF INDIA,CITI BANK (CIT)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BH2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BQ2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
+      <formula1>"Buying new property,Buying resale property,Construction of property,Renovation of existing property"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CB2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AU5" sqref="AU5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="12.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="34.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="12" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="25" style="4" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" style="4" customWidth="1"/>
+    <col min="18" max="20" width="24" style="4" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" style="4" customWidth="1"/>
+    <col min="22" max="22" width="20.85546875" style="4" customWidth="1"/>
+    <col min="23" max="23" width="29.140625" style="4" customWidth="1"/>
+    <col min="24" max="24" width="16.7109375" style="4" customWidth="1"/>
+    <col min="25" max="26" width="27.5703125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" style="4" customWidth="1"/>
+    <col min="28" max="28" width="11.140625" style="4" customWidth="1"/>
+    <col min="29" max="29" width="24.5703125" style="4" customWidth="1"/>
+    <col min="30" max="30" width="17.7109375" style="4" customWidth="1"/>
+    <col min="31" max="32" width="19.42578125" style="4" customWidth="1"/>
+    <col min="33" max="34" width="34.42578125" style="5" customWidth="1"/>
+    <col min="35" max="35" width="21.7109375" style="4" customWidth="1"/>
+    <col min="36" max="36" width="24.140625" style="4" customWidth="1"/>
+    <col min="37" max="37" width="26.7109375" style="4" customWidth="1"/>
+    <col min="38" max="39" width="19.140625" style="4" customWidth="1"/>
+    <col min="40" max="40" width="16.5703125" style="4" customWidth="1"/>
+    <col min="41" max="41" width="21.42578125" style="4" customWidth="1"/>
+    <col min="42" max="42" width="12.85546875" style="4" customWidth="1"/>
+    <col min="43" max="43" width="30.7109375" style="4" customWidth="1"/>
+    <col min="44" max="44" width="35.42578125" style="4" customWidth="1"/>
+    <col min="45" max="45" width="10.5703125" style="4" customWidth="1"/>
+    <col min="46" max="46" width="13" style="4" customWidth="1"/>
+    <col min="47" max="47" width="13.28515625" style="4" customWidth="1"/>
+    <col min="48" max="48" width="15.28515625" style="4" customWidth="1"/>
+    <col min="49" max="49" width="12.42578125" style="4" customWidth="1"/>
+    <col min="50" max="50" width="9.140625" style="4"/>
+    <col min="51" max="51" width="19.85546875" style="4" customWidth="1"/>
+    <col min="52" max="52" width="25.7109375" style="4" customWidth="1"/>
+    <col min="53" max="53" width="13.42578125" style="4" customWidth="1"/>
+    <col min="54" max="54" width="15" style="4" customWidth="1"/>
+    <col min="55" max="55" width="20.140625" style="4" customWidth="1"/>
+    <col min="56" max="56" width="21.7109375" style="4" customWidth="1"/>
+    <col min="57" max="57" width="17.28515625" style="4" customWidth="1"/>
+    <col min="58" max="58" width="17.85546875" style="4" customWidth="1"/>
+    <col min="59" max="59" width="32.5703125" style="4" customWidth="1"/>
+    <col min="60" max="60" width="24.7109375" style="4" customWidth="1"/>
+    <col min="61" max="61" width="26.5703125" style="4" customWidth="1"/>
+    <col min="62" max="62" width="32.7109375" style="4" customWidth="1"/>
+    <col min="63" max="63" width="18.42578125" style="4" customWidth="1"/>
+    <col min="64" max="64" width="17.85546875" style="4" customWidth="1"/>
+    <col min="65" max="65" width="17.140625" style="4" customWidth="1"/>
+    <col min="66" max="66" width="18.5703125" style="4" customWidth="1"/>
+    <col min="67" max="67" width="18.42578125" style="4" customWidth="1"/>
+    <col min="68" max="69" width="17.85546875" style="4" customWidth="1"/>
+    <col min="70" max="72" width="25.28515625" style="4" customWidth="1"/>
+    <col min="73" max="73" width="17.28515625" style="4" customWidth="1"/>
+    <col min="74" max="74" width="19.28515625" style="4" customWidth="1"/>
+    <col min="75" max="75" width="24.140625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="16.28515625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="16" style="4" customWidth="1"/>
+    <col min="78" max="78" width="19.42578125" style="4" customWidth="1"/>
+    <col min="79" max="79" width="19.85546875" style="4" customWidth="1"/>
+    <col min="80" max="80" width="17.5703125" style="4" customWidth="1"/>
+    <col min="81" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:80" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AG1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AM1" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="AN1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AO1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AP1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AQ1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AR1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="AT1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="AU1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AV1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="AW1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="AX1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="BG1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BH1" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="BI1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BK1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="BX1" t="s">
+        <v>265</v>
+      </c>
+      <c r="BY1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:80" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>334</v>
+      </c>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="S2" s="23">
+        <v>2700000</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="V2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>200</v>
+      </c>
+      <c r="AA2" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="AF2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AG2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AH2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AI2" s="17"/>
+      <c r="AJ2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AK2" s="17"/>
+      <c r="AL2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AM2" s="17" t="s">
+        <v>256</v>
+      </c>
+      <c r="AN2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AO2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AP2" s="17"/>
+      <c r="AQ2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AR2" s="17"/>
+      <c r="AS2" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="AT2" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="AU2" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AW2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="AX2" s="17"/>
+      <c r="AY2" s="17"/>
+      <c r="AZ2" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="BA2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BB2" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="BC2" s="17"/>
+      <c r="BD2" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="BE2" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="BF2" s="17" t="s">
+        <v>335</v>
+      </c>
+      <c r="BG2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BH2" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="BI2" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="BJ2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BK2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="BL2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BM2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="BX2"/>
+      <c r="BY2"/>
+      <c r="BZ2"/>
+      <c r="CA2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2">
+      <formula1>"Residential,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT2">
+      <formula1>" January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -1659,27 +2879,27 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f ca="1">CONCATENATE("HLNew Lead"," ",RANDBETWEEN(1,999))</f>
-        <v>HLNew Lead 386</v>
+        <v>HLNew Lead 848</v>
       </c>
       <c r="B2" s="2">
         <f ca="1">RANDBETWEEN(6789000000,9999999999)</f>
-        <v>8248573667</v>
+        <v>7006561851</v>
       </c>
       <c r="C2" s="2" t="str">
         <f ca="1">CONCATENATE(SUBSTITUTE($A2," ",""),"@gmail.com")</f>
-        <v>HLNewLead386@gmail.com</v>
+        <v>HLNewLead848@gmail.com</v>
       </c>
       <c r="D2" s="2" t="str">
         <f ca="1">CONCATENATE(RANDBETWEEN(10,30),RANDBETWEEN(10,12),RANDBETWEEN(1951,2004))</f>
-        <v>24111978</v>
+        <v>23111959</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">CONCATENATE(CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),CHAR(RANDBETWEEN(65,90)))</f>
-        <v>JLTFS9511V</v>
+        <v>NLQBX9693A</v>
       </c>
       <c r="F2" s="4" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Male","Female")</f>
-        <v>Female</v>
+        <v>Male</v>
       </c>
     </row>
   </sheetData>
@@ -1687,7 +2907,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
@@ -2590,7 +3810,7 @@
   <dimension ref="A1:BW3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2931,18 +4151,18 @@
       <c r="L2" s="10"/>
       <c r="M2" s="12" t="str">
         <f ca="1">Sheet1!A2</f>
-        <v>HLNew Lead 386</v>
+        <v>HLNew Lead 848</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>174</v>
       </c>
       <c r="O2" s="10" t="str">
         <f ca="1">Sheet1!C2</f>
-        <v>HLNewLead386@gmail.com</v>
+        <v>HLNewLead848@gmail.com</v>
       </c>
       <c r="P2" s="10" t="str">
         <f ca="1">Sheet1!D2</f>
-        <v>24111978</v>
+        <v>23111959</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>76</v>
@@ -2977,7 +4197,7 @@
       <c r="AC2" s="10"/>
       <c r="AD2" s="10" t="str">
         <f ca="1">Sheet1!E2</f>
-        <v>JLTFS9511V</v>
+        <v>NLQBX9693A</v>
       </c>
       <c r="AE2" s="10" t="s">
         <v>36</v>
@@ -3083,7 +4303,7 @@
       <c r="N3" s="12" t="s">
         <v>274</v>
       </c>
-      <c r="O3" s="27" t="s">
+      <c r="O3" s="26" t="s">
         <v>168</v>
       </c>
       <c r="P3" s="17"/>
@@ -3270,7 +4490,7 @@
   <dimension ref="A1:BK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3525,7 +4745,7 @@
       <c r="A2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>302</v>
       </c>
       <c r="C2" s="10" t="s">
@@ -3561,18 +4781,18 @@
       <c r="M2" s="10"/>
       <c r="N2" s="12" t="str">
         <f ca="1">Sheet1!A2</f>
-        <v>HLNew Lead 386</v>
+        <v>HLNew Lead 848</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>174</v>
       </c>
       <c r="P2" s="10" t="str">
         <f ca="1">Sheet1!C2</f>
-        <v>HLNewLead386@gmail.com</v>
+        <v>HLNewLead848@gmail.com</v>
       </c>
       <c r="Q2" s="10" t="str">
         <f ca="1">Sheet1!D2</f>
-        <v>24111978</v>
+        <v>23111959</v>
       </c>
       <c r="R2" s="13" t="s">
         <v>76</v>
@@ -3607,7 +4827,7 @@
       <c r="AD2" s="10"/>
       <c r="AE2" s="10" t="str">
         <f ca="1">Sheet1!E2</f>
-        <v>JLTFS9511V</v>
+        <v>NLQBX9693A</v>
       </c>
       <c r="AF2" s="10" t="s">
         <v>36</v>
@@ -3700,7 +4920,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="28" t="s">
         <v>102</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -3708,7 +4928,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="27" t="s">
         <v>103</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3716,37 +4936,37 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="27" t="s">
         <v>104</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="27" t="s">
         <v>106</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>105</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="28" t="s">
+      <c r="A6" s="27" t="s">
         <v>108</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="27" t="s">
         <v>109</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>107</v>
       </c>
       <c r="B8" s="2"/>
@@ -3762,7 +4982,7 @@
   <dimension ref="A1:CG2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4342,7 +5562,7 @@
   <dimension ref="A1:CC2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S1048576"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6045,8 +7265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CB1" workbookViewId="0">
-      <selection activeCell="CI7" sqref="CI7"/>
+    <sheetView topLeftCell="BJ1" workbookViewId="0">
+      <selection activeCell="BJ2" sqref="BJ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added script for Top Up Self Employed
</commit_message>
<xml_diff>
--- a/KMBAutomation/TestData/TestData_LeadDetails.xlsx
+++ b/KMBAutomation/TestData/TestData_LeadDetails.xlsx
@@ -4,32 +4,34 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="7470" tabRatio="847" firstSheet="8" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="7470" tabRatio="847" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TestScenario" sheetId="3" r:id="rId1"/>
     <sheet name="HLNewLead" sheetId="1" r:id="rId2"/>
     <sheet name="CRMHLLeadGeneration" sheetId="7" r:id="rId3"/>
     <sheet name="SecuredCCDAP" sheetId="5" r:id="rId4"/>
-    <sheet name="HLDAPSalariedHomeLoanIndian" sheetId="6" r:id="rId5"/>
-    <sheet name="HLDAPSalariedHomeLoanNRI" sheetId="8" r:id="rId6"/>
-    <sheet name="HLDAPSelfEmpIndividualHomeLoan" sheetId="9" r:id="rId7"/>
-    <sheet name="HLDAPSelfEmpNonIndividualHomeLo" sheetId="10" r:id="rId8"/>
-    <sheet name="HLDAPSalariedBalanceTransferInd" sheetId="11" r:id="rId9"/>
-    <sheet name="HLDAPSalariedBalanceTransferNRI" sheetId="13" r:id="rId10"/>
-    <sheet name="HLDAPIndividualBalTransfer" sheetId="16" r:id="rId11"/>
-    <sheet name="HLDAPNonIndividualBalTransfer" sheetId="17" r:id="rId12"/>
-    <sheet name="HLDAPSalariedOnlyTopUpIndian" sheetId="14" r:id="rId13"/>
-    <sheet name="HLDAPSalariedOnlyTopUpNRI" sheetId="15" r:id="rId14"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId15"/>
-    <sheet name="Output" sheetId="2" r:id="rId16"/>
+    <sheet name="HLDAPHomeLoanSalariedIndian" sheetId="6" r:id="rId5"/>
+    <sheet name="HLDAPHomeLoanSalariedNRI" sheetId="8" r:id="rId6"/>
+    <sheet name="HLDAPHomeLoanIndividual" sheetId="9" r:id="rId7"/>
+    <sheet name="HLDAPHomeLoanNonIndividual" sheetId="10" r:id="rId8"/>
+    <sheet name="HLDAPBalTransferSalariedInd" sheetId="11" r:id="rId9"/>
+    <sheet name="HLDAPBalanceTransferSalariedNRI" sheetId="13" r:id="rId10"/>
+    <sheet name="HLDAPBalanceTransferIndividual" sheetId="16" r:id="rId11"/>
+    <sheet name="HLDAPBalTransferNonIndividual" sheetId="17" r:id="rId12"/>
+    <sheet name="HLDAPOnlyTopUpSalariedIndian" sheetId="14" r:id="rId13"/>
+    <sheet name="HLDAPOnlyTopUpSalariedNRI" sheetId="15" r:id="rId14"/>
+    <sheet name="HLDAPOnlyTopUpIndividual" sheetId="18" r:id="rId15"/>
+    <sheet name="HLDAPOnlyTopUpNonIndividual" sheetId="19" r:id="rId16"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId17"/>
+    <sheet name="Output" sheetId="2" r:id="rId18"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2070" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="360">
   <si>
     <t>Username</t>
   </si>
@@ -845,12 +847,6 @@
     <t>TC04</t>
   </si>
   <si>
-    <t>HLDAPSalariedHomeLoanNRI</t>
-  </si>
-  <si>
-    <t>HLDAPSalariedHomeLoanIndian</t>
-  </si>
-  <si>
     <t>9879879818</t>
   </si>
   <si>
@@ -884,9 +880,6 @@
     <t>TC05</t>
   </si>
   <si>
-    <t>HLDAPSelfEmpIndividualHomeLoan</t>
-  </si>
-  <si>
     <t>Self employed</t>
   </si>
   <si>
@@ -905,9 +898,6 @@
     <t>TC06</t>
   </si>
   <si>
-    <t>HLDAPSelfEmpNonIndividualHomeLoan</t>
-  </si>
-  <si>
     <t>Non-Individual</t>
   </si>
   <si>
@@ -935,9 +925,6 @@
     <t>https://kmb.crmnext.com/sng7/app/login/login</t>
   </si>
   <si>
-    <t>Natraj Pvt Ltd</t>
-  </si>
-  <si>
     <t>9879879825</t>
   </si>
   <si>
@@ -974,9 +961,6 @@
     <t>TC07</t>
   </si>
   <si>
-    <t>HLDAPSalariedBalanceTransferIndian</t>
-  </si>
-  <si>
     <t>Balance Transfer/BT+Top up</t>
   </si>
   <si>
@@ -1004,18 +988,12 @@
     <t>500000</t>
   </si>
   <si>
-    <t>HLDAPSalariedBalanceTransferNRI</t>
-  </si>
-  <si>
     <t>TC08</t>
   </si>
   <si>
     <t>TC09</t>
   </si>
   <si>
-    <t>HLDAPSalariedOnlyTopUpIndian</t>
-  </si>
-  <si>
     <t>Only Top up</t>
   </si>
   <si>
@@ -1043,18 +1021,9 @@
     <t>22/06/2022 3:32 PM</t>
   </si>
   <si>
-    <t>HLDAPSalariedOnlyTopUpNRI</t>
-  </si>
-  <si>
     <t>TC10</t>
   </si>
   <si>
-    <t>HLDAPSelfEmpIndividualBalTransfer</t>
-  </si>
-  <si>
-    <t>HLDAPSelfEmpNonIndividualBalTransfer</t>
-  </si>
-  <si>
     <t>TC11</t>
   </si>
   <si>
@@ -1064,15 +1033,9 @@
     <t>TC13</t>
   </si>
   <si>
-    <t>HLDAPSelfEmpIndividualOnlyTopUp</t>
-  </si>
-  <si>
     <t>TC14</t>
   </si>
   <si>
-    <t>HLDAPSelfEmpNonIndividualOnlyTopUp</t>
-  </si>
-  <si>
     <t>00104517</t>
   </si>
   <si>
@@ -1082,28 +1045,73 @@
     <t>April</t>
   </si>
   <si>
-    <t>00104612</t>
-  </si>
-  <si>
-    <t>24/06/2022 12:36 PM</t>
-  </si>
-  <si>
-    <t>00104628</t>
-  </si>
-  <si>
-    <t>24/06/2022 3:36 PM</t>
-  </si>
-  <si>
-    <t>24/06/2022 3:42 PM</t>
-  </si>
-  <si>
     <t>00104637</t>
   </si>
   <si>
-    <t>24/06/2022 4:34 PM</t>
-  </si>
-  <si>
     <t>24/06/2022 4:39 PM</t>
+  </si>
+  <si>
+    <t>V Creations</t>
+  </si>
+  <si>
+    <t>HLDAPOnlyTopUpIndividual</t>
+  </si>
+  <si>
+    <t>HLDAPOnlyTopUpNonIndividual</t>
+  </si>
+  <si>
+    <t>HLDAPOnlyTopUpSalariedIndian</t>
+  </si>
+  <si>
+    <t>HLDAPOnlyTopUpSalariedNRI</t>
+  </si>
+  <si>
+    <t>HLDAPHomeLoanSalariedIndian</t>
+  </si>
+  <si>
+    <t>HLDAPHomeLoanSalariedNRI</t>
+  </si>
+  <si>
+    <t>HLDAPHomeLoanIndividual</t>
+  </si>
+  <si>
+    <t>HLDAPHomeLoanNonIndividual</t>
+  </si>
+  <si>
+    <t>HLDAPBalanceTransferSalariedIndian</t>
+  </si>
+  <si>
+    <t>HLDAPBalanceTransferSalariedNRI</t>
+  </si>
+  <si>
+    <t>HLDAPBalanceTransferIndividual</t>
+  </si>
+  <si>
+    <t>HLDAPBalanceTransferNonIndividual</t>
+  </si>
+  <si>
+    <t>00104724</t>
+  </si>
+  <si>
+    <t>27/06/2022 2:02 PM</t>
+  </si>
+  <si>
+    <t>00104727</t>
+  </si>
+  <si>
+    <t>27/06/2022 3:03 PM</t>
+  </si>
+  <si>
+    <t>00104730</t>
+  </si>
+  <si>
+    <t>27/06/2022 3:27 PM</t>
+  </si>
+  <si>
+    <t>00104751</t>
+  </si>
+  <si>
+    <t>27/06/2022 3:54 PM</t>
   </si>
 </sst>
 </file>
@@ -1648,7 +1656,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1703,7 +1711,7 @@
         <v>101</v>
       </c>
       <c r="B4" s="39" t="s">
-        <v>272</v>
+        <v>344</v>
       </c>
       <c r="C4" s="22" t="s">
         <v>100</v>
@@ -1715,7 +1723,7 @@
         <v>270</v>
       </c>
       <c r="B5" s="39" t="s">
-        <v>271</v>
+        <v>345</v>
       </c>
       <c r="C5" s="22" t="s">
         <v>100</v>
@@ -1724,10 +1732,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B6" s="29" t="s">
-        <v>284</v>
+        <v>346</v>
       </c>
       <c r="C6" s="22" t="s">
         <v>100</v>
@@ -1736,10 +1744,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>291</v>
+        <v>347</v>
       </c>
       <c r="C7" s="22" t="s">
         <v>100</v>
@@ -1748,10 +1756,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>314</v>
+        <v>348</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>100</v>
@@ -1759,21 +1767,21 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>324</v>
+        <v>349</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>339</v>
+        <v>350</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>100</v>
@@ -1781,10 +1789,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B11" s="28" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>100</v>
@@ -1792,10 +1800,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="B12" s="38" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="C12" s="42" t="s">
         <v>100</v>
@@ -1803,10 +1811,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>337</v>
+        <v>343</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>100</v>
@@ -1814,21 +1822,21 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="B14" s="38" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>100</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
       <c r="B15" s="38" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>100</v>
@@ -1868,8 +1876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1960,7 +1968,7 @@
         <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>72</v>
@@ -2014,16 +2022,16 @@
         <v>18</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>200</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="X1" s="7" t="s">
         <v>19</v>
@@ -2032,10 +2040,10 @@
         <v>20</v>
       </c>
       <c r="Z1" s="7" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="AA1" s="7" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="AB1" s="7" t="s">
         <v>24</v>
@@ -2188,16 +2196,16 @@
         <v>222</v>
       </c>
       <c r="BZ1" s="3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="CA1" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="CB1" s="3" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="CC1" s="3" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="CD1" s="3" t="s">
         <v>228</v>
@@ -2226,10 +2234,10 @@
     </row>
     <row r="2" spans="1:89" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17" t="s">
@@ -2247,7 +2255,7 @@
         <v>22</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
@@ -2267,28 +2275,28 @@
         <v>100</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="U2" s="24" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="V2" s="23" t="s">
         <v>201</v>
       </c>
       <c r="W2" s="23" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="Y2" s="17" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="Z2" s="17" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="AA2" s="17" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="AD2" s="17"/>
       <c r="AE2" s="17"/>
@@ -2348,7 +2356,7 @@
         <v>155</v>
       </c>
       <c r="BC2" s="17" t="s">
-        <v>349</v>
+        <v>336</v>
       </c>
       <c r="BD2" s="17" t="s">
         <v>266</v>
@@ -2362,7 +2370,7 @@
       <c r="BG2" s="17"/>
       <c r="BH2" s="17"/>
       <c r="BI2" s="17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="BJ2" s="17" t="s">
         <v>268</v>
@@ -2417,10 +2425,10 @@
         <v>166</v>
       </c>
       <c r="CB2" s="4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="CC2" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="CD2" s="4" t="s">
         <v>230</v>
@@ -2435,13 +2443,13 @@
         <v>260</v>
       </c>
       <c r="CH2" t="s">
-        <v>355</v>
+        <v>337</v>
       </c>
       <c r="CI2" t="s">
         <v>83</v>
       </c>
       <c r="CJ2" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
     </row>
   </sheetData>
@@ -2490,10 +2498,637 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CL2"/>
+  <sheetViews>
+    <sheetView topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="AW24" sqref="AW24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="4" width="9.140625"/>
+    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
+    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
+    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
+    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
+    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
+    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
+    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
+    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
+    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
+    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
+    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
+    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
+    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
+    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
+    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
+    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
+    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
+    <col min="19" max="23" customWidth="true" style="4" width="24.0"/>
+    <col min="24" max="24" customWidth="true" style="4" width="15.7109375"/>
+    <col min="25" max="25" customWidth="true" style="4" width="20.85546875"/>
+    <col min="26" max="26" customWidth="true" style="4" width="36.28515625"/>
+    <col min="27" max="27" customWidth="true" style="4" width="29.140625"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
+    <col min="30" max="30" customWidth="true" style="4" width="22.42578125"/>
+    <col min="31" max="31" customWidth="true" style="4" width="25.42578125"/>
+    <col min="32" max="32" customWidth="true" style="4" width="17.85546875"/>
+    <col min="33" max="33" customWidth="true" style="4" width="16.7109375"/>
+    <col min="34" max="35" customWidth="true" style="4" width="27.5703125"/>
+    <col min="36" max="36" customWidth="true" style="4" width="16.7109375"/>
+    <col min="37" max="37" customWidth="true" style="4" width="11.140625"/>
+    <col min="38" max="38" customWidth="true" style="4" width="24.5703125"/>
+    <col min="39" max="39" customWidth="true" style="4" width="17.7109375"/>
+    <col min="40" max="41" customWidth="true" style="4" width="19.42578125"/>
+    <col min="42" max="43" customWidth="true" style="5" width="34.42578125"/>
+    <col min="44" max="44" customWidth="true" style="4" width="21.7109375"/>
+    <col min="45" max="45" customWidth="true" style="4" width="24.140625"/>
+    <col min="46" max="47" customWidth="true" style="4" width="26.7109375"/>
+    <col min="48" max="49" customWidth="true" style="4" width="19.140625"/>
+    <col min="50" max="50" customWidth="true" style="4" width="16.5703125"/>
+    <col min="51" max="51" customWidth="true" style="4" width="21.42578125"/>
+    <col min="52" max="52" customWidth="true" style="4" width="12.85546875"/>
+    <col min="53" max="53" customWidth="true" style="4" width="30.7109375"/>
+    <col min="54" max="54" customWidth="true" style="4" width="39.5703125"/>
+    <col min="55" max="55" customWidth="true" style="4" width="10.5703125"/>
+    <col min="56" max="56" customWidth="true" style="4" width="13.0"/>
+    <col min="57" max="57" customWidth="true" style="4" width="13.28515625"/>
+    <col min="58" max="58" customWidth="true" style="4" width="15.28515625"/>
+    <col min="59" max="59" customWidth="true" style="4" width="12.42578125"/>
+    <col min="60" max="60" style="4" width="9.140625"/>
+    <col min="61" max="61" customWidth="true" style="4" width="19.85546875"/>
+    <col min="62" max="62" customWidth="true" style="4" width="25.7109375"/>
+    <col min="63" max="63" customWidth="true" style="4" width="13.42578125"/>
+    <col min="64" max="64" customWidth="true" style="4" width="15.0"/>
+    <col min="65" max="65" customWidth="true" style="4" width="20.140625"/>
+    <col min="66" max="66" customWidth="true" style="4" width="21.7109375"/>
+    <col min="67" max="67" customWidth="true" style="4" width="17.28515625"/>
+    <col min="68" max="68" customWidth="true" style="4" width="17.85546875"/>
+    <col min="69" max="69" customWidth="true" style="4" width="32.5703125"/>
+    <col min="70" max="70" customWidth="true" style="4" width="24.7109375"/>
+    <col min="71" max="71" customWidth="true" style="4" width="26.5703125"/>
+    <col min="72" max="72" customWidth="true" style="4" width="32.7109375"/>
+    <col min="73" max="73" customWidth="true" style="4" width="18.42578125"/>
+    <col min="74" max="74" customWidth="true" style="4" width="17.85546875"/>
+    <col min="75" max="75" customWidth="true" style="4" width="17.140625"/>
+    <col min="76" max="76" customWidth="true" style="4" width="18.5703125"/>
+    <col min="77" max="77" customWidth="true" style="4" width="18.42578125"/>
+    <col min="78" max="79" customWidth="true" style="4" width="17.85546875"/>
+    <col min="80" max="82" customWidth="true" style="4" width="25.28515625"/>
+    <col min="83" max="83" customWidth="true" style="4" width="17.28515625"/>
+    <col min="84" max="84" customWidth="true" style="4" width="19.28515625"/>
+    <col min="85" max="85" customWidth="true" style="4" width="24.140625"/>
+    <col min="86" max="86" customWidth="true" style="4" width="16.28515625"/>
+    <col min="87" max="87" customWidth="true" style="4" width="16.0"/>
+    <col min="88" max="88" customWidth="true" style="4" width="19.42578125"/>
+    <col min="89" max="89" customWidth="true" style="4" width="19.85546875"/>
+    <col min="90" max="90" customWidth="true" style="4" width="17.5703125"/>
+    <col min="91" max="16384" style="4" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:90" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AP1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AQ1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AU1" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="AV1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AW1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AY1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AZ1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="BA1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="BB1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BM1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BN1" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="BO1" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="BP1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="CA1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="CB1" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="CC1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="CD1" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="CE1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="CF1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="CG1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>264</v>
+      </c>
+      <c r="CI1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="CJ1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CK1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CL1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:90" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="17" t="s">
+        <v>313</v>
+      </c>
+      <c r="U2" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="W2" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="Z2" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="AA2" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AJ2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AK2" s="17"/>
+      <c r="AL2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AM2" s="17"/>
+      <c r="AN2" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="AO2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AP2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AQ2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AR2" s="17"/>
+      <c r="AS2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AT2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AU2" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AW2" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="AX2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AY2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AZ2" s="17"/>
+      <c r="BA2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="BB2" s="17"/>
+      <c r="BC2" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="BD2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="BE2" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="BF2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BG2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="BH2" s="17"/>
+      <c r="BI2" s="17"/>
+      <c r="BJ2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="BK2" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="BL2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BM2" s="17"/>
+      <c r="BN2" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="BO2" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="BP2" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BX2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BY2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BZ2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="CA2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="CB2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="CC2" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="CD2" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="CE2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="CF2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="CG2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="CH2"/>
+      <c r="CI2"/>
+      <c r="CJ2"/>
+      <c r="CK2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2">
+      <formula1>"Just Balance Transfer,Balance Transfer Plus TopUp"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
+      <formula1>"Residential,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2">
+      <formula1>"BANK OF MAHARASHTRA,BANK OF INDIA,CITI BANK (CIT)"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BT2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BS2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2">
+      <formula1>"Buying new property,Buying resale property,Construction of property,Renovation of existing property"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BD2">
+      <formula1>" January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU2">
+      <formula1>"Less than 3 years,3 or more years"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CK2"/>
   <sheetViews>
     <sheetView topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BC6" sqref="BC6"/>
+      <selection activeCell="BF20" sqref="BF20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,7 +3177,7 @@
     <col min="50" max="50" customWidth="true" style="4" width="21.42578125"/>
     <col min="51" max="51" customWidth="true" style="4" width="12.85546875"/>
     <col min="52" max="52" customWidth="true" style="4" width="30.7109375"/>
-    <col min="53" max="53" customWidth="true" style="4" width="91.42578125"/>
+    <col min="53" max="53" customWidth="true" style="4" width="18.140625"/>
     <col min="54" max="54" customWidth="true" style="4" width="10.5703125"/>
     <col min="55" max="55" customWidth="true" style="4" width="13.0"/>
     <col min="56" max="56" customWidth="true" style="4" width="13.28515625"/>
@@ -2584,7 +3219,7 @@
         <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>72</v>
@@ -2638,16 +3273,16 @@
         <v>18</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>200</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="X1" s="7" t="s">
         <v>19</v>
@@ -2656,10 +3291,10 @@
         <v>20</v>
       </c>
       <c r="Z1" s="7" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="AA1" s="7" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="AB1" s="7" t="s">
         <v>24</v>
@@ -2812,16 +3447,16 @@
         <v>222</v>
       </c>
       <c r="BZ1" s="3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="CA1" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="CB1" s="3" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="CC1" s="3" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="CD1" s="3" t="s">
         <v>228</v>
@@ -2850,10 +3485,10 @@
     </row>
     <row r="2" spans="1:89" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17" t="s">
@@ -2868,10 +3503,10 @@
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
@@ -2891,28 +3526,28 @@
         <v>100</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="U2" s="24" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="V2" s="23" t="s">
         <v>201</v>
       </c>
       <c r="W2" s="23" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="Y2" s="17" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="Z2" s="17" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="AA2" s="17" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="AD2" s="17"/>
       <c r="AE2" s="17"/>
@@ -2951,7 +3586,7 @@
         <v>94</v>
       </c>
       <c r="AT2" s="17" t="s">
-        <v>50</v>
+        <v>288</v>
       </c>
       <c r="AU2" s="17" t="s">
         <v>226</v>
@@ -2974,7 +3609,7 @@
         <v>155</v>
       </c>
       <c r="BC2" s="17" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="BD2" s="17" t="s">
         <v>156</v>
@@ -2986,7 +3621,9 @@
         <v>130</v>
       </c>
       <c r="BG2" s="17"/>
-      <c r="BH2" s="17"/>
+      <c r="BH2" s="17" t="s">
+        <v>339</v>
+      </c>
       <c r="BI2" s="17" t="s">
         <v>246</v>
       </c>
@@ -3043,628 +3680,10 @@
         <v>166</v>
       </c>
       <c r="CB2" s="4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="CC2" s="4" t="s">
-        <v>310</v>
-      </c>
-      <c r="CD2" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="CE2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="CF2" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="CG2"/>
-      <c r="CH2"/>
-      <c r="CI2"/>
-      <c r="CJ2"/>
-    </row>
-  </sheetData>
-  <dataValidations count="11">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Z2">
-      <formula1>"Just Balance Transfer,Balance Transfer Plus TopUp"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
-      <formula1>"Residential,Commercial"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2">
-      <formula1>"BANK OF MAHARASHTRA,BANK OF INDIA,CITI BANK (CIT)"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
-      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
-      <formula1>"RM,DST"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BI2">
-      <formula1>"Indian,NRI"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2">
-      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BS2">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2">
-      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2">
-      <formula1>"Buying new property,Buying resale property,Construction of property,Renovation of existing property"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BC2">
-      <formula1>" January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CK2"/>
-  <sheetViews>
-    <sheetView topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BA5" sqref="BA5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="23" customWidth="true" style="4" width="24.0"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.7109375"/>
-    <col min="25" max="25" customWidth="true" style="4" width="20.85546875"/>
-    <col min="26" max="26" customWidth="true" style="4" width="36.28515625"/>
-    <col min="27" max="27" customWidth="true" style="4" width="29.140625"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
-    <col min="30" max="30" customWidth="true" style="4" width="22.42578125"/>
-    <col min="31" max="31" customWidth="true" style="4" width="25.42578125"/>
-    <col min="32" max="32" customWidth="true" style="4" width="17.85546875"/>
-    <col min="33" max="33" customWidth="true" style="4" width="16.7109375"/>
-    <col min="34" max="35" customWidth="true" style="4" width="27.5703125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="16.7109375"/>
-    <col min="37" max="37" customWidth="true" style="4" width="11.140625"/>
-    <col min="38" max="38" customWidth="true" style="4" width="24.5703125"/>
-    <col min="39" max="39" customWidth="true" style="4" width="17.7109375"/>
-    <col min="40" max="41" customWidth="true" style="4" width="19.42578125"/>
-    <col min="42" max="43" customWidth="true" style="5" width="34.42578125"/>
-    <col min="44" max="44" customWidth="true" style="4" width="21.7109375"/>
-    <col min="45" max="45" customWidth="true" style="4" width="24.140625"/>
-    <col min="46" max="46" customWidth="true" style="4" width="26.7109375"/>
-    <col min="47" max="48" customWidth="true" style="4" width="19.140625"/>
-    <col min="49" max="49" customWidth="true" style="4" width="16.5703125"/>
-    <col min="50" max="50" customWidth="true" style="4" width="21.42578125"/>
-    <col min="51" max="51" customWidth="true" style="4" width="12.85546875"/>
-    <col min="52" max="52" customWidth="true" style="4" width="30.7109375"/>
-    <col min="53" max="53" customWidth="true" style="4" width="91.42578125"/>
-    <col min="54" max="54" customWidth="true" style="4" width="10.5703125"/>
-    <col min="55" max="55" customWidth="true" style="4" width="13.0"/>
-    <col min="56" max="56" customWidth="true" style="4" width="13.28515625"/>
-    <col min="57" max="57" customWidth="true" style="4" width="15.28515625"/>
-    <col min="58" max="58" customWidth="true" style="4" width="12.42578125"/>
-    <col min="59" max="59" style="4" width="9.140625"/>
-    <col min="60" max="60" customWidth="true" style="4" width="19.85546875"/>
-    <col min="61" max="61" customWidth="true" style="4" width="25.7109375"/>
-    <col min="62" max="62" customWidth="true" style="4" width="13.42578125"/>
-    <col min="63" max="63" customWidth="true" style="4" width="15.0"/>
-    <col min="64" max="64" customWidth="true" style="4" width="20.140625"/>
-    <col min="65" max="65" customWidth="true" style="4" width="21.7109375"/>
-    <col min="66" max="66" customWidth="true" style="4" width="17.28515625"/>
-    <col min="67" max="67" customWidth="true" style="4" width="17.85546875"/>
-    <col min="68" max="68" customWidth="true" style="4" width="32.5703125"/>
-    <col min="69" max="69" customWidth="true" style="4" width="24.7109375"/>
-    <col min="70" max="70" customWidth="true" style="4" width="26.5703125"/>
-    <col min="71" max="71" customWidth="true" style="4" width="32.7109375"/>
-    <col min="72" max="72" customWidth="true" style="4" width="18.42578125"/>
-    <col min="73" max="73" customWidth="true" style="4" width="17.85546875"/>
-    <col min="74" max="74" customWidth="true" style="4" width="17.140625"/>
-    <col min="75" max="75" customWidth="true" style="4" width="18.5703125"/>
-    <col min="76" max="76" customWidth="true" style="4" width="18.42578125"/>
-    <col min="77" max="78" customWidth="true" style="4" width="17.85546875"/>
-    <col min="79" max="81" customWidth="true" style="4" width="25.28515625"/>
-    <col min="82" max="82" customWidth="true" style="4" width="17.28515625"/>
-    <col min="83" max="83" customWidth="true" style="4" width="19.28515625"/>
-    <col min="84" max="84" customWidth="true" style="4" width="24.140625"/>
-    <col min="85" max="85" customWidth="true" style="4" width="16.28515625"/>
-    <col min="86" max="86" customWidth="true" style="4" width="16.0"/>
-    <col min="87" max="87" customWidth="true" style="4" width="19.42578125"/>
-    <col min="88" max="88" customWidth="true" style="4" width="19.85546875"/>
-    <col min="89" max="89" customWidth="true" style="4" width="17.5703125"/>
-    <col min="90" max="16384" style="4" width="9.140625"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:89" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y1" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z1" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="AA1" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="AB1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="AG1" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH1" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="AI1" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="AJ1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="AK1" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL1" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AM1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="AO1" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="AP1" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="AQ1" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="AR1" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="AS1" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="AT1" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="AU1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="AV1" s="7" t="s">
-        <v>225</v>
-      </c>
-      <c r="AW1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AX1" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="AY1" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="AZ1" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="BA1" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="BB1" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="BC1" s="16" t="s">
-        <v>112</v>
-      </c>
-      <c r="BD1" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="BE1" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="BF1" s="16" t="s">
-        <v>129</v>
-      </c>
-      <c r="BG1" s="16" t="s">
-        <v>102</v>
-      </c>
-      <c r="BH1" s="16" t="s">
-        <v>131</v>
-      </c>
-      <c r="BI1" s="16" t="s">
-        <v>134</v>
-      </c>
-      <c r="BJ1" s="16" t="s">
-        <v>137</v>
-      </c>
-      <c r="BK1" s="16" t="s">
-        <v>138</v>
-      </c>
-      <c r="BL1" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="BM1" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="BN1" s="16" t="s">
-        <v>162</v>
-      </c>
-      <c r="BO1" s="16" t="s">
-        <v>163</v>
-      </c>
-      <c r="BP1" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="BQ1" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="BR1" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="BS1" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="BT1" s="3" t="s">
-        <v>213</v>
-      </c>
-      <c r="BU1" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="BV1" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="BW1" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="BX1" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="BY1" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="BZ1" s="3" t="s">
         <v>305</v>
-      </c>
-      <c r="CA1" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="CB1" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="CC1" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="CD1" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="CE1" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="CF1" s="3" t="s">
-        <v>244</v>
-      </c>
-      <c r="CG1" t="s">
-        <v>264</v>
-      </c>
-      <c r="CH1" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="CI1" t="s">
-        <v>56</v>
-      </c>
-      <c r="CJ1" t="s">
-        <v>57</v>
-      </c>
-      <c r="CK1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:89" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>326</v>
-      </c>
-      <c r="B2" s="30" t="s">
-        <v>300</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17" t="s">
-        <v>285</v>
-      </c>
-      <c r="J2" s="17" t="s">
-        <v>315</v>
-      </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>260</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="17"/>
-      <c r="S2" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="T2" s="17" t="s">
-        <v>319</v>
-      </c>
-      <c r="U2" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="V2" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="W2" s="23" t="s">
-        <v>298</v>
-      </c>
-      <c r="X2" s="17" t="s">
-        <v>296</v>
-      </c>
-      <c r="Y2" s="17" t="s">
-        <v>318</v>
-      </c>
-      <c r="Z2" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="AA2" s="17" t="s">
-        <v>323</v>
-      </c>
-      <c r="AD2" s="17"/>
-      <c r="AE2" s="17"/>
-      <c r="AF2" s="17"/>
-      <c r="AG2" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>197</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AJ2" s="17" t="s">
-        <v>159</v>
-      </c>
-      <c r="AK2" s="17"/>
-      <c r="AL2" s="17" t="s">
-        <v>227</v>
-      </c>
-      <c r="AM2" s="17"/>
-      <c r="AN2" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="AO2" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="AP2" s="20" t="s">
-        <v>153</v>
-      </c>
-      <c r="AQ2" s="20" t="s">
-        <v>154</v>
-      </c>
-      <c r="AR2" s="17"/>
-      <c r="AS2" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="AT2" s="17" t="s">
-        <v>292</v>
-      </c>
-      <c r="AU2" s="17" t="s">
-        <v>226</v>
-      </c>
-      <c r="AV2" s="17" t="s">
-        <v>255</v>
-      </c>
-      <c r="AW2" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="AX2" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="AY2" s="17"/>
-      <c r="AZ2" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="BA2" s="17"/>
-      <c r="BB2" s="17" t="s">
-        <v>155</v>
-      </c>
-      <c r="BC2" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="BD2" s="17" t="s">
-        <v>156</v>
-      </c>
-      <c r="BE2" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="BF2" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="BG2" s="17"/>
-      <c r="BH2" s="17"/>
-      <c r="BI2" s="17" t="s">
-        <v>246</v>
-      </c>
-      <c r="BJ2" s="17" t="s">
-        <v>268</v>
-      </c>
-      <c r="BK2" s="17" t="s">
-        <v>269</v>
-      </c>
-      <c r="BL2" s="17"/>
-      <c r="BM2" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="BN2" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="BO2" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="BP2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="BQ2" s="4" t="s">
-        <v>206</v>
-      </c>
-      <c r="BR2" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="BS2" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="BT2" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="BU2" s="4" t="s">
-        <v>218</v>
-      </c>
-      <c r="BV2" s="4" t="s">
-        <v>219</v>
-      </c>
-      <c r="BW2" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="BX2" s="4" t="s">
-        <v>224</v>
-      </c>
-      <c r="BY2" s="4" t="s">
-        <v>223</v>
-      </c>
-      <c r="BZ2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="CA2" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="CB2" s="4" t="s">
-        <v>308</v>
-      </c>
-      <c r="CC2" s="4" t="s">
-        <v>310</v>
       </c>
       <c r="CD2" s="4" t="s">
         <v>230</v>
@@ -3729,7 +3748,7 @@
   <dimension ref="A1:CC2"/>
   <sheetViews>
     <sheetView topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AU2" sqref="AU2"/>
+      <selection activeCell="AR21" sqref="AR21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3814,7 +3833,7 @@
         <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>72</v>
@@ -3868,7 +3887,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>200</v>
@@ -3880,7 +3899,7 @@
         <v>20</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="Y1" s="7" t="s">
         <v>33</v>
@@ -4018,16 +4037,16 @@
         <v>222</v>
       </c>
       <c r="BR1" s="3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="BS1" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="BT1" s="3" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="BU1" s="3" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="BV1" s="3" t="s">
         <v>228</v>
@@ -4056,10 +4075,10 @@
     </row>
     <row r="2" spans="1:81" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17" t="s">
@@ -4077,7 +4096,7 @@
         <v>22</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
@@ -4086,7 +4105,7 @@
         <v>166</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>167</v>
@@ -4097,19 +4116,19 @@
         <v>100</v>
       </c>
       <c r="T2" s="24" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="U2" s="23" t="s">
         <v>201</v>
       </c>
       <c r="V2" s="17" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="W2" s="17" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="Y2" s="17" t="s">
         <v>34</v>
@@ -4166,7 +4185,7 @@
         <v>155</v>
       </c>
       <c r="AU2" s="17" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="AV2" s="17" t="s">
         <v>266</v>
@@ -4196,7 +4215,7 @@
         <v>164</v>
       </c>
       <c r="BG2" s="17" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="BH2" s="4" t="s">
         <v>49</v>
@@ -4235,10 +4254,10 @@
         <v>166</v>
       </c>
       <c r="BT2" s="4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="BU2" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="BV2" s="4" t="s">
         <v>230</v>
@@ -4259,7 +4278,7 @@
         <v>83</v>
       </c>
       <c r="CB2" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -4302,7 +4321,7 @@
   <dimension ref="A1:CC2"/>
   <sheetViews>
     <sheetView topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AU2" sqref="AU2"/>
+      <selection activeCell="AS24" sqref="AS24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4387,7 +4406,7 @@
         <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>72</v>
@@ -4441,7 +4460,7 @@
         <v>18</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>200</v>
@@ -4453,7 +4472,7 @@
         <v>20</v>
       </c>
       <c r="X1" s="7" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="Y1" s="7" t="s">
         <v>33</v>
@@ -4591,16 +4610,16 @@
         <v>222</v>
       </c>
       <c r="BR1" s="3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="BS1" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="BT1" s="3" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="BU1" s="3" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="BV1" s="3" t="s">
         <v>228</v>
@@ -4629,10 +4648,10 @@
     </row>
     <row r="2" spans="1:81" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17" t="s">
@@ -4650,7 +4669,7 @@
         <v>22</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
@@ -4659,7 +4678,7 @@
         <v>166</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>167</v>
@@ -4670,7 +4689,7 @@
         <v>100</v>
       </c>
       <c r="T2" s="24" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="U2" s="23" t="s">
         <v>201</v>
@@ -4679,10 +4698,10 @@
         <v>202</v>
       </c>
       <c r="W2" s="17" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="Y2" s="17" t="s">
         <v>34</v>
@@ -4739,7 +4758,7 @@
         <v>265</v>
       </c>
       <c r="AU2" s="17" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="AV2" s="17" t="s">
         <v>266</v>
@@ -4753,7 +4772,7 @@
       <c r="AY2" s="17"/>
       <c r="AZ2" s="17"/>
       <c r="BA2" s="17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="BB2" s="17" t="s">
         <v>268</v>
@@ -4769,7 +4788,7 @@
         <v>164</v>
       </c>
       <c r="BG2" s="17" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="BH2" s="4" t="s">
         <v>49</v>
@@ -4808,10 +4827,10 @@
         <v>166</v>
       </c>
       <c r="BT2" s="4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="BU2" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="BV2" s="4" t="s">
         <v>230</v>
@@ -4863,6 +4882,1167 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CD2"/>
+  <sheetViews>
+    <sheetView topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AL17" sqref="AL17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="4" width="9.140625"/>
+    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
+    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
+    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
+    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
+    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
+    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
+    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
+    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
+    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
+    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
+    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
+    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
+    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
+    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
+    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
+    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
+    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
+    <col min="19" max="21" customWidth="true" style="4" width="24.0"/>
+    <col min="22" max="22" customWidth="true" style="4" width="15.7109375"/>
+    <col min="23" max="23" customWidth="true" style="4" width="20.85546875"/>
+    <col min="24" max="24" customWidth="true" style="4" width="29.140625"/>
+    <col min="25" max="25" customWidth="true" style="4" width="16.7109375"/>
+    <col min="26" max="27" customWidth="true" style="4" width="27.5703125"/>
+    <col min="28" max="28" customWidth="true" style="4" width="16.7109375"/>
+    <col min="29" max="29" customWidth="true" style="4" width="11.140625"/>
+    <col min="30" max="30" customWidth="true" style="4" width="24.5703125"/>
+    <col min="31" max="31" customWidth="true" style="4" width="17.7109375"/>
+    <col min="32" max="33" customWidth="true" style="4" width="19.42578125"/>
+    <col min="34" max="35" customWidth="true" style="5" width="34.42578125"/>
+    <col min="36" max="36" customWidth="true" style="4" width="21.7109375"/>
+    <col min="37" max="37" customWidth="true" style="4" width="24.140625"/>
+    <col min="38" max="39" customWidth="true" style="4" width="26.7109375"/>
+    <col min="40" max="41" customWidth="true" style="4" width="19.140625"/>
+    <col min="42" max="42" customWidth="true" style="4" width="16.5703125"/>
+    <col min="43" max="43" customWidth="true" style="4" width="21.42578125"/>
+    <col min="44" max="44" customWidth="true" style="4" width="12.85546875"/>
+    <col min="45" max="45" customWidth="true" style="4" width="30.7109375"/>
+    <col min="46" max="46" customWidth="true" style="4" width="35.42578125"/>
+    <col min="47" max="47" customWidth="true" style="4" width="10.5703125"/>
+    <col min="48" max="48" customWidth="true" style="4" width="13.0"/>
+    <col min="49" max="49" customWidth="true" style="4" width="13.28515625"/>
+    <col min="50" max="50" customWidth="true" style="4" width="15.28515625"/>
+    <col min="51" max="51" customWidth="true" style="4" width="12.42578125"/>
+    <col min="52" max="52" style="4" width="9.140625"/>
+    <col min="53" max="53" customWidth="true" style="4" width="19.85546875"/>
+    <col min="54" max="54" customWidth="true" style="4" width="25.7109375"/>
+    <col min="55" max="55" customWidth="true" style="4" width="13.42578125"/>
+    <col min="56" max="56" customWidth="true" style="4" width="15.0"/>
+    <col min="57" max="57" customWidth="true" style="4" width="20.140625"/>
+    <col min="58" max="58" customWidth="true" style="4" width="21.7109375"/>
+    <col min="59" max="59" customWidth="true" style="4" width="17.28515625"/>
+    <col min="60" max="60" customWidth="true" style="4" width="17.85546875"/>
+    <col min="61" max="61" customWidth="true" style="4" width="32.5703125"/>
+    <col min="62" max="62" customWidth="true" style="4" width="24.7109375"/>
+    <col min="63" max="63" customWidth="true" style="4" width="26.5703125"/>
+    <col min="64" max="64" customWidth="true" style="4" width="32.7109375"/>
+    <col min="65" max="65" customWidth="true" style="4" width="18.42578125"/>
+    <col min="66" max="66" customWidth="true" style="4" width="17.85546875"/>
+    <col min="67" max="67" customWidth="true" style="4" width="17.140625"/>
+    <col min="68" max="68" customWidth="true" style="4" width="18.5703125"/>
+    <col min="69" max="69" customWidth="true" style="4" width="18.42578125"/>
+    <col min="70" max="71" customWidth="true" style="4" width="17.85546875"/>
+    <col min="72" max="74" customWidth="true" style="4" width="25.28515625"/>
+    <col min="75" max="75" customWidth="true" style="4" width="17.28515625"/>
+    <col min="76" max="76" customWidth="true" style="4" width="19.28515625"/>
+    <col min="77" max="77" customWidth="true" style="4" width="24.140625"/>
+    <col min="78" max="78" customWidth="true" style="4" width="16.28515625"/>
+    <col min="79" max="79" customWidth="true" style="4" width="16.0"/>
+    <col min="80" max="80" customWidth="true" style="4" width="19.42578125"/>
+    <col min="81" max="81" customWidth="true" style="4" width="19.85546875"/>
+    <col min="82" max="82" customWidth="true" style="4" width="17.5703125"/>
+    <col min="83" max="16384" style="4" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:82" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM1" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AP1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="AV1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="AW1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AX1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BI1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BK1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>264</v>
+      </c>
+      <c r="CA1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:82" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="V2" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AH2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AI2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM2" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="AN2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AO2" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="AP2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR2" s="17"/>
+      <c r="AS2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT2" s="17"/>
+      <c r="AU2" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="AW2" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="AX2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AY2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ2" s="17"/>
+      <c r="BA2" s="17"/>
+      <c r="BB2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="BD2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BE2" s="17"/>
+      <c r="BF2" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="BG2" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="BH2" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="BI2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BJ2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="BK2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="BL2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BM2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="BX2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>327</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>358</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>83</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2">
+      <formula1>" January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BL2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2">
+      <formula1>"Residential,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
+      <formula1>"Less than 3 years,3 or more years"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CD2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="4" width="9.140625"/>
+    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
+    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
+    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
+    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
+    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
+    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
+    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
+    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
+    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
+    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
+    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
+    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
+    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
+    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
+    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
+    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
+    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
+    <col min="19" max="21" customWidth="true" style="4" width="24.0"/>
+    <col min="22" max="22" customWidth="true" style="4" width="15.7109375"/>
+    <col min="23" max="23" customWidth="true" style="4" width="20.85546875"/>
+    <col min="24" max="24" customWidth="true" style="4" width="29.140625"/>
+    <col min="25" max="25" customWidth="true" style="4" width="16.7109375"/>
+    <col min="26" max="27" customWidth="true" style="4" width="27.5703125"/>
+    <col min="28" max="28" customWidth="true" style="4" width="16.7109375"/>
+    <col min="29" max="29" customWidth="true" style="4" width="11.140625"/>
+    <col min="30" max="30" customWidth="true" style="4" width="24.5703125"/>
+    <col min="31" max="31" customWidth="true" style="4" width="17.7109375"/>
+    <col min="32" max="33" customWidth="true" style="4" width="19.42578125"/>
+    <col min="34" max="35" customWidth="true" style="5" width="34.42578125"/>
+    <col min="36" max="36" customWidth="true" style="4" width="21.7109375"/>
+    <col min="37" max="37" customWidth="true" style="4" width="24.140625"/>
+    <col min="38" max="39" customWidth="true" style="4" width="26.7109375"/>
+    <col min="40" max="41" customWidth="true" style="4" width="19.140625"/>
+    <col min="42" max="42" customWidth="true" style="4" width="16.5703125"/>
+    <col min="43" max="43" customWidth="true" style="4" width="21.42578125"/>
+    <col min="44" max="44" customWidth="true" style="4" width="12.85546875"/>
+    <col min="45" max="45" customWidth="true" style="4" width="30.7109375"/>
+    <col min="46" max="46" customWidth="true" style="4" width="35.42578125"/>
+    <col min="47" max="47" customWidth="true" style="4" width="10.5703125"/>
+    <col min="48" max="48" customWidth="true" style="4" width="13.0"/>
+    <col min="49" max="49" customWidth="true" style="4" width="13.28515625"/>
+    <col min="50" max="50" customWidth="true" style="4" width="15.28515625"/>
+    <col min="51" max="51" customWidth="true" style="4" width="12.42578125"/>
+    <col min="52" max="52" customWidth="true" style="4" width="17.7109375"/>
+    <col min="53" max="54" customWidth="true" style="4" width="25.7109375"/>
+    <col min="55" max="55" customWidth="true" style="4" width="13.42578125"/>
+    <col min="56" max="56" customWidth="true" style="4" width="15.0"/>
+    <col min="57" max="57" customWidth="true" style="4" width="20.140625"/>
+    <col min="58" max="58" customWidth="true" style="4" width="21.7109375"/>
+    <col min="59" max="59" customWidth="true" style="4" width="17.28515625"/>
+    <col min="60" max="60" customWidth="true" style="4" width="17.85546875"/>
+    <col min="61" max="61" customWidth="true" style="4" width="32.5703125"/>
+    <col min="62" max="62" customWidth="true" style="4" width="24.7109375"/>
+    <col min="63" max="63" customWidth="true" style="4" width="26.5703125"/>
+    <col min="64" max="64" customWidth="true" style="4" width="32.7109375"/>
+    <col min="65" max="65" customWidth="true" style="4" width="18.42578125"/>
+    <col min="66" max="66" customWidth="true" style="4" width="17.85546875"/>
+    <col min="67" max="67" customWidth="true" style="4" width="17.140625"/>
+    <col min="68" max="68" customWidth="true" style="4" width="18.5703125"/>
+    <col min="69" max="69" customWidth="true" style="4" width="18.42578125"/>
+    <col min="70" max="71" customWidth="true" style="4" width="17.85546875"/>
+    <col min="72" max="74" customWidth="true" style="4" width="25.28515625"/>
+    <col min="75" max="75" customWidth="true" style="4" width="17.28515625"/>
+    <col min="76" max="76" customWidth="true" style="4" width="19.28515625"/>
+    <col min="77" max="77" customWidth="true" style="4" width="24.140625"/>
+    <col min="78" max="78" customWidth="true" style="4" width="16.28515625"/>
+    <col min="79" max="79" customWidth="true" style="4" width="16.0"/>
+    <col min="80" max="80" customWidth="true" style="4" width="19.42578125"/>
+    <col min="81" max="81" customWidth="true" style="4" width="19.85546875"/>
+    <col min="82" max="82" customWidth="true" style="4" width="17.5703125"/>
+    <col min="83" max="16384" style="4" width="9.140625"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:82" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM1" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AP1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="AV1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="AW1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AX1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BI1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BK1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>264</v>
+      </c>
+      <c r="CA1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="CB1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:82" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>327</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="V2" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AH2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AI2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="AM2" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="AN2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AO2" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="AP2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR2" s="17"/>
+      <c r="AS2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT2" s="17"/>
+      <c r="AU2" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="AW2" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="AX2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AY2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ2" s="17"/>
+      <c r="BA2" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="BB2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="BD2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BE2" s="17"/>
+      <c r="BF2" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="BG2" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="BH2" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="BI2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BJ2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="BK2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="BL2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BM2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="BX2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="BY2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="BZ2"/>
+      <c r="CA2"/>
+      <c r="CB2"/>
+      <c r="CC2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
+      <formula1>"Less than 3 years,3 or more years"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2">
+      <formula1>"Residential,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BL2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2">
+      <formula1>" January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -4903,27 +6083,27 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f ca="1">CONCATENATE("HLNew Lead"," ",RANDBETWEEN(1,999))</f>
-        <v>HLNew Lead 395</v>
+        <v>HLNew Lead 864</v>
       </c>
       <c r="B2" s="2">
         <f ca="1">RANDBETWEEN(6789000000,9999999999)</f>
-        <v>8300537878</v>
+        <v>8770801242</v>
       </c>
       <c r="C2" s="2" t="str">
         <f ca="1">CONCATENATE(SUBSTITUTE($A2," ",""),"@gmail.com")</f>
-        <v>HLNewLead395@gmail.com</v>
+        <v>HLNewLead864@gmail.com</v>
       </c>
       <c r="D2" s="2" t="str">
         <f ca="1">CONCATENATE(RANDBETWEEN(10,30),RANDBETWEEN(10,12),RANDBETWEEN(1951,2004))</f>
-        <v>17111978</v>
+        <v>19101970</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">CONCATENATE(CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),CHAR(RANDBETWEEN(65,90)))</f>
-        <v>KLLQH5474I</v>
+        <v>IFGAT4632N</v>
       </c>
       <c r="F2" s="4" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Male","Female")</f>
-        <v>Male</v>
+        <v>Female</v>
       </c>
     </row>
   </sheetData>
@@ -4931,7 +6111,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
@@ -5760,16 +6940,16 @@
         <v>270</v>
       </c>
       <c r="B47" t="s">
+        <v>271</v>
+      </c>
+      <c r="C47" t="s">
         <v>273</v>
-      </c>
-      <c r="C47" t="s">
-        <v>275</v>
       </c>
       <c r="D47" t="s">
         <v>83</v>
       </c>
       <c r="E47" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -5777,16 +6957,16 @@
         <v>270</v>
       </c>
       <c r="B48" t="s">
+        <v>271</v>
+      </c>
+      <c r="C48" t="s">
         <v>273</v>
-      </c>
-      <c r="C48" t="s">
-        <v>275</v>
       </c>
       <c r="D48" t="s">
         <v>83</v>
       </c>
       <c r="E48" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -5794,16 +6974,16 @@
         <v>270</v>
       </c>
       <c r="B49" t="s">
+        <v>271</v>
+      </c>
+      <c r="C49" t="s">
         <v>273</v>
-      </c>
-      <c r="C49" t="s">
-        <v>275</v>
       </c>
       <c r="D49" t="s">
         <v>83</v>
       </c>
       <c r="E49" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -5811,16 +6991,16 @@
         <v>270</v>
       </c>
       <c r="B50" t="s">
+        <v>277</v>
+      </c>
+      <c r="C50" t="s">
         <v>279</v>
-      </c>
-      <c r="C50" t="s">
-        <v>281</v>
       </c>
       <c r="D50" t="s">
         <v>83</v>
       </c>
       <c r="E50" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -5834,7 +7014,7 @@
   <dimension ref="A1:BW3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6175,18 +7355,18 @@
       <c r="L2" s="10"/>
       <c r="M2" s="12" t="str">
         <f ca="1">Sheet1!A2</f>
-        <v>HLNew Lead 395</v>
+        <v>HLNew Lead 864</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>173</v>
       </c>
       <c r="O2" s="10" t="str">
         <f ca="1">Sheet1!C2</f>
-        <v>HLNewLead395@gmail.com</v>
+        <v>HLNewLead864@gmail.com</v>
       </c>
       <c r="P2" s="10" t="str">
         <f ca="1">Sheet1!D2</f>
-        <v>17111978</v>
+        <v>19101970</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>76</v>
@@ -6221,7 +7401,7 @@
       <c r="AC2" s="10"/>
       <c r="AD2" s="10" t="str">
         <f ca="1">Sheet1!E2</f>
-        <v>KLLQH5474I</v>
+        <v>IFGAT4632N</v>
       </c>
       <c r="AE2" s="10" t="s">
         <v>36</v>
@@ -6281,7 +7461,7 @@
       <c r="BB2" s="17"/>
       <c r="BC2" s="17"/>
       <c r="BD2" s="17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="BE2" s="17" t="s">
         <v>268</v>
@@ -6325,7 +7505,7 @@
         <v>166</v>
       </c>
       <c r="N3" s="12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="O3" s="26" t="s">
         <v>167</v>
@@ -6419,7 +7599,7 @@
       <c r="BB3" s="17"/>
       <c r="BC3" s="17"/>
       <c r="BD3" s="17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="BE3" s="17" t="s">
         <v>268</v>
@@ -6597,7 +7777,7 @@
         <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>72</v>
@@ -6770,13 +7950,13 @@
         <v>71</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>73</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>2</v>
@@ -6805,18 +7985,18 @@
       <c r="M2" s="10"/>
       <c r="N2" s="12" t="str">
         <f ca="1">Sheet1!A2</f>
-        <v>HLNew Lead 395</v>
+        <v>HLNew Lead 864</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>173</v>
       </c>
       <c r="P2" s="10" t="str">
         <f ca="1">Sheet1!C2</f>
-        <v>HLNewLead395@gmail.com</v>
+        <v>HLNewLead864@gmail.com</v>
       </c>
       <c r="Q2" s="10" t="str">
         <f ca="1">Sheet1!D2</f>
-        <v>17111978</v>
+        <v>19101970</v>
       </c>
       <c r="R2" s="13" t="s">
         <v>76</v>
@@ -6851,7 +8031,7 @@
       <c r="AD2" s="10"/>
       <c r="AE2" s="10" t="str">
         <f ca="1">Sheet1!E2</f>
-        <v>KLLQH5474I</v>
+        <v>IFGAT4632N</v>
       </c>
       <c r="AF2" s="10" t="s">
         <v>36</v>
@@ -6932,7 +8112,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6947,7 +8127,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="B1" s="32" t="s">
         <v>102</v>
@@ -6958,7 +8138,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B2" s="35" t="s">
         <v>103</v>
@@ -6969,7 +8149,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B3" s="35" t="s">
         <v>104</v>
@@ -6978,7 +8158,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="36" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B4" s="35" t="s">
         <v>106</v>
@@ -6987,7 +8167,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="36" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B5" s="35" t="s">
         <v>105</v>
@@ -6996,7 +8176,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="36" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B6" s="35" t="s">
         <v>108</v>
@@ -7005,7 +8185,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="36" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B7" s="35" t="s">
         <v>109</v>
@@ -7014,7 +8194,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="36" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="B8" s="35" t="s">
         <v>107</v>
@@ -7035,7 +8215,7 @@
   <dimension ref="A1:CH2"/>
   <sheetViews>
     <sheetView topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="AX7" sqref="AX7"/>
+      <selection activeCell="AX21" sqref="AX21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7124,7 +8304,7 @@
         <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>72</v>
@@ -7181,10 +8361,10 @@
         <v>200</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="W1" s="7" t="s">
         <v>19</v>
@@ -7343,16 +8523,16 @@
         <v>222</v>
       </c>
       <c r="BW1" s="3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="BX1" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="BY1" s="3" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="BZ1" s="3" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="CA1" s="3" t="s">
         <v>228</v>
@@ -7384,7 +8564,7 @@
         <v>101</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17" t="s">
@@ -7411,7 +8591,7 @@
         <v>166</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>167</v>
@@ -7492,7 +8672,7 @@
         <v>155</v>
       </c>
       <c r="AZ2" s="17" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="BA2" s="17" t="s">
         <v>156</v>
@@ -7561,10 +8741,10 @@
         <v>166</v>
       </c>
       <c r="BY2" s="4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="BZ2" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="CA2" s="4" t="s">
         <v>230</v>
@@ -7576,16 +8756,16 @@
         <v>245</v>
       </c>
       <c r="CD2" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="CE2" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="CF2" t="s">
         <v>83</v>
       </c>
       <c r="CG2" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -7627,9 +8807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AX9" sqref="AX9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7716,7 +8894,7 @@
         <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>72</v>
@@ -7770,13 +8948,13 @@
         <v>18</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>200</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="W1" s="7" t="s">
         <v>19</v>
@@ -7964,7 +9142,7 @@
         <v>270</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17" t="s">
@@ -7991,7 +9169,7 @@
         <v>166</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>167</v>
@@ -8008,7 +9186,7 @@
         <v>201</v>
       </c>
       <c r="V2" s="23" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="W2" s="17" t="s">
         <v>202</v>
@@ -8076,7 +9254,7 @@
         <v>265</v>
       </c>
       <c r="AZ2" s="17" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="BA2" s="17" t="s">
         <v>266</v>
@@ -8090,7 +9268,7 @@
       <c r="BD2" s="17"/>
       <c r="BE2" s="17"/>
       <c r="BF2" s="17" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="BG2" s="17" t="s">
         <v>268</v>
@@ -8148,16 +9326,16 @@
         <v>245</v>
       </c>
       <c r="BZ2" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="CA2" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="CB2" t="s">
         <v>83</v>
       </c>
       <c r="CC2" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -8199,8 +9377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF2"/>
   <sheetViews>
-    <sheetView topLeftCell="AU1" workbookViewId="0">
-      <selection activeCell="BB2" sqref="BB2"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
+      <selection activeCell="AU18" sqref="AU18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8288,7 +9466,7 @@
         <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>72</v>
@@ -8345,13 +9523,13 @@
         <v>18</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>200</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="X1" s="7" t="s">
         <v>19</v>
@@ -8417,7 +9595,7 @@
         <v>53</v>
       </c>
       <c r="AS1" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="AT1" s="7" t="s">
         <v>59</v>
@@ -8539,10 +9717,10 @@
     </row>
     <row r="2" spans="1:84" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17" t="s">
@@ -8557,7 +9735,7 @@
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>23</v>
@@ -8589,7 +9767,7 @@
         <v>201</v>
       </c>
       <c r="W2" s="23" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="X2" s="17" t="s">
         <v>202</v>
@@ -8637,7 +9815,7 @@
         <v>50</v>
       </c>
       <c r="AS2" s="17" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="AT2" s="17" t="s">
         <v>226</v>
@@ -8660,7 +9838,7 @@
         <v>155</v>
       </c>
       <c r="BB2" s="17" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="BC2" s="17" t="s">
         <v>266</v>
@@ -8684,10 +9862,10 @@
       </c>
       <c r="BK2" s="17"/>
       <c r="BL2" s="17" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="BM2" s="17" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="BN2" s="17" t="s">
         <v>165</v>
@@ -8777,8 +9955,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF2"/>
   <sheetViews>
-    <sheetView topLeftCell="BA1" workbookViewId="0">
-      <selection activeCell="BA2" sqref="BA2"/>
+    <sheetView topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="BH23" sqref="BH23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8867,7 +10045,7 @@
         <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>72</v>
@@ -8921,13 +10099,13 @@
         <v>18</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>200</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="W1" s="7" t="s">
         <v>19</v>
@@ -8993,7 +10171,7 @@
         <v>53</v>
       </c>
       <c r="AR1" s="7" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="AS1" s="7" t="s">
         <v>59</v>
@@ -9050,10 +10228,10 @@
         <v>142</v>
       </c>
       <c r="BK1" s="16" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="BL1" s="16" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="BM1" s="16" t="s">
         <v>162</v>
@@ -9118,10 +10296,10 @@
     </row>
     <row r="2" spans="1:84" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17" t="s">
@@ -9136,7 +10314,7 @@
       </c>
       <c r="H2" s="17"/>
       <c r="I2" s="17" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>23</v>
@@ -9165,10 +10343,10 @@
         <v>201</v>
       </c>
       <c r="V2" s="23" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="W2" s="17" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="X2" s="17"/>
       <c r="Y2" s="17"/>
@@ -9210,10 +10388,10 @@
         <v>94</v>
       </c>
       <c r="AQ2" s="17" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="AR2" s="17" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="AS2" s="17" t="s">
         <v>226</v>
@@ -9236,7 +10414,7 @@
         <v>155</v>
       </c>
       <c r="BA2" s="17" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="BB2" s="17" t="s">
         <v>156</v>
@@ -9249,7 +10427,7 @@
       </c>
       <c r="BE2" s="17"/>
       <c r="BF2" s="17" t="s">
-        <v>301</v>
+        <v>339</v>
       </c>
       <c r="BG2" s="17" t="s">
         <v>246</v>
@@ -9262,13 +10440,13 @@
       </c>
       <c r="BJ2" s="17"/>
       <c r="BK2" s="17" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="BL2" s="17" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="BM2" s="17" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="BN2" s="17" t="s">
         <v>165</v>
@@ -9316,13 +10494,13 @@
         <v>260</v>
       </c>
       <c r="CC2" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="CD2" t="s">
         <v>83</v>
       </c>
       <c r="CE2" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -9371,7 +10549,7 @@
   <dimension ref="A1:CK2"/>
   <sheetViews>
     <sheetView topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="BC2" sqref="BC2"/>
+      <selection activeCell="BA23" sqref="BA23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9461,7 +10639,7 @@
         <v>74</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C1" s="7" t="s">
         <v>72</v>
@@ -9515,16 +10693,16 @@
         <v>18</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>200</v>
       </c>
       <c r="W1" s="7" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="X1" s="7" t="s">
         <v>19</v>
@@ -9533,10 +10711,10 @@
         <v>20</v>
       </c>
       <c r="Z1" s="7" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="AA1" s="7" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="AB1" s="7" t="s">
         <v>24</v>
@@ -9689,16 +10867,16 @@
         <v>222</v>
       </c>
       <c r="BZ1" s="3" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="CA1" s="3" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="CB1" s="3" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="CC1" s="3" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="CD1" s="3" t="s">
         <v>228</v>
@@ -9727,10 +10905,10 @@
     </row>
     <row r="2" spans="1:89" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="B2" s="30" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="17" t="s">
@@ -9748,7 +10926,7 @@
         <v>22</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="K2" s="17"/>
       <c r="L2" s="17"/>
@@ -9768,28 +10946,28 @@
         <v>100</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="U2" s="24" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="V2" s="23" t="s">
         <v>201</v>
       </c>
       <c r="W2" s="23" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="Y2" s="17" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="Z2" s="17" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="AA2" s="17" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="AD2" s="17"/>
       <c r="AE2" s="17"/>
@@ -9849,7 +11027,7 @@
         <v>155</v>
       </c>
       <c r="BC2" s="17" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="BD2" s="17" t="s">
         <v>156</v>
@@ -9918,10 +11096,10 @@
         <v>166</v>
       </c>
       <c r="CB2" s="4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="CC2" s="4" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="CD2" s="4" t="s">
         <v>230</v>
@@ -9936,13 +11114,13 @@
         <v>260</v>
       </c>
       <c r="CH2" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="CI2" t="s">
         <v>83</v>
       </c>
       <c r="CJ2" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committed Individual TopUp module changes
</commit_message>
<xml_diff>
--- a/KMBAutomation/TestData/TestData_LeadDetails.xlsx
+++ b/KMBAutomation/TestData/TestData_LeadDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="7470" tabRatio="847" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="7470" tabRatio="847" firstSheet="11" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="TestScenario" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2360" uniqueCount="360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="354">
   <si>
     <t>Username</t>
   </si>
@@ -1090,35 +1090,16 @@
     <t>HLDAPBalanceTransferNonIndividual</t>
   </si>
   <si>
-    <t>00104724</t>
-  </si>
-  <si>
-    <t>27/06/2022 2:02 PM</t>
-  </si>
-  <si>
-    <t>00104727</t>
-  </si>
-  <si>
-    <t>27/06/2022 3:03 PM</t>
-  </si>
-  <si>
-    <t>00104730</t>
-  </si>
-  <si>
-    <t>27/06/2022 3:27 PM</t>
-  </si>
-  <si>
-    <t>00104751</t>
-  </si>
-  <si>
-    <t>27/06/2022 3:54 PM</t>
+    <t>00104844</t>
+  </si>
+  <si>
+    <t>28/06/2022 12:32 PM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1661,11 +1642,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="25" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="25" width="49.140625"/>
-    <col min="3" max="3" customWidth="true" style="25" width="17.85546875"/>
-    <col min="4" max="4" customWidth="true" style="25" width="18.85546875"/>
-    <col min="5" max="16384" style="25" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="25"/>
+    <col min="2" max="2" width="49.140625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="25" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" style="25" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1882,85 +1863,85 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="23" customWidth="true" style="4" width="24.0"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.7109375"/>
-    <col min="25" max="25" customWidth="true" style="4" width="20.85546875"/>
-    <col min="26" max="26" customWidth="true" style="4" width="36.28515625"/>
-    <col min="27" max="27" customWidth="true" style="4" width="29.140625"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
-    <col min="30" max="30" customWidth="true" style="4" width="22.42578125"/>
-    <col min="31" max="31" customWidth="true" style="4" width="25.42578125"/>
-    <col min="32" max="32" customWidth="true" style="4" width="17.85546875"/>
-    <col min="33" max="33" customWidth="true" style="4" width="16.7109375"/>
-    <col min="34" max="35" customWidth="true" style="4" width="27.5703125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="16.7109375"/>
-    <col min="37" max="37" customWidth="true" style="4" width="11.140625"/>
-    <col min="38" max="38" customWidth="true" style="4" width="24.5703125"/>
-    <col min="39" max="39" customWidth="true" style="4" width="17.7109375"/>
-    <col min="40" max="41" customWidth="true" style="4" width="19.42578125"/>
-    <col min="42" max="43" customWidth="true" style="5" width="34.42578125"/>
-    <col min="44" max="44" customWidth="true" style="4" width="21.7109375"/>
-    <col min="45" max="45" customWidth="true" style="4" width="24.140625"/>
-    <col min="46" max="46" customWidth="true" style="4" width="26.7109375"/>
-    <col min="47" max="48" customWidth="true" style="4" width="19.140625"/>
-    <col min="49" max="49" customWidth="true" style="4" width="16.5703125"/>
-    <col min="50" max="50" customWidth="true" style="4" width="21.42578125"/>
-    <col min="51" max="51" customWidth="true" style="4" width="12.85546875"/>
-    <col min="52" max="52" customWidth="true" style="4" width="30.7109375"/>
-    <col min="53" max="53" customWidth="true" style="4" width="14.42578125"/>
-    <col min="54" max="54" customWidth="true" style="4" width="10.5703125"/>
-    <col min="55" max="55" customWidth="true" style="4" width="13.0"/>
-    <col min="56" max="56" customWidth="true" style="4" width="13.28515625"/>
-    <col min="57" max="57" customWidth="true" style="4" width="15.28515625"/>
-    <col min="58" max="58" customWidth="true" style="4" width="12.42578125"/>
-    <col min="59" max="59" style="4" width="9.140625"/>
-    <col min="60" max="60" customWidth="true" style="4" width="19.85546875"/>
-    <col min="61" max="61" customWidth="true" style="4" width="25.7109375"/>
-    <col min="62" max="62" customWidth="true" style="4" width="13.42578125"/>
-    <col min="63" max="63" customWidth="true" style="4" width="15.0"/>
-    <col min="64" max="64" customWidth="true" style="4" width="20.140625"/>
-    <col min="65" max="65" customWidth="true" style="4" width="21.7109375"/>
-    <col min="66" max="66" customWidth="true" style="4" width="17.28515625"/>
-    <col min="67" max="67" customWidth="true" style="4" width="17.85546875"/>
-    <col min="68" max="68" customWidth="true" style="4" width="32.5703125"/>
-    <col min="69" max="69" customWidth="true" style="4" width="24.7109375"/>
-    <col min="70" max="70" customWidth="true" style="4" width="26.5703125"/>
-    <col min="71" max="71" customWidth="true" style="4" width="32.7109375"/>
-    <col min="72" max="72" customWidth="true" style="4" width="18.42578125"/>
-    <col min="73" max="73" customWidth="true" style="4" width="17.85546875"/>
-    <col min="74" max="74" customWidth="true" style="4" width="17.140625"/>
-    <col min="75" max="75" customWidth="true" style="4" width="18.5703125"/>
-    <col min="76" max="76" customWidth="true" style="4" width="18.42578125"/>
-    <col min="77" max="78" customWidth="true" style="4" width="17.85546875"/>
-    <col min="79" max="81" customWidth="true" style="4" width="25.28515625"/>
-    <col min="82" max="82" customWidth="true" style="4" width="17.28515625"/>
-    <col min="83" max="83" customWidth="true" style="4" width="19.28515625"/>
-    <col min="84" max="84" customWidth="true" style="4" width="24.140625"/>
-    <col min="85" max="85" customWidth="true" style="4" width="16.28515625"/>
-    <col min="86" max="86" customWidth="true" style="4" width="16.0"/>
-    <col min="87" max="87" customWidth="true" style="4" width="19.42578125"/>
-    <col min="88" max="88" customWidth="true" style="4" width="19.85546875"/>
-    <col min="89" max="89" customWidth="true" style="4" width="17.5703125"/>
-    <col min="90" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="23" width="24" style="4" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="4" customWidth="1"/>
+    <col min="25" max="25" width="20.85546875" style="4" customWidth="1"/>
+    <col min="26" max="26" width="36.28515625" style="4" customWidth="1"/>
+    <col min="27" max="27" width="29.140625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.42578125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="25.42578125" style="4" customWidth="1"/>
+    <col min="32" max="32" width="17.85546875" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="35" width="27.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="16.7109375" style="4" customWidth="1"/>
+    <col min="37" max="37" width="11.140625" style="4" customWidth="1"/>
+    <col min="38" max="38" width="24.5703125" style="4" customWidth="1"/>
+    <col min="39" max="39" width="17.7109375" style="4" customWidth="1"/>
+    <col min="40" max="41" width="19.42578125" style="4" customWidth="1"/>
+    <col min="42" max="43" width="34.42578125" style="5" customWidth="1"/>
+    <col min="44" max="44" width="21.7109375" style="4" customWidth="1"/>
+    <col min="45" max="45" width="24.140625" style="4" customWidth="1"/>
+    <col min="46" max="46" width="26.7109375" style="4" customWidth="1"/>
+    <col min="47" max="48" width="19.140625" style="4" customWidth="1"/>
+    <col min="49" max="49" width="16.5703125" style="4" customWidth="1"/>
+    <col min="50" max="50" width="21.42578125" style="4" customWidth="1"/>
+    <col min="51" max="51" width="12.85546875" style="4" customWidth="1"/>
+    <col min="52" max="52" width="30.7109375" style="4" customWidth="1"/>
+    <col min="53" max="53" width="14.42578125" style="4" customWidth="1"/>
+    <col min="54" max="54" width="10.5703125" style="4" customWidth="1"/>
+    <col min="55" max="55" width="13" style="4" customWidth="1"/>
+    <col min="56" max="56" width="13.28515625" style="4" customWidth="1"/>
+    <col min="57" max="57" width="15.28515625" style="4" customWidth="1"/>
+    <col min="58" max="58" width="12.42578125" style="4" customWidth="1"/>
+    <col min="59" max="59" width="9.140625" style="4"/>
+    <col min="60" max="60" width="19.85546875" style="4" customWidth="1"/>
+    <col min="61" max="61" width="25.7109375" style="4" customWidth="1"/>
+    <col min="62" max="62" width="13.42578125" style="4" customWidth="1"/>
+    <col min="63" max="63" width="15" style="4" customWidth="1"/>
+    <col min="64" max="64" width="20.140625" style="4" customWidth="1"/>
+    <col min="65" max="65" width="21.7109375" style="4" customWidth="1"/>
+    <col min="66" max="66" width="17.28515625" style="4" customWidth="1"/>
+    <col min="67" max="67" width="17.85546875" style="4" customWidth="1"/>
+    <col min="68" max="68" width="32.5703125" style="4" customWidth="1"/>
+    <col min="69" max="69" width="24.7109375" style="4" customWidth="1"/>
+    <col min="70" max="70" width="26.5703125" style="4" customWidth="1"/>
+    <col min="71" max="71" width="32.7109375" style="4" customWidth="1"/>
+    <col min="72" max="72" width="18.42578125" style="4" customWidth="1"/>
+    <col min="73" max="73" width="17.85546875" style="4" customWidth="1"/>
+    <col min="74" max="74" width="17.140625" style="4" customWidth="1"/>
+    <col min="75" max="75" width="18.5703125" style="4" customWidth="1"/>
+    <col min="76" max="76" width="18.42578125" style="4" customWidth="1"/>
+    <col min="77" max="78" width="17.85546875" style="4" customWidth="1"/>
+    <col min="79" max="81" width="25.28515625" style="4" customWidth="1"/>
+    <col min="82" max="82" width="17.28515625" style="4" customWidth="1"/>
+    <col min="83" max="83" width="19.28515625" style="4" customWidth="1"/>
+    <col min="84" max="84" width="24.140625" style="4" customWidth="1"/>
+    <col min="85" max="85" width="16.28515625" style="4" customWidth="1"/>
+    <col min="86" max="86" width="16" style="4" customWidth="1"/>
+    <col min="87" max="87" width="19.42578125" style="4" customWidth="1"/>
+    <col min="88" max="88" width="19.85546875" style="4" customWidth="1"/>
+    <col min="89" max="89" width="17.5703125" style="4" customWidth="1"/>
+    <col min="90" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:89" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -2506,85 +2487,85 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="23" customWidth="true" style="4" width="24.0"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.7109375"/>
-    <col min="25" max="25" customWidth="true" style="4" width="20.85546875"/>
-    <col min="26" max="26" customWidth="true" style="4" width="36.28515625"/>
-    <col min="27" max="27" customWidth="true" style="4" width="29.140625"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
-    <col min="30" max="30" customWidth="true" style="4" width="22.42578125"/>
-    <col min="31" max="31" customWidth="true" style="4" width="25.42578125"/>
-    <col min="32" max="32" customWidth="true" style="4" width="17.85546875"/>
-    <col min="33" max="33" customWidth="true" style="4" width="16.7109375"/>
-    <col min="34" max="35" customWidth="true" style="4" width="27.5703125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="16.7109375"/>
-    <col min="37" max="37" customWidth="true" style="4" width="11.140625"/>
-    <col min="38" max="38" customWidth="true" style="4" width="24.5703125"/>
-    <col min="39" max="39" customWidth="true" style="4" width="17.7109375"/>
-    <col min="40" max="41" customWidth="true" style="4" width="19.42578125"/>
-    <col min="42" max="43" customWidth="true" style="5" width="34.42578125"/>
-    <col min="44" max="44" customWidth="true" style="4" width="21.7109375"/>
-    <col min="45" max="45" customWidth="true" style="4" width="24.140625"/>
-    <col min="46" max="47" customWidth="true" style="4" width="26.7109375"/>
-    <col min="48" max="49" customWidth="true" style="4" width="19.140625"/>
-    <col min="50" max="50" customWidth="true" style="4" width="16.5703125"/>
-    <col min="51" max="51" customWidth="true" style="4" width="21.42578125"/>
-    <col min="52" max="52" customWidth="true" style="4" width="12.85546875"/>
-    <col min="53" max="53" customWidth="true" style="4" width="30.7109375"/>
-    <col min="54" max="54" customWidth="true" style="4" width="39.5703125"/>
-    <col min="55" max="55" customWidth="true" style="4" width="10.5703125"/>
-    <col min="56" max="56" customWidth="true" style="4" width="13.0"/>
-    <col min="57" max="57" customWidth="true" style="4" width="13.28515625"/>
-    <col min="58" max="58" customWidth="true" style="4" width="15.28515625"/>
-    <col min="59" max="59" customWidth="true" style="4" width="12.42578125"/>
-    <col min="60" max="60" style="4" width="9.140625"/>
-    <col min="61" max="61" customWidth="true" style="4" width="19.85546875"/>
-    <col min="62" max="62" customWidth="true" style="4" width="25.7109375"/>
-    <col min="63" max="63" customWidth="true" style="4" width="13.42578125"/>
-    <col min="64" max="64" customWidth="true" style="4" width="15.0"/>
-    <col min="65" max="65" customWidth="true" style="4" width="20.140625"/>
-    <col min="66" max="66" customWidth="true" style="4" width="21.7109375"/>
-    <col min="67" max="67" customWidth="true" style="4" width="17.28515625"/>
-    <col min="68" max="68" customWidth="true" style="4" width="17.85546875"/>
-    <col min="69" max="69" customWidth="true" style="4" width="32.5703125"/>
-    <col min="70" max="70" customWidth="true" style="4" width="24.7109375"/>
-    <col min="71" max="71" customWidth="true" style="4" width="26.5703125"/>
-    <col min="72" max="72" customWidth="true" style="4" width="32.7109375"/>
-    <col min="73" max="73" customWidth="true" style="4" width="18.42578125"/>
-    <col min="74" max="74" customWidth="true" style="4" width="17.85546875"/>
-    <col min="75" max="75" customWidth="true" style="4" width="17.140625"/>
-    <col min="76" max="76" customWidth="true" style="4" width="18.5703125"/>
-    <col min="77" max="77" customWidth="true" style="4" width="18.42578125"/>
-    <col min="78" max="79" customWidth="true" style="4" width="17.85546875"/>
-    <col min="80" max="82" customWidth="true" style="4" width="25.28515625"/>
-    <col min="83" max="83" customWidth="true" style="4" width="17.28515625"/>
-    <col min="84" max="84" customWidth="true" style="4" width="19.28515625"/>
-    <col min="85" max="85" customWidth="true" style="4" width="24.140625"/>
-    <col min="86" max="86" customWidth="true" style="4" width="16.28515625"/>
-    <col min="87" max="87" customWidth="true" style="4" width="16.0"/>
-    <col min="88" max="88" customWidth="true" style="4" width="19.42578125"/>
-    <col min="89" max="89" customWidth="true" style="4" width="19.85546875"/>
-    <col min="90" max="90" customWidth="true" style="4" width="17.5703125"/>
-    <col min="91" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="23" width="24" style="4" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="4" customWidth="1"/>
+    <col min="25" max="25" width="20.85546875" style="4" customWidth="1"/>
+    <col min="26" max="26" width="36.28515625" style="4" customWidth="1"/>
+    <col min="27" max="27" width="29.140625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.42578125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="25.42578125" style="4" customWidth="1"/>
+    <col min="32" max="32" width="17.85546875" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="35" width="27.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="16.7109375" style="4" customWidth="1"/>
+    <col min="37" max="37" width="11.140625" style="4" customWidth="1"/>
+    <col min="38" max="38" width="24.5703125" style="4" customWidth="1"/>
+    <col min="39" max="39" width="17.7109375" style="4" customWidth="1"/>
+    <col min="40" max="41" width="19.42578125" style="4" customWidth="1"/>
+    <col min="42" max="43" width="34.42578125" style="5" customWidth="1"/>
+    <col min="44" max="44" width="21.7109375" style="4" customWidth="1"/>
+    <col min="45" max="45" width="24.140625" style="4" customWidth="1"/>
+    <col min="46" max="47" width="26.7109375" style="4" customWidth="1"/>
+    <col min="48" max="49" width="19.140625" style="4" customWidth="1"/>
+    <col min="50" max="50" width="16.5703125" style="4" customWidth="1"/>
+    <col min="51" max="51" width="21.42578125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="12.85546875" style="4" customWidth="1"/>
+    <col min="53" max="53" width="30.7109375" style="4" customWidth="1"/>
+    <col min="54" max="54" width="39.5703125" style="4" customWidth="1"/>
+    <col min="55" max="55" width="10.5703125" style="4" customWidth="1"/>
+    <col min="56" max="56" width="13" style="4" customWidth="1"/>
+    <col min="57" max="57" width="13.28515625" style="4" customWidth="1"/>
+    <col min="58" max="58" width="15.28515625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="12.42578125" style="4" customWidth="1"/>
+    <col min="60" max="60" width="9.140625" style="4"/>
+    <col min="61" max="61" width="19.85546875" style="4" customWidth="1"/>
+    <col min="62" max="62" width="25.7109375" style="4" customWidth="1"/>
+    <col min="63" max="63" width="13.42578125" style="4" customWidth="1"/>
+    <col min="64" max="64" width="15" style="4" customWidth="1"/>
+    <col min="65" max="65" width="20.140625" style="4" customWidth="1"/>
+    <col min="66" max="66" width="21.7109375" style="4" customWidth="1"/>
+    <col min="67" max="67" width="17.28515625" style="4" customWidth="1"/>
+    <col min="68" max="68" width="17.85546875" style="4" customWidth="1"/>
+    <col min="69" max="69" width="32.5703125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="24.7109375" style="4" customWidth="1"/>
+    <col min="71" max="71" width="26.5703125" style="4" customWidth="1"/>
+    <col min="72" max="72" width="32.7109375" style="4" customWidth="1"/>
+    <col min="73" max="73" width="18.42578125" style="4" customWidth="1"/>
+    <col min="74" max="74" width="17.85546875" style="4" customWidth="1"/>
+    <col min="75" max="75" width="17.140625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="18.5703125" style="4" customWidth="1"/>
+    <col min="77" max="77" width="18.42578125" style="4" customWidth="1"/>
+    <col min="78" max="79" width="17.85546875" style="4" customWidth="1"/>
+    <col min="80" max="82" width="25.28515625" style="4" customWidth="1"/>
+    <col min="83" max="83" width="17.28515625" style="4" customWidth="1"/>
+    <col min="84" max="84" width="19.28515625" style="4" customWidth="1"/>
+    <col min="85" max="85" width="24.140625" style="4" customWidth="1"/>
+    <col min="86" max="86" width="16.28515625" style="4" customWidth="1"/>
+    <col min="87" max="87" width="16" style="4" customWidth="1"/>
+    <col min="88" max="88" width="19.42578125" style="4" customWidth="1"/>
+    <col min="89" max="89" width="19.85546875" style="4" customWidth="1"/>
+    <col min="90" max="90" width="17.5703125" style="4" customWidth="1"/>
+    <col min="91" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:90" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3133,85 +3114,85 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="23" customWidth="true" style="4" width="24.0"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.7109375"/>
-    <col min="25" max="25" customWidth="true" style="4" width="20.85546875"/>
-    <col min="26" max="26" customWidth="true" style="4" width="36.28515625"/>
-    <col min="27" max="27" customWidth="true" style="4" width="29.140625"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
-    <col min="30" max="30" customWidth="true" style="4" width="22.42578125"/>
-    <col min="31" max="31" customWidth="true" style="4" width="25.42578125"/>
-    <col min="32" max="32" customWidth="true" style="4" width="17.85546875"/>
-    <col min="33" max="33" customWidth="true" style="4" width="16.7109375"/>
-    <col min="34" max="35" customWidth="true" style="4" width="27.5703125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="16.7109375"/>
-    <col min="37" max="37" customWidth="true" style="4" width="11.140625"/>
-    <col min="38" max="38" customWidth="true" style="4" width="24.5703125"/>
-    <col min="39" max="39" customWidth="true" style="4" width="17.7109375"/>
-    <col min="40" max="41" customWidth="true" style="4" width="19.42578125"/>
-    <col min="42" max="43" customWidth="true" style="5" width="34.42578125"/>
-    <col min="44" max="44" customWidth="true" style="4" width="21.7109375"/>
-    <col min="45" max="45" customWidth="true" style="4" width="24.140625"/>
-    <col min="46" max="46" customWidth="true" style="4" width="26.7109375"/>
-    <col min="47" max="48" customWidth="true" style="4" width="19.140625"/>
-    <col min="49" max="49" customWidth="true" style="4" width="16.5703125"/>
-    <col min="50" max="50" customWidth="true" style="4" width="21.42578125"/>
-    <col min="51" max="51" customWidth="true" style="4" width="12.85546875"/>
-    <col min="52" max="52" customWidth="true" style="4" width="30.7109375"/>
-    <col min="53" max="53" customWidth="true" style="4" width="18.140625"/>
-    <col min="54" max="54" customWidth="true" style="4" width="10.5703125"/>
-    <col min="55" max="55" customWidth="true" style="4" width="13.0"/>
-    <col min="56" max="56" customWidth="true" style="4" width="13.28515625"/>
-    <col min="57" max="57" customWidth="true" style="4" width="15.28515625"/>
-    <col min="58" max="58" customWidth="true" style="4" width="12.42578125"/>
-    <col min="59" max="59" style="4" width="9.140625"/>
-    <col min="60" max="60" customWidth="true" style="4" width="19.85546875"/>
-    <col min="61" max="61" customWidth="true" style="4" width="25.7109375"/>
-    <col min="62" max="62" customWidth="true" style="4" width="13.42578125"/>
-    <col min="63" max="63" customWidth="true" style="4" width="15.0"/>
-    <col min="64" max="64" customWidth="true" style="4" width="20.140625"/>
-    <col min="65" max="65" customWidth="true" style="4" width="21.7109375"/>
-    <col min="66" max="66" customWidth="true" style="4" width="17.28515625"/>
-    <col min="67" max="67" customWidth="true" style="4" width="17.85546875"/>
-    <col min="68" max="68" customWidth="true" style="4" width="32.5703125"/>
-    <col min="69" max="69" customWidth="true" style="4" width="24.7109375"/>
-    <col min="70" max="70" customWidth="true" style="4" width="26.5703125"/>
-    <col min="71" max="71" customWidth="true" style="4" width="32.7109375"/>
-    <col min="72" max="72" customWidth="true" style="4" width="18.42578125"/>
-    <col min="73" max="73" customWidth="true" style="4" width="17.85546875"/>
-    <col min="74" max="74" customWidth="true" style="4" width="17.140625"/>
-    <col min="75" max="75" customWidth="true" style="4" width="18.5703125"/>
-    <col min="76" max="76" customWidth="true" style="4" width="18.42578125"/>
-    <col min="77" max="78" customWidth="true" style="4" width="17.85546875"/>
-    <col min="79" max="81" customWidth="true" style="4" width="25.28515625"/>
-    <col min="82" max="82" customWidth="true" style="4" width="17.28515625"/>
-    <col min="83" max="83" customWidth="true" style="4" width="19.28515625"/>
-    <col min="84" max="84" customWidth="true" style="4" width="24.140625"/>
-    <col min="85" max="85" customWidth="true" style="4" width="16.28515625"/>
-    <col min="86" max="86" customWidth="true" style="4" width="16.0"/>
-    <col min="87" max="87" customWidth="true" style="4" width="19.42578125"/>
-    <col min="88" max="88" customWidth="true" style="4" width="19.85546875"/>
-    <col min="89" max="89" customWidth="true" style="4" width="17.5703125"/>
-    <col min="90" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="23" width="24" style="4" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="4" customWidth="1"/>
+    <col min="25" max="25" width="20.85546875" style="4" customWidth="1"/>
+    <col min="26" max="26" width="36.28515625" style="4" customWidth="1"/>
+    <col min="27" max="27" width="29.140625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.42578125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="25.42578125" style="4" customWidth="1"/>
+    <col min="32" max="32" width="17.85546875" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="35" width="27.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="16.7109375" style="4" customWidth="1"/>
+    <col min="37" max="37" width="11.140625" style="4" customWidth="1"/>
+    <col min="38" max="38" width="24.5703125" style="4" customWidth="1"/>
+    <col min="39" max="39" width="17.7109375" style="4" customWidth="1"/>
+    <col min="40" max="41" width="19.42578125" style="4" customWidth="1"/>
+    <col min="42" max="43" width="34.42578125" style="5" customWidth="1"/>
+    <col min="44" max="44" width="21.7109375" style="4" customWidth="1"/>
+    <col min="45" max="45" width="24.140625" style="4" customWidth="1"/>
+    <col min="46" max="46" width="26.7109375" style="4" customWidth="1"/>
+    <col min="47" max="48" width="19.140625" style="4" customWidth="1"/>
+    <col min="49" max="49" width="16.5703125" style="4" customWidth="1"/>
+    <col min="50" max="50" width="21.42578125" style="4" customWidth="1"/>
+    <col min="51" max="51" width="12.85546875" style="4" customWidth="1"/>
+    <col min="52" max="52" width="30.7109375" style="4" customWidth="1"/>
+    <col min="53" max="53" width="18.140625" style="4" customWidth="1"/>
+    <col min="54" max="54" width="10.5703125" style="4" customWidth="1"/>
+    <col min="55" max="55" width="13" style="4" customWidth="1"/>
+    <col min="56" max="56" width="13.28515625" style="4" customWidth="1"/>
+    <col min="57" max="57" width="15.28515625" style="4" customWidth="1"/>
+    <col min="58" max="58" width="12.42578125" style="4" customWidth="1"/>
+    <col min="59" max="59" width="9.140625" style="4"/>
+    <col min="60" max="60" width="19.85546875" style="4" customWidth="1"/>
+    <col min="61" max="61" width="25.7109375" style="4" customWidth="1"/>
+    <col min="62" max="62" width="13.42578125" style="4" customWidth="1"/>
+    <col min="63" max="63" width="15" style="4" customWidth="1"/>
+    <col min="64" max="64" width="20.140625" style="4" customWidth="1"/>
+    <col min="65" max="65" width="21.7109375" style="4" customWidth="1"/>
+    <col min="66" max="66" width="17.28515625" style="4" customWidth="1"/>
+    <col min="67" max="67" width="17.85546875" style="4" customWidth="1"/>
+    <col min="68" max="68" width="32.5703125" style="4" customWidth="1"/>
+    <col min="69" max="69" width="24.7109375" style="4" customWidth="1"/>
+    <col min="70" max="70" width="26.5703125" style="4" customWidth="1"/>
+    <col min="71" max="71" width="32.7109375" style="4" customWidth="1"/>
+    <col min="72" max="72" width="18.42578125" style="4" customWidth="1"/>
+    <col min="73" max="73" width="17.85546875" style="4" customWidth="1"/>
+    <col min="74" max="74" width="17.140625" style="4" customWidth="1"/>
+    <col min="75" max="75" width="18.5703125" style="4" customWidth="1"/>
+    <col min="76" max="76" width="18.42578125" style="4" customWidth="1"/>
+    <col min="77" max="78" width="17.85546875" style="4" customWidth="1"/>
+    <col min="79" max="81" width="25.28515625" style="4" customWidth="1"/>
+    <col min="82" max="82" width="17.28515625" style="4" customWidth="1"/>
+    <col min="83" max="83" width="19.28515625" style="4" customWidth="1"/>
+    <col min="84" max="84" width="24.140625" style="4" customWidth="1"/>
+    <col min="85" max="85" width="16.28515625" style="4" customWidth="1"/>
+    <col min="86" max="86" width="16" style="4" customWidth="1"/>
+    <col min="87" max="87" width="19.42578125" style="4" customWidth="1"/>
+    <col min="88" max="88" width="19.85546875" style="4" customWidth="1"/>
+    <col min="89" max="89" width="17.5703125" style="4" customWidth="1"/>
+    <col min="90" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:89" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -3753,79 +3734,79 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="21" customWidth="true" style="4" width="24.0"/>
-    <col min="22" max="22" customWidth="true" style="4" width="15.7109375"/>
-    <col min="23" max="23" customWidth="true" style="4" width="20.85546875"/>
-    <col min="24" max="24" customWidth="true" style="4" width="29.140625"/>
-    <col min="25" max="25" customWidth="true" style="4" width="16.7109375"/>
-    <col min="26" max="27" customWidth="true" style="4" width="27.5703125"/>
-    <col min="28" max="28" customWidth="true" style="4" width="16.7109375"/>
-    <col min="29" max="29" customWidth="true" style="4" width="11.140625"/>
-    <col min="30" max="30" customWidth="true" style="4" width="24.5703125"/>
-    <col min="31" max="31" customWidth="true" style="4" width="17.7109375"/>
-    <col min="32" max="33" customWidth="true" style="4" width="19.42578125"/>
-    <col min="34" max="35" customWidth="true" style="5" width="34.42578125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="21.7109375"/>
-    <col min="37" max="37" customWidth="true" style="4" width="24.140625"/>
-    <col min="38" max="38" customWidth="true" style="4" width="26.7109375"/>
-    <col min="39" max="40" customWidth="true" style="4" width="19.140625"/>
-    <col min="41" max="41" customWidth="true" style="4" width="16.5703125"/>
-    <col min="42" max="42" customWidth="true" style="4" width="21.42578125"/>
-    <col min="43" max="43" customWidth="true" style="4" width="12.85546875"/>
-    <col min="44" max="44" customWidth="true" style="4" width="30.7109375"/>
-    <col min="45" max="45" customWidth="true" style="4" width="35.42578125"/>
-    <col min="46" max="46" customWidth="true" style="4" width="10.5703125"/>
-    <col min="47" max="47" customWidth="true" style="4" width="13.0"/>
-    <col min="48" max="48" customWidth="true" style="4" width="13.28515625"/>
-    <col min="49" max="49" customWidth="true" style="4" width="15.28515625"/>
-    <col min="50" max="50" customWidth="true" style="4" width="12.42578125"/>
-    <col min="51" max="51" style="4" width="9.140625"/>
-    <col min="52" max="52" customWidth="true" style="4" width="19.85546875"/>
-    <col min="53" max="53" customWidth="true" style="4" width="25.7109375"/>
-    <col min="54" max="54" customWidth="true" style="4" width="13.42578125"/>
-    <col min="55" max="55" customWidth="true" style="4" width="15.0"/>
-    <col min="56" max="56" customWidth="true" style="4" width="20.140625"/>
-    <col min="57" max="57" customWidth="true" style="4" width="21.7109375"/>
-    <col min="58" max="58" customWidth="true" style="4" width="17.28515625"/>
-    <col min="59" max="59" customWidth="true" style="4" width="17.85546875"/>
-    <col min="60" max="60" customWidth="true" style="4" width="32.5703125"/>
-    <col min="61" max="61" customWidth="true" style="4" width="24.7109375"/>
-    <col min="62" max="62" customWidth="true" style="4" width="26.5703125"/>
-    <col min="63" max="63" customWidth="true" style="4" width="32.7109375"/>
-    <col min="64" max="64" customWidth="true" style="4" width="18.42578125"/>
-    <col min="65" max="65" customWidth="true" style="4" width="17.85546875"/>
-    <col min="66" max="66" customWidth="true" style="4" width="17.140625"/>
-    <col min="67" max="67" customWidth="true" style="4" width="18.5703125"/>
-    <col min="68" max="68" customWidth="true" style="4" width="18.42578125"/>
-    <col min="69" max="70" customWidth="true" style="4" width="17.85546875"/>
-    <col min="71" max="73" customWidth="true" style="4" width="25.28515625"/>
-    <col min="74" max="74" customWidth="true" style="4" width="17.28515625"/>
-    <col min="75" max="75" customWidth="true" style="4" width="19.28515625"/>
-    <col min="76" max="76" customWidth="true" style="4" width="24.140625"/>
-    <col min="77" max="77" customWidth="true" style="4" width="16.28515625"/>
-    <col min="78" max="78" customWidth="true" style="4" width="16.0"/>
-    <col min="79" max="79" customWidth="true" style="4" width="19.42578125"/>
-    <col min="80" max="80" customWidth="true" style="4" width="19.85546875"/>
-    <col min="81" max="81" customWidth="true" style="4" width="17.5703125"/>
-    <col min="82" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="21" width="24" style="4" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" style="4" customWidth="1"/>
+    <col min="23" max="23" width="20.85546875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="29.140625" style="4" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" style="4" customWidth="1"/>
+    <col min="26" max="27" width="27.5703125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" style="4" customWidth="1"/>
+    <col min="29" max="29" width="11.140625" style="4" customWidth="1"/>
+    <col min="30" max="30" width="24.5703125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="17.7109375" style="4" customWidth="1"/>
+    <col min="32" max="33" width="19.42578125" style="4" customWidth="1"/>
+    <col min="34" max="35" width="34.42578125" style="5" customWidth="1"/>
+    <col min="36" max="36" width="21.7109375" style="4" customWidth="1"/>
+    <col min="37" max="37" width="24.140625" style="4" customWidth="1"/>
+    <col min="38" max="38" width="26.7109375" style="4" customWidth="1"/>
+    <col min="39" max="40" width="19.140625" style="4" customWidth="1"/>
+    <col min="41" max="41" width="16.5703125" style="4" customWidth="1"/>
+    <col min="42" max="42" width="21.42578125" style="4" customWidth="1"/>
+    <col min="43" max="43" width="12.85546875" style="4" customWidth="1"/>
+    <col min="44" max="44" width="30.7109375" style="4" customWidth="1"/>
+    <col min="45" max="45" width="35.42578125" style="4" customWidth="1"/>
+    <col min="46" max="46" width="10.5703125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="13" style="4" customWidth="1"/>
+    <col min="48" max="48" width="13.28515625" style="4" customWidth="1"/>
+    <col min="49" max="49" width="15.28515625" style="4" customWidth="1"/>
+    <col min="50" max="50" width="12.42578125" style="4" customWidth="1"/>
+    <col min="51" max="51" width="9.140625" style="4"/>
+    <col min="52" max="52" width="19.85546875" style="4" customWidth="1"/>
+    <col min="53" max="53" width="25.7109375" style="4" customWidth="1"/>
+    <col min="54" max="54" width="13.42578125" style="4" customWidth="1"/>
+    <col min="55" max="55" width="15" style="4" customWidth="1"/>
+    <col min="56" max="56" width="20.140625" style="4" customWidth="1"/>
+    <col min="57" max="57" width="21.7109375" style="4" customWidth="1"/>
+    <col min="58" max="58" width="17.28515625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="17.85546875" style="4" customWidth="1"/>
+    <col min="60" max="60" width="32.5703125" style="4" customWidth="1"/>
+    <col min="61" max="61" width="24.7109375" style="4" customWidth="1"/>
+    <col min="62" max="62" width="26.5703125" style="4" customWidth="1"/>
+    <col min="63" max="63" width="32.7109375" style="4" customWidth="1"/>
+    <col min="64" max="64" width="18.42578125" style="4" customWidth="1"/>
+    <col min="65" max="65" width="17.85546875" style="4" customWidth="1"/>
+    <col min="66" max="66" width="17.140625" style="4" customWidth="1"/>
+    <col min="67" max="67" width="18.5703125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="18.42578125" style="4" customWidth="1"/>
+    <col min="69" max="70" width="17.85546875" style="4" customWidth="1"/>
+    <col min="71" max="73" width="25.28515625" style="4" customWidth="1"/>
+    <col min="74" max="74" width="17.28515625" style="4" customWidth="1"/>
+    <col min="75" max="75" width="19.28515625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="24.140625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="16.28515625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="16" style="4" customWidth="1"/>
+    <col min="79" max="79" width="19.42578125" style="4" customWidth="1"/>
+    <col min="80" max="80" width="19.85546875" style="4" customWidth="1"/>
+    <col min="81" max="81" width="17.5703125" style="4" customWidth="1"/>
+    <col min="82" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4326,79 +4307,79 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="21" customWidth="true" style="4" width="24.0"/>
-    <col min="22" max="22" customWidth="true" style="4" width="15.7109375"/>
-    <col min="23" max="23" customWidth="true" style="4" width="20.85546875"/>
-    <col min="24" max="24" customWidth="true" style="4" width="29.140625"/>
-    <col min="25" max="25" customWidth="true" style="4" width="16.7109375"/>
-    <col min="26" max="27" customWidth="true" style="4" width="27.5703125"/>
-    <col min="28" max="28" customWidth="true" style="4" width="16.7109375"/>
-    <col min="29" max="29" customWidth="true" style="4" width="11.140625"/>
-    <col min="30" max="30" customWidth="true" style="4" width="24.5703125"/>
-    <col min="31" max="31" customWidth="true" style="4" width="17.7109375"/>
-    <col min="32" max="33" customWidth="true" style="4" width="19.42578125"/>
-    <col min="34" max="35" customWidth="true" style="5" width="34.42578125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="21.7109375"/>
-    <col min="37" max="37" customWidth="true" style="4" width="24.140625"/>
-    <col min="38" max="38" customWidth="true" style="4" width="26.7109375"/>
-    <col min="39" max="40" customWidth="true" style="4" width="19.140625"/>
-    <col min="41" max="41" customWidth="true" style="4" width="16.5703125"/>
-    <col min="42" max="42" customWidth="true" style="4" width="21.42578125"/>
-    <col min="43" max="43" customWidth="true" style="4" width="12.85546875"/>
-    <col min="44" max="44" customWidth="true" style="4" width="30.7109375"/>
-    <col min="45" max="45" customWidth="true" style="4" width="35.42578125"/>
-    <col min="46" max="46" customWidth="true" style="4" width="10.5703125"/>
-    <col min="47" max="47" customWidth="true" style="4" width="13.0"/>
-    <col min="48" max="48" customWidth="true" style="4" width="13.28515625"/>
-    <col min="49" max="49" customWidth="true" style="4" width="15.28515625"/>
-    <col min="50" max="50" customWidth="true" style="4" width="12.42578125"/>
-    <col min="51" max="51" style="4" width="9.140625"/>
-    <col min="52" max="52" customWidth="true" style="4" width="19.85546875"/>
-    <col min="53" max="53" customWidth="true" style="4" width="25.7109375"/>
-    <col min="54" max="54" customWidth="true" style="4" width="13.42578125"/>
-    <col min="55" max="55" customWidth="true" style="4" width="15.0"/>
-    <col min="56" max="56" customWidth="true" style="4" width="20.140625"/>
-    <col min="57" max="57" customWidth="true" style="4" width="21.7109375"/>
-    <col min="58" max="58" customWidth="true" style="4" width="17.28515625"/>
-    <col min="59" max="59" customWidth="true" style="4" width="17.85546875"/>
-    <col min="60" max="60" customWidth="true" style="4" width="32.5703125"/>
-    <col min="61" max="61" customWidth="true" style="4" width="24.7109375"/>
-    <col min="62" max="62" customWidth="true" style="4" width="26.5703125"/>
-    <col min="63" max="63" customWidth="true" style="4" width="32.7109375"/>
-    <col min="64" max="64" customWidth="true" style="4" width="18.42578125"/>
-    <col min="65" max="65" customWidth="true" style="4" width="17.85546875"/>
-    <col min="66" max="66" customWidth="true" style="4" width="17.140625"/>
-    <col min="67" max="67" customWidth="true" style="4" width="18.5703125"/>
-    <col min="68" max="68" customWidth="true" style="4" width="18.42578125"/>
-    <col min="69" max="70" customWidth="true" style="4" width="17.85546875"/>
-    <col min="71" max="73" customWidth="true" style="4" width="25.28515625"/>
-    <col min="74" max="74" customWidth="true" style="4" width="17.28515625"/>
-    <col min="75" max="75" customWidth="true" style="4" width="19.28515625"/>
-    <col min="76" max="76" customWidth="true" style="4" width="24.140625"/>
-    <col min="77" max="77" customWidth="true" style="4" width="16.28515625"/>
-    <col min="78" max="78" customWidth="true" style="4" width="16.0"/>
-    <col min="79" max="79" customWidth="true" style="4" width="19.42578125"/>
-    <col min="80" max="80" customWidth="true" style="4" width="19.85546875"/>
-    <col min="81" max="81" customWidth="true" style="4" width="17.5703125"/>
-    <col min="82" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="21" width="24" style="4" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" style="4" customWidth="1"/>
+    <col min="23" max="23" width="20.85546875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="29.140625" style="4" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" style="4" customWidth="1"/>
+    <col min="26" max="27" width="27.5703125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" style="4" customWidth="1"/>
+    <col min="29" max="29" width="11.140625" style="4" customWidth="1"/>
+    <col min="30" max="30" width="24.5703125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="17.7109375" style="4" customWidth="1"/>
+    <col min="32" max="33" width="19.42578125" style="4" customWidth="1"/>
+    <col min="34" max="35" width="34.42578125" style="5" customWidth="1"/>
+    <col min="36" max="36" width="21.7109375" style="4" customWidth="1"/>
+    <col min="37" max="37" width="24.140625" style="4" customWidth="1"/>
+    <col min="38" max="38" width="26.7109375" style="4" customWidth="1"/>
+    <col min="39" max="40" width="19.140625" style="4" customWidth="1"/>
+    <col min="41" max="41" width="16.5703125" style="4" customWidth="1"/>
+    <col min="42" max="42" width="21.42578125" style="4" customWidth="1"/>
+    <col min="43" max="43" width="12.85546875" style="4" customWidth="1"/>
+    <col min="44" max="44" width="30.7109375" style="4" customWidth="1"/>
+    <col min="45" max="45" width="35.42578125" style="4" customWidth="1"/>
+    <col min="46" max="46" width="10.5703125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="13" style="4" customWidth="1"/>
+    <col min="48" max="48" width="13.28515625" style="4" customWidth="1"/>
+    <col min="49" max="49" width="15.28515625" style="4" customWidth="1"/>
+    <col min="50" max="50" width="12.42578125" style="4" customWidth="1"/>
+    <col min="51" max="51" width="9.140625" style="4"/>
+    <col min="52" max="52" width="19.85546875" style="4" customWidth="1"/>
+    <col min="53" max="53" width="25.7109375" style="4" customWidth="1"/>
+    <col min="54" max="54" width="13.42578125" style="4" customWidth="1"/>
+    <col min="55" max="55" width="15" style="4" customWidth="1"/>
+    <col min="56" max="56" width="20.140625" style="4" customWidth="1"/>
+    <col min="57" max="57" width="21.7109375" style="4" customWidth="1"/>
+    <col min="58" max="58" width="17.28515625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="17.85546875" style="4" customWidth="1"/>
+    <col min="60" max="60" width="32.5703125" style="4" customWidth="1"/>
+    <col min="61" max="61" width="24.7109375" style="4" customWidth="1"/>
+    <col min="62" max="62" width="26.5703125" style="4" customWidth="1"/>
+    <col min="63" max="63" width="32.7109375" style="4" customWidth="1"/>
+    <col min="64" max="64" width="18.42578125" style="4" customWidth="1"/>
+    <col min="65" max="65" width="17.85546875" style="4" customWidth="1"/>
+    <col min="66" max="66" width="17.140625" style="4" customWidth="1"/>
+    <col min="67" max="67" width="18.5703125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="18.42578125" style="4" customWidth="1"/>
+    <col min="69" max="70" width="17.85546875" style="4" customWidth="1"/>
+    <col min="71" max="73" width="25.28515625" style="4" customWidth="1"/>
+    <col min="74" max="74" width="17.28515625" style="4" customWidth="1"/>
+    <col min="75" max="75" width="19.28515625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="24.140625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="16.28515625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="16" style="4" customWidth="1"/>
+    <col min="79" max="79" width="19.42578125" style="4" customWidth="1"/>
+    <col min="80" max="80" width="19.85546875" style="4" customWidth="1"/>
+    <col min="81" max="81" width="17.5703125" style="4" customWidth="1"/>
+    <col min="82" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:81" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -4885,85 +4866,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AL17" sqref="AL17"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AD19" sqref="AD19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="21" customWidth="true" style="4" width="24.0"/>
-    <col min="22" max="22" customWidth="true" style="4" width="15.7109375"/>
-    <col min="23" max="23" customWidth="true" style="4" width="20.85546875"/>
-    <col min="24" max="24" customWidth="true" style="4" width="29.140625"/>
-    <col min="25" max="25" customWidth="true" style="4" width="16.7109375"/>
-    <col min="26" max="27" customWidth="true" style="4" width="27.5703125"/>
-    <col min="28" max="28" customWidth="true" style="4" width="16.7109375"/>
-    <col min="29" max="29" customWidth="true" style="4" width="11.140625"/>
-    <col min="30" max="30" customWidth="true" style="4" width="24.5703125"/>
-    <col min="31" max="31" customWidth="true" style="4" width="17.7109375"/>
-    <col min="32" max="33" customWidth="true" style="4" width="19.42578125"/>
-    <col min="34" max="35" customWidth="true" style="5" width="34.42578125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="21.7109375"/>
-    <col min="37" max="37" customWidth="true" style="4" width="24.140625"/>
-    <col min="38" max="39" customWidth="true" style="4" width="26.7109375"/>
-    <col min="40" max="41" customWidth="true" style="4" width="19.140625"/>
-    <col min="42" max="42" customWidth="true" style="4" width="16.5703125"/>
-    <col min="43" max="43" customWidth="true" style="4" width="21.42578125"/>
-    <col min="44" max="44" customWidth="true" style="4" width="12.85546875"/>
-    <col min="45" max="45" customWidth="true" style="4" width="30.7109375"/>
-    <col min="46" max="46" customWidth="true" style="4" width="35.42578125"/>
-    <col min="47" max="47" customWidth="true" style="4" width="10.5703125"/>
-    <col min="48" max="48" customWidth="true" style="4" width="13.0"/>
-    <col min="49" max="49" customWidth="true" style="4" width="13.28515625"/>
-    <col min="50" max="50" customWidth="true" style="4" width="15.28515625"/>
-    <col min="51" max="51" customWidth="true" style="4" width="12.42578125"/>
-    <col min="52" max="52" style="4" width="9.140625"/>
-    <col min="53" max="53" customWidth="true" style="4" width="19.85546875"/>
-    <col min="54" max="54" customWidth="true" style="4" width="25.7109375"/>
-    <col min="55" max="55" customWidth="true" style="4" width="13.42578125"/>
-    <col min="56" max="56" customWidth="true" style="4" width="15.0"/>
-    <col min="57" max="57" customWidth="true" style="4" width="20.140625"/>
-    <col min="58" max="58" customWidth="true" style="4" width="21.7109375"/>
-    <col min="59" max="59" customWidth="true" style="4" width="17.28515625"/>
-    <col min="60" max="60" customWidth="true" style="4" width="17.85546875"/>
-    <col min="61" max="61" customWidth="true" style="4" width="32.5703125"/>
-    <col min="62" max="62" customWidth="true" style="4" width="24.7109375"/>
-    <col min="63" max="63" customWidth="true" style="4" width="26.5703125"/>
-    <col min="64" max="64" customWidth="true" style="4" width="32.7109375"/>
-    <col min="65" max="65" customWidth="true" style="4" width="18.42578125"/>
-    <col min="66" max="66" customWidth="true" style="4" width="17.85546875"/>
-    <col min="67" max="67" customWidth="true" style="4" width="17.140625"/>
-    <col min="68" max="68" customWidth="true" style="4" width="18.5703125"/>
-    <col min="69" max="69" customWidth="true" style="4" width="18.42578125"/>
-    <col min="70" max="71" customWidth="true" style="4" width="17.85546875"/>
-    <col min="72" max="74" customWidth="true" style="4" width="25.28515625"/>
-    <col min="75" max="75" customWidth="true" style="4" width="17.28515625"/>
-    <col min="76" max="76" customWidth="true" style="4" width="19.28515625"/>
-    <col min="77" max="77" customWidth="true" style="4" width="24.140625"/>
-    <col min="78" max="78" customWidth="true" style="4" width="16.28515625"/>
-    <col min="79" max="79" customWidth="true" style="4" width="16.0"/>
-    <col min="80" max="80" customWidth="true" style="4" width="19.42578125"/>
-    <col min="81" max="81" customWidth="true" style="4" width="19.85546875"/>
-    <col min="82" max="82" customWidth="true" style="4" width="17.5703125"/>
-    <col min="83" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="21" width="24" style="4" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" style="4" customWidth="1"/>
+    <col min="23" max="23" width="20.85546875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="29.140625" style="4" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" style="4" customWidth="1"/>
+    <col min="26" max="27" width="27.5703125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" style="4" customWidth="1"/>
+    <col min="29" max="29" width="11.140625" style="4" customWidth="1"/>
+    <col min="30" max="30" width="24.5703125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="17.7109375" style="4" customWidth="1"/>
+    <col min="32" max="33" width="19.42578125" style="4" customWidth="1"/>
+    <col min="34" max="35" width="34.42578125" style="5" customWidth="1"/>
+    <col min="36" max="36" width="21.7109375" style="4" customWidth="1"/>
+    <col min="37" max="37" width="24.140625" style="4" customWidth="1"/>
+    <col min="38" max="39" width="26.7109375" style="4" customWidth="1"/>
+    <col min="40" max="41" width="19.140625" style="4" customWidth="1"/>
+    <col min="42" max="42" width="16.5703125" style="4" customWidth="1"/>
+    <col min="43" max="43" width="21.42578125" style="4" customWidth="1"/>
+    <col min="44" max="44" width="12.85546875" style="4" customWidth="1"/>
+    <col min="45" max="45" width="30.7109375" style="4" customWidth="1"/>
+    <col min="46" max="46" width="35.42578125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="10.5703125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="13" style="4" customWidth="1"/>
+    <col min="49" max="49" width="13.28515625" style="4" customWidth="1"/>
+    <col min="50" max="50" width="15.28515625" style="4" customWidth="1"/>
+    <col min="51" max="51" width="12.42578125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="9.140625" style="4"/>
+    <col min="53" max="53" width="19.85546875" style="4" customWidth="1"/>
+    <col min="54" max="54" width="25.7109375" style="4" customWidth="1"/>
+    <col min="55" max="55" width="13.42578125" style="4" customWidth="1"/>
+    <col min="56" max="56" width="15" style="4" customWidth="1"/>
+    <col min="57" max="57" width="20.140625" style="4" customWidth="1"/>
+    <col min="58" max="58" width="21.7109375" style="4" customWidth="1"/>
+    <col min="59" max="59" width="17.28515625" style="4" customWidth="1"/>
+    <col min="60" max="60" width="17.85546875" style="4" customWidth="1"/>
+    <col min="61" max="61" width="32.5703125" style="4" customWidth="1"/>
+    <col min="62" max="62" width="24.7109375" style="4" customWidth="1"/>
+    <col min="63" max="63" width="26.5703125" style="4" customWidth="1"/>
+    <col min="64" max="64" width="32.7109375" style="4" customWidth="1"/>
+    <col min="65" max="65" width="18.42578125" style="4" customWidth="1"/>
+    <col min="66" max="66" width="17.85546875" style="4" customWidth="1"/>
+    <col min="67" max="67" width="17.140625" style="4" customWidth="1"/>
+    <col min="68" max="68" width="18.5703125" style="4" customWidth="1"/>
+    <col min="69" max="69" width="18.42578125" style="4" customWidth="1"/>
+    <col min="70" max="71" width="17.85546875" style="4" customWidth="1"/>
+    <col min="72" max="74" width="25.28515625" style="4" customWidth="1"/>
+    <col min="75" max="75" width="17.28515625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="19.28515625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="24.140625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="16.28515625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="16" style="4" customWidth="1"/>
+    <col min="80" max="80" width="19.42578125" style="4" customWidth="1"/>
+    <col min="81" max="81" width="19.85546875" style="4" customWidth="1"/>
+    <col min="82" max="82" width="17.5703125" style="4" customWidth="1"/>
+    <col min="83" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:82" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -5328,7 +5309,7 @@
       </c>
       <c r="AT2" s="17"/>
       <c r="AU2" s="17" t="s">
-        <v>155</v>
+        <v>265</v>
       </c>
       <c r="AV2" s="17" t="s">
         <v>322</v>
@@ -5418,13 +5399,13 @@
         <v>327</v>
       </c>
       <c r="CA2" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="CB2" t="s">
         <v>83</v>
       </c>
       <c r="CC2" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -5475,78 +5456,78 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="21" customWidth="true" style="4" width="24.0"/>
-    <col min="22" max="22" customWidth="true" style="4" width="15.7109375"/>
-    <col min="23" max="23" customWidth="true" style="4" width="20.85546875"/>
-    <col min="24" max="24" customWidth="true" style="4" width="29.140625"/>
-    <col min="25" max="25" customWidth="true" style="4" width="16.7109375"/>
-    <col min="26" max="27" customWidth="true" style="4" width="27.5703125"/>
-    <col min="28" max="28" customWidth="true" style="4" width="16.7109375"/>
-    <col min="29" max="29" customWidth="true" style="4" width="11.140625"/>
-    <col min="30" max="30" customWidth="true" style="4" width="24.5703125"/>
-    <col min="31" max="31" customWidth="true" style="4" width="17.7109375"/>
-    <col min="32" max="33" customWidth="true" style="4" width="19.42578125"/>
-    <col min="34" max="35" customWidth="true" style="5" width="34.42578125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="21.7109375"/>
-    <col min="37" max="37" customWidth="true" style="4" width="24.140625"/>
-    <col min="38" max="39" customWidth="true" style="4" width="26.7109375"/>
-    <col min="40" max="41" customWidth="true" style="4" width="19.140625"/>
-    <col min="42" max="42" customWidth="true" style="4" width="16.5703125"/>
-    <col min="43" max="43" customWidth="true" style="4" width="21.42578125"/>
-    <col min="44" max="44" customWidth="true" style="4" width="12.85546875"/>
-    <col min="45" max="45" customWidth="true" style="4" width="30.7109375"/>
-    <col min="46" max="46" customWidth="true" style="4" width="35.42578125"/>
-    <col min="47" max="47" customWidth="true" style="4" width="10.5703125"/>
-    <col min="48" max="48" customWidth="true" style="4" width="13.0"/>
-    <col min="49" max="49" customWidth="true" style="4" width="13.28515625"/>
-    <col min="50" max="50" customWidth="true" style="4" width="15.28515625"/>
-    <col min="51" max="51" customWidth="true" style="4" width="12.42578125"/>
-    <col min="52" max="52" customWidth="true" style="4" width="17.7109375"/>
-    <col min="53" max="54" customWidth="true" style="4" width="25.7109375"/>
-    <col min="55" max="55" customWidth="true" style="4" width="13.42578125"/>
-    <col min="56" max="56" customWidth="true" style="4" width="15.0"/>
-    <col min="57" max="57" customWidth="true" style="4" width="20.140625"/>
-    <col min="58" max="58" customWidth="true" style="4" width="21.7109375"/>
-    <col min="59" max="59" customWidth="true" style="4" width="17.28515625"/>
-    <col min="60" max="60" customWidth="true" style="4" width="17.85546875"/>
-    <col min="61" max="61" customWidth="true" style="4" width="32.5703125"/>
-    <col min="62" max="62" customWidth="true" style="4" width="24.7109375"/>
-    <col min="63" max="63" customWidth="true" style="4" width="26.5703125"/>
-    <col min="64" max="64" customWidth="true" style="4" width="32.7109375"/>
-    <col min="65" max="65" customWidth="true" style="4" width="18.42578125"/>
-    <col min="66" max="66" customWidth="true" style="4" width="17.85546875"/>
-    <col min="67" max="67" customWidth="true" style="4" width="17.140625"/>
-    <col min="68" max="68" customWidth="true" style="4" width="18.5703125"/>
-    <col min="69" max="69" customWidth="true" style="4" width="18.42578125"/>
-    <col min="70" max="71" customWidth="true" style="4" width="17.85546875"/>
-    <col min="72" max="74" customWidth="true" style="4" width="25.28515625"/>
-    <col min="75" max="75" customWidth="true" style="4" width="17.28515625"/>
-    <col min="76" max="76" customWidth="true" style="4" width="19.28515625"/>
-    <col min="77" max="77" customWidth="true" style="4" width="24.140625"/>
-    <col min="78" max="78" customWidth="true" style="4" width="16.28515625"/>
-    <col min="79" max="79" customWidth="true" style="4" width="16.0"/>
-    <col min="80" max="80" customWidth="true" style="4" width="19.42578125"/>
-    <col min="81" max="81" customWidth="true" style="4" width="19.85546875"/>
-    <col min="82" max="82" customWidth="true" style="4" width="17.5703125"/>
-    <col min="83" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="21" width="24" style="4" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" style="4" customWidth="1"/>
+    <col min="23" max="23" width="20.85546875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="29.140625" style="4" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" style="4" customWidth="1"/>
+    <col min="26" max="27" width="27.5703125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" style="4" customWidth="1"/>
+    <col min="29" max="29" width="11.140625" style="4" customWidth="1"/>
+    <col min="30" max="30" width="24.5703125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="17.7109375" style="4" customWidth="1"/>
+    <col min="32" max="33" width="19.42578125" style="4" customWidth="1"/>
+    <col min="34" max="35" width="34.42578125" style="5" customWidth="1"/>
+    <col min="36" max="36" width="21.7109375" style="4" customWidth="1"/>
+    <col min="37" max="37" width="24.140625" style="4" customWidth="1"/>
+    <col min="38" max="39" width="26.7109375" style="4" customWidth="1"/>
+    <col min="40" max="41" width="19.140625" style="4" customWidth="1"/>
+    <col min="42" max="42" width="16.5703125" style="4" customWidth="1"/>
+    <col min="43" max="43" width="21.42578125" style="4" customWidth="1"/>
+    <col min="44" max="44" width="12.85546875" style="4" customWidth="1"/>
+    <col min="45" max="45" width="30.7109375" style="4" customWidth="1"/>
+    <col min="46" max="46" width="35.42578125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="10.5703125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="13" style="4" customWidth="1"/>
+    <col min="49" max="49" width="13.28515625" style="4" customWidth="1"/>
+    <col min="50" max="50" width="15.28515625" style="4" customWidth="1"/>
+    <col min="51" max="51" width="12.42578125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="17.7109375" style="4" customWidth="1"/>
+    <col min="53" max="54" width="25.7109375" style="4" customWidth="1"/>
+    <col min="55" max="55" width="13.42578125" style="4" customWidth="1"/>
+    <col min="56" max="56" width="15" style="4" customWidth="1"/>
+    <col min="57" max="57" width="20.140625" style="4" customWidth="1"/>
+    <col min="58" max="58" width="21.7109375" style="4" customWidth="1"/>
+    <col min="59" max="59" width="17.28515625" style="4" customWidth="1"/>
+    <col min="60" max="60" width="17.85546875" style="4" customWidth="1"/>
+    <col min="61" max="61" width="32.5703125" style="4" customWidth="1"/>
+    <col min="62" max="62" width="24.7109375" style="4" customWidth="1"/>
+    <col min="63" max="63" width="26.5703125" style="4" customWidth="1"/>
+    <col min="64" max="64" width="32.7109375" style="4" customWidth="1"/>
+    <col min="65" max="65" width="18.42578125" style="4" customWidth="1"/>
+    <col min="66" max="66" width="17.85546875" style="4" customWidth="1"/>
+    <col min="67" max="67" width="17.140625" style="4" customWidth="1"/>
+    <col min="68" max="68" width="18.5703125" style="4" customWidth="1"/>
+    <col min="69" max="69" width="18.42578125" style="4" customWidth="1"/>
+    <col min="70" max="71" width="17.85546875" style="4" customWidth="1"/>
+    <col min="72" max="74" width="25.28515625" style="4" customWidth="1"/>
+    <col min="75" max="75" width="17.28515625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="19.28515625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="24.140625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="16.28515625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="16" style="4" customWidth="1"/>
+    <col min="80" max="80" width="19.42578125" style="4" customWidth="1"/>
+    <col min="81" max="81" width="19.85546875" style="4" customWidth="1"/>
+    <col min="82" max="82" width="17.5703125" style="4" customWidth="1"/>
+    <col min="83" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:82" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -6052,12 +6033,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.28515625"/>
-    <col min="2" max="2" customWidth="true" width="21.85546875"/>
-    <col min="3" max="3" customWidth="true" width="31.0"/>
-    <col min="4" max="4" customWidth="true" width="25.0"/>
-    <col min="5" max="5" customWidth="true" width="17.85546875"/>
-    <col min="6" max="6" customWidth="true" style="4" width="27.42578125"/>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -6083,23 +6064,23 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f ca="1">CONCATENATE("HLNew Lead"," ",RANDBETWEEN(1,999))</f>
-        <v>HLNew Lead 864</v>
+        <v>HLNew Lead 230</v>
       </c>
       <c r="B2" s="2">
         <f ca="1">RANDBETWEEN(6789000000,9999999999)</f>
-        <v>8770801242</v>
+        <v>9079859646</v>
       </c>
       <c r="C2" s="2" t="str">
         <f ca="1">CONCATENATE(SUBSTITUTE($A2," ",""),"@gmail.com")</f>
-        <v>HLNewLead864@gmail.com</v>
+        <v>HLNewLead230@gmail.com</v>
       </c>
       <c r="D2" s="2" t="str">
         <f ca="1">CONCATENATE(RANDBETWEEN(10,30),RANDBETWEEN(10,12),RANDBETWEEN(1951,2004))</f>
-        <v>19101970</v>
+        <v>13111982</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">CONCATENATE(CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),CHAR(RANDBETWEEN(65,90)))</f>
-        <v>IFGAT4632N</v>
+        <v>STSFV1733Z</v>
       </c>
       <c r="F2" s="4" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Male","Female")</f>
@@ -6121,12 +6102,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.42578125"/>
-    <col min="2" max="2" customWidth="true" width="24.140625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="17.0"/>
-    <col min="4" max="4" customWidth="true" width="25.85546875"/>
-    <col min="5" max="5" customWidth="true" width="21.7109375"/>
-    <col min="6" max="6" customWidth="true" width="19.7109375"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="17" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -7019,76 +7000,76 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="22.42578125"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.7109375"/>
-    <col min="4" max="4" customWidth="true" style="4" width="14.7109375"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="4" width="11.5703125"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.7109375"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="4" width="12.140625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="21.5703125"/>
-    <col min="9" max="9" customWidth="true" style="4" width="18.42578125"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="4" width="10.0"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="4" width="10.5703125"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.28515625"/>
-    <col min="13" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="30.7109375"/>
-    <col min="16" max="16" customWidth="true" style="4" width="12.85546875"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="18" max="19" customWidth="true" style="4" width="24.0"/>
-    <col min="20" max="20" customWidth="true" style="4" width="15.7109375"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="4" width="12.0"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="4" width="35.85546875"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="4" width="61.7109375"/>
-    <col min="26" max="26" customWidth="true" style="4" width="17.85546875"/>
-    <col min="27" max="27" customWidth="true" style="4" width="16.7109375"/>
-    <col min="28" max="29" customWidth="true" style="4" width="27.5703125"/>
-    <col min="30" max="30" customWidth="true" style="4" width="16.7109375"/>
-    <col min="31" max="31" customWidth="true" style="4" width="15.5703125"/>
-    <col min="32" max="32" customWidth="true" style="4" width="11.140625"/>
-    <col min="33" max="33" customWidth="true" style="4" width="24.5703125"/>
-    <col min="34" max="34" customWidth="true" style="4" width="17.7109375"/>
-    <col min="35" max="36" customWidth="true" style="4" width="19.42578125"/>
-    <col min="37" max="38" customWidth="true" style="5" width="34.42578125"/>
-    <col min="39" max="39" customWidth="true" style="4" width="21.7109375"/>
-    <col min="40" max="40" customWidth="true" style="4" width="24.140625"/>
-    <col min="41" max="41" customWidth="true" style="4" width="26.7109375"/>
-    <col min="42" max="43" customWidth="true" style="4" width="19.140625"/>
-    <col min="44" max="44" customWidth="true" style="4" width="16.5703125"/>
-    <col min="45" max="45" customWidth="true" style="4" width="21.42578125"/>
-    <col min="46" max="46" customWidth="true" style="4" width="12.85546875"/>
-    <col min="47" max="47" customWidth="true" style="4" width="30.7109375"/>
-    <col min="48" max="48" customWidth="true" style="4" width="91.42578125"/>
-    <col min="49" max="49" customWidth="true" style="4" width="10.5703125"/>
-    <col min="50" max="50" customWidth="true" style="4" width="13.0"/>
-    <col min="51" max="51" customWidth="true" style="4" width="13.28515625"/>
-    <col min="52" max="52" customWidth="true" style="4" width="15.28515625"/>
-    <col min="53" max="53" customWidth="true" style="4" width="12.42578125"/>
-    <col min="54" max="54" customWidth="true" style="4" width="20.85546875"/>
-    <col min="55" max="55" customWidth="true" style="4" width="19.85546875"/>
-    <col min="56" max="56" customWidth="true" style="4" width="25.7109375"/>
-    <col min="57" max="57" customWidth="true" style="4" width="13.42578125"/>
-    <col min="58" max="58" style="4" width="9.140625"/>
-    <col min="59" max="59" customWidth="true" style="4" width="20.140625"/>
-    <col min="60" max="60" customWidth="true" style="4" width="21.7109375"/>
-    <col min="61" max="61" customWidth="true" style="4" width="17.28515625"/>
-    <col min="62" max="62" customWidth="true" style="4" width="17.85546875"/>
-    <col min="63" max="63" customWidth="true" style="4" width="32.5703125"/>
-    <col min="64" max="64" customWidth="true" style="4" width="24.7109375"/>
-    <col min="65" max="65" customWidth="true" style="4" width="26.5703125"/>
-    <col min="66" max="66" customWidth="true" style="4" width="32.7109375"/>
-    <col min="67" max="67" customWidth="true" style="4" width="18.42578125"/>
-    <col min="68" max="68" customWidth="true" style="4" width="17.85546875"/>
-    <col min="69" max="69" customWidth="true" style="4" width="17.140625"/>
-    <col min="70" max="70" customWidth="true" style="4" width="18.5703125"/>
-    <col min="71" max="71" customWidth="true" style="4" width="18.42578125"/>
-    <col min="72" max="72" customWidth="true" style="4" width="17.85546875"/>
-    <col min="73" max="73" customWidth="true" style="4" width="17.28515625"/>
-    <col min="74" max="74" customWidth="true" style="4" width="19.28515625"/>
-    <col min="75" max="75" customWidth="true" style="4" width="26.0"/>
-    <col min="76" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="22.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" style="4" customWidth="1"/>
+    <col min="13" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="30.7109375" style="4" customWidth="1"/>
+    <col min="16" max="16" width="12.85546875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="24" style="4" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" style="4" customWidth="1"/>
+    <col min="21" max="21" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="35.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="61.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="17.85546875" style="4" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" style="4" customWidth="1"/>
+    <col min="28" max="29" width="27.5703125" style="4" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="4" customWidth="1"/>
+    <col min="31" max="31" width="15.5703125" style="4" customWidth="1"/>
+    <col min="32" max="32" width="11.140625" style="4" customWidth="1"/>
+    <col min="33" max="33" width="24.5703125" style="4" customWidth="1"/>
+    <col min="34" max="34" width="17.7109375" style="4" customWidth="1"/>
+    <col min="35" max="36" width="19.42578125" style="4" customWidth="1"/>
+    <col min="37" max="38" width="34.42578125" style="5" customWidth="1"/>
+    <col min="39" max="39" width="21.7109375" style="4" customWidth="1"/>
+    <col min="40" max="40" width="24.140625" style="4" customWidth="1"/>
+    <col min="41" max="41" width="26.7109375" style="4" customWidth="1"/>
+    <col min="42" max="43" width="19.140625" style="4" customWidth="1"/>
+    <col min="44" max="44" width="16.5703125" style="4" customWidth="1"/>
+    <col min="45" max="45" width="21.42578125" style="4" customWidth="1"/>
+    <col min="46" max="46" width="12.85546875" style="4" customWidth="1"/>
+    <col min="47" max="47" width="30.7109375" style="4" customWidth="1"/>
+    <col min="48" max="48" width="91.42578125" style="4" customWidth="1"/>
+    <col min="49" max="49" width="10.5703125" style="4" customWidth="1"/>
+    <col min="50" max="50" width="13" style="4" customWidth="1"/>
+    <col min="51" max="51" width="13.28515625" style="4" customWidth="1"/>
+    <col min="52" max="52" width="15.28515625" style="4" customWidth="1"/>
+    <col min="53" max="53" width="12.42578125" style="4" customWidth="1"/>
+    <col min="54" max="54" width="20.85546875" style="4" customWidth="1"/>
+    <col min="55" max="55" width="19.85546875" style="4" customWidth="1"/>
+    <col min="56" max="56" width="25.7109375" style="4" customWidth="1"/>
+    <col min="57" max="57" width="13.42578125" style="4" customWidth="1"/>
+    <col min="58" max="58" width="9.140625" style="4"/>
+    <col min="59" max="59" width="20.140625" style="4" customWidth="1"/>
+    <col min="60" max="60" width="21.7109375" style="4" customWidth="1"/>
+    <col min="61" max="61" width="17.28515625" style="4" customWidth="1"/>
+    <col min="62" max="62" width="17.85546875" style="4" customWidth="1"/>
+    <col min="63" max="63" width="32.5703125" style="4" customWidth="1"/>
+    <col min="64" max="64" width="24.7109375" style="4" customWidth="1"/>
+    <col min="65" max="65" width="26.5703125" style="4" customWidth="1"/>
+    <col min="66" max="66" width="32.7109375" style="4" customWidth="1"/>
+    <col min="67" max="67" width="18.42578125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="17.85546875" style="4" customWidth="1"/>
+    <col min="69" max="69" width="17.140625" style="4" customWidth="1"/>
+    <col min="70" max="70" width="18.5703125" style="4" customWidth="1"/>
+    <col min="71" max="71" width="18.42578125" style="4" customWidth="1"/>
+    <col min="72" max="72" width="17.85546875" style="4" customWidth="1"/>
+    <col min="73" max="73" width="17.28515625" style="4" customWidth="1"/>
+    <col min="74" max="74" width="19.28515625" style="4" customWidth="1"/>
+    <col min="75" max="75" width="26" style="4" customWidth="1"/>
+    <col min="76" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:75" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -7355,18 +7336,18 @@
       <c r="L2" s="10"/>
       <c r="M2" s="12" t="str">
         <f ca="1">Sheet1!A2</f>
-        <v>HLNew Lead 864</v>
+        <v>HLNew Lead 230</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>173</v>
       </c>
       <c r="O2" s="10" t="str">
         <f ca="1">Sheet1!C2</f>
-        <v>HLNewLead864@gmail.com</v>
+        <v>HLNewLead230@gmail.com</v>
       </c>
       <c r="P2" s="10" t="str">
         <f ca="1">Sheet1!D2</f>
-        <v>19101970</v>
+        <v>13111982</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>76</v>
@@ -7401,7 +7382,7 @@
       <c r="AC2" s="10"/>
       <c r="AD2" s="10" t="str">
         <f ca="1">Sheet1!E2</f>
-        <v>IFGAT4632N</v>
+        <v>STSFV1733Z</v>
       </c>
       <c r="AE2" s="10" t="s">
         <v>36</v>
@@ -7699,77 +7680,77 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="12.140625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="22.42578125"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="11.5703125"/>
-    <col min="7" max="7" customWidth="true" style="4" width="14.7109375"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="4" width="12.140625"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="18.42578125"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="4" width="10.0"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="4" width="10.5703125"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="15" customWidth="true" style="4" width="25.0"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="19" max="20" customWidth="true" style="4" width="24.0"/>
-    <col min="21" max="21" customWidth="true" style="4" width="15.7109375"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="4" width="12.0"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="4" width="35.85546875"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="4" width="61.7109375"/>
-    <col min="27" max="27" customWidth="true" style="4" width="17.85546875"/>
-    <col min="28" max="28" customWidth="true" style="4" width="16.7109375"/>
-    <col min="29" max="30" customWidth="true" style="4" width="27.5703125"/>
-    <col min="31" max="31" customWidth="true" style="4" width="16.7109375"/>
-    <col min="32" max="32" customWidth="true" style="4" width="15.5703125"/>
-    <col min="33" max="33" customWidth="true" style="4" width="11.140625"/>
-    <col min="34" max="34" customWidth="true" style="4" width="24.5703125"/>
-    <col min="35" max="35" customWidth="true" style="4" width="17.7109375"/>
-    <col min="36" max="37" customWidth="true" style="4" width="19.42578125"/>
-    <col min="38" max="39" customWidth="true" style="5" width="34.42578125"/>
-    <col min="40" max="40" customWidth="true" style="4" width="21.7109375"/>
-    <col min="41" max="41" customWidth="true" style="4" width="24.140625"/>
-    <col min="42" max="42" customWidth="true" style="4" width="26.7109375"/>
-    <col min="43" max="44" customWidth="true" style="4" width="19.140625"/>
-    <col min="45" max="45" customWidth="true" style="4" width="16.5703125"/>
-    <col min="46" max="46" customWidth="true" style="4" width="21.42578125"/>
-    <col min="47" max="47" customWidth="true" style="4" width="12.85546875"/>
-    <col min="48" max="48" customWidth="true" style="4" width="30.7109375"/>
-    <col min="49" max="49" customWidth="true" style="4" width="101.7109375"/>
-    <col min="50" max="50" customWidth="true" style="4" width="19.85546875"/>
-    <col min="51" max="51" customWidth="true" style="4" width="13.0"/>
-    <col min="52" max="52" customWidth="true" style="4" width="14.28515625"/>
-    <col min="53" max="53" customWidth="true" style="4" width="19.42578125"/>
-    <col min="54" max="54" customWidth="true" style="4" width="12.42578125"/>
-    <col min="55" max="55" customWidth="true" style="4" width="20.85546875"/>
-    <col min="56" max="56" customWidth="true" style="4" width="19.85546875"/>
-    <col min="57" max="57" customWidth="true" style="4" width="25.7109375"/>
-    <col min="58" max="58" customWidth="true" style="4" width="13.42578125"/>
-    <col min="59" max="59" style="4" width="9.140625"/>
-    <col min="60" max="60" customWidth="true" style="4" width="20.140625"/>
-    <col min="61" max="61" customWidth="true" style="4" width="21.7109375"/>
-    <col min="62" max="62" customWidth="true" style="4" width="17.28515625"/>
-    <col min="63" max="63" customWidth="true" style="4" width="17.85546875"/>
-    <col min="64" max="64" customWidth="true" style="4" width="32.5703125"/>
-    <col min="65" max="65" customWidth="true" style="4" width="24.7109375"/>
-    <col min="66" max="66" customWidth="true" style="4" width="26.5703125"/>
-    <col min="67" max="67" customWidth="true" style="4" width="32.7109375"/>
-    <col min="68" max="68" customWidth="true" style="4" width="18.42578125"/>
-    <col min="69" max="69" customWidth="true" style="4" width="17.85546875"/>
-    <col min="70" max="70" customWidth="true" style="4" width="17.140625"/>
-    <col min="71" max="71" customWidth="true" style="4" width="18.5703125"/>
-    <col min="72" max="72" customWidth="true" style="4" width="18.42578125"/>
-    <col min="73" max="73" customWidth="true" style="4" width="17.85546875"/>
-    <col min="74" max="74" customWidth="true" style="4" width="17.28515625"/>
-    <col min="75" max="75" customWidth="true" style="4" width="19.28515625"/>
-    <col min="76" max="76" customWidth="true" style="4" width="22.140625"/>
-    <col min="77" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="12.140625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="15" width="25" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="24" style="4" customWidth="1"/>
+    <col min="21" max="21" width="15.7109375" style="4" customWidth="1"/>
+    <col min="22" max="22" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="61.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17.85546875" style="4" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" style="4" customWidth="1"/>
+    <col min="29" max="30" width="27.5703125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" style="4" customWidth="1"/>
+    <col min="32" max="32" width="15.5703125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="11.140625" style="4" customWidth="1"/>
+    <col min="34" max="34" width="24.5703125" style="4" customWidth="1"/>
+    <col min="35" max="35" width="17.7109375" style="4" customWidth="1"/>
+    <col min="36" max="37" width="19.42578125" style="4" customWidth="1"/>
+    <col min="38" max="39" width="34.42578125" style="5" customWidth="1"/>
+    <col min="40" max="40" width="21.7109375" style="4" customWidth="1"/>
+    <col min="41" max="41" width="24.140625" style="4" customWidth="1"/>
+    <col min="42" max="42" width="26.7109375" style="4" customWidth="1"/>
+    <col min="43" max="44" width="19.140625" style="4" customWidth="1"/>
+    <col min="45" max="45" width="16.5703125" style="4" customWidth="1"/>
+    <col min="46" max="46" width="21.42578125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="12.85546875" style="4" customWidth="1"/>
+    <col min="48" max="48" width="30.7109375" style="4" customWidth="1"/>
+    <col min="49" max="49" width="101.7109375" style="4" customWidth="1"/>
+    <col min="50" max="50" width="19.85546875" style="4" customWidth="1"/>
+    <col min="51" max="51" width="13" style="4" customWidth="1"/>
+    <col min="52" max="52" width="14.28515625" style="4" customWidth="1"/>
+    <col min="53" max="53" width="19.42578125" style="4" customWidth="1"/>
+    <col min="54" max="54" width="12.42578125" style="4" customWidth="1"/>
+    <col min="55" max="55" width="20.85546875" style="4" customWidth="1"/>
+    <col min="56" max="56" width="19.85546875" style="4" customWidth="1"/>
+    <col min="57" max="57" width="25.7109375" style="4" customWidth="1"/>
+    <col min="58" max="58" width="13.42578125" style="4" customWidth="1"/>
+    <col min="59" max="59" width="9.140625" style="4"/>
+    <col min="60" max="60" width="20.140625" style="4" customWidth="1"/>
+    <col min="61" max="61" width="21.7109375" style="4" customWidth="1"/>
+    <col min="62" max="62" width="17.28515625" style="4" customWidth="1"/>
+    <col min="63" max="63" width="17.85546875" style="4" customWidth="1"/>
+    <col min="64" max="64" width="32.5703125" style="4" customWidth="1"/>
+    <col min="65" max="65" width="24.7109375" style="4" customWidth="1"/>
+    <col min="66" max="66" width="26.5703125" style="4" customWidth="1"/>
+    <col min="67" max="67" width="32.7109375" style="4" customWidth="1"/>
+    <col min="68" max="68" width="18.42578125" style="4" customWidth="1"/>
+    <col min="69" max="69" width="17.85546875" style="4" customWidth="1"/>
+    <col min="70" max="70" width="17.140625" style="4" customWidth="1"/>
+    <col min="71" max="71" width="18.5703125" style="4" customWidth="1"/>
+    <col min="72" max="72" width="18.42578125" style="4" customWidth="1"/>
+    <col min="73" max="73" width="17.85546875" style="4" customWidth="1"/>
+    <col min="74" max="74" width="17.28515625" style="4" customWidth="1"/>
+    <col min="75" max="75" width="19.28515625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="22.140625" style="4" customWidth="1"/>
+    <col min="77" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:63" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -7985,18 +7966,18 @@
       <c r="M2" s="10"/>
       <c r="N2" s="12" t="str">
         <f ca="1">Sheet1!A2</f>
-        <v>HLNew Lead 864</v>
+        <v>HLNew Lead 230</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>173</v>
       </c>
       <c r="P2" s="10" t="str">
         <f ca="1">Sheet1!C2</f>
-        <v>HLNewLead864@gmail.com</v>
+        <v>HLNewLead230@gmail.com</v>
       </c>
       <c r="Q2" s="10" t="str">
         <f ca="1">Sheet1!D2</f>
-        <v>19101970</v>
+        <v>13111982</v>
       </c>
       <c r="R2" s="13" t="s">
         <v>76</v>
@@ -8031,7 +8012,7 @@
       <c r="AD2" s="10"/>
       <c r="AE2" s="10" t="str">
         <f ca="1">Sheet1!E2</f>
-        <v>IFGAT4632N</v>
+        <v>STSFV1733Z</v>
       </c>
       <c r="AF2" s="10" t="s">
         <v>36</v>
@@ -8117,12 +8098,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" style="33" width="39.7109375"/>
-    <col min="2" max="2" customWidth="true" style="37" width="21.0"/>
-    <col min="3" max="3" customWidth="true" style="33" width="14.0"/>
-    <col min="4" max="4" customWidth="true" style="33" width="17.28515625"/>
-    <col min="5" max="5" customWidth="true" style="33" width="17.5703125"/>
-    <col min="6" max="16384" style="33" width="9.140625"/>
+    <col min="1" max="1" width="39.7109375" style="33" customWidth="1"/>
+    <col min="2" max="2" width="21" style="37" customWidth="1"/>
+    <col min="3" max="3" width="14" style="33" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="33" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -8220,83 +8201,83 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="18.42578125"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="22" customWidth="true" style="4" width="24.0"/>
-    <col min="23" max="23" customWidth="true" style="4" width="15.7109375"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="4" width="12.0"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
-    <col min="27" max="27" customWidth="true" style="4" width="22.42578125"/>
-    <col min="28" max="28" customWidth="true" style="4" width="25.42578125"/>
-    <col min="29" max="29" customWidth="true" style="4" width="17.85546875"/>
-    <col min="30" max="30" customWidth="true" style="4" width="16.7109375"/>
-    <col min="31" max="32" customWidth="true" style="4" width="27.5703125"/>
-    <col min="33" max="33" customWidth="true" style="4" width="16.7109375"/>
-    <col min="34" max="34" customWidth="true" style="4" width="11.140625"/>
-    <col min="35" max="35" customWidth="true" style="4" width="24.5703125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="17.7109375"/>
-    <col min="37" max="38" customWidth="true" style="4" width="19.42578125"/>
-    <col min="39" max="40" customWidth="true" style="5" width="34.42578125"/>
-    <col min="41" max="41" customWidth="true" style="4" width="21.7109375"/>
-    <col min="42" max="42" customWidth="true" style="4" width="24.140625"/>
-    <col min="43" max="43" customWidth="true" style="4" width="26.7109375"/>
-    <col min="44" max="45" customWidth="true" style="4" width="19.140625"/>
-    <col min="46" max="46" customWidth="true" style="4" width="16.5703125"/>
-    <col min="47" max="47" customWidth="true" style="4" width="21.42578125"/>
-    <col min="48" max="48" customWidth="true" style="4" width="12.85546875"/>
-    <col min="49" max="49" customWidth="true" style="4" width="30.7109375"/>
-    <col min="50" max="50" customWidth="true" style="4" width="91.42578125"/>
-    <col min="51" max="51" customWidth="true" style="4" width="10.5703125"/>
-    <col min="52" max="52" customWidth="true" style="4" width="13.0"/>
-    <col min="53" max="53" customWidth="true" style="4" width="13.28515625"/>
-    <col min="54" max="54" customWidth="true" style="4" width="15.28515625"/>
-    <col min="55" max="55" customWidth="true" style="4" width="12.42578125"/>
-    <col min="56" max="56" style="4" width="9.140625"/>
-    <col min="57" max="57" customWidth="true" style="4" width="19.85546875"/>
-    <col min="58" max="58" customWidth="true" style="4" width="25.7109375"/>
-    <col min="59" max="59" customWidth="true" style="4" width="13.42578125"/>
-    <col min="60" max="60" customWidth="true" style="4" width="15.0"/>
-    <col min="61" max="61" customWidth="true" style="4" width="20.140625"/>
-    <col min="62" max="62" customWidth="true" style="4" width="21.7109375"/>
-    <col min="63" max="63" customWidth="true" style="4" width="17.28515625"/>
-    <col min="64" max="64" customWidth="true" style="4" width="17.85546875"/>
-    <col min="65" max="65" customWidth="true" style="4" width="32.5703125"/>
-    <col min="66" max="66" customWidth="true" style="4" width="24.7109375"/>
-    <col min="67" max="67" customWidth="true" style="4" width="26.5703125"/>
-    <col min="68" max="68" customWidth="true" style="4" width="32.7109375"/>
-    <col min="69" max="69" customWidth="true" style="4" width="18.42578125"/>
-    <col min="70" max="70" customWidth="true" style="4" width="17.85546875"/>
-    <col min="71" max="71" customWidth="true" style="4" width="17.140625"/>
-    <col min="72" max="72" customWidth="true" style="4" width="18.5703125"/>
-    <col min="73" max="73" customWidth="true" style="4" width="18.42578125"/>
-    <col min="74" max="75" customWidth="true" style="4" width="17.85546875"/>
-    <col min="76" max="78" customWidth="true" style="4" width="25.28515625"/>
-    <col min="79" max="79" customWidth="true" style="4" width="17.28515625"/>
-    <col min="80" max="80" customWidth="true" style="4" width="19.28515625"/>
-    <col min="81" max="81" customWidth="true" style="4" width="24.140625"/>
-    <col min="82" max="82" customWidth="true" style="4" width="16.28515625"/>
-    <col min="83" max="83" customWidth="true" style="4" width="16.0"/>
-    <col min="84" max="84" customWidth="true" style="4" width="19.42578125"/>
-    <col min="85" max="85" customWidth="true" style="4" width="19.85546875"/>
-    <col min="86" max="86" customWidth="true" style="4" width="17.5703125"/>
-    <col min="87" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="22" width="24" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="25.42578125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="4" customWidth="1"/>
+    <col min="31" max="32" width="27.5703125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="17.7109375" style="4" customWidth="1"/>
+    <col min="37" max="38" width="19.42578125" style="4" customWidth="1"/>
+    <col min="39" max="40" width="34.42578125" style="5" customWidth="1"/>
+    <col min="41" max="41" width="21.7109375" style="4" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" style="4" customWidth="1"/>
+    <col min="43" max="43" width="26.7109375" style="4" customWidth="1"/>
+    <col min="44" max="45" width="19.140625" style="4" customWidth="1"/>
+    <col min="46" max="46" width="16.5703125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="21.42578125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="12.85546875" style="4" customWidth="1"/>
+    <col min="49" max="49" width="30.7109375" style="4" customWidth="1"/>
+    <col min="50" max="50" width="91.42578125" style="4" customWidth="1"/>
+    <col min="51" max="51" width="10.5703125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="13" style="4" customWidth="1"/>
+    <col min="53" max="53" width="13.28515625" style="4" customWidth="1"/>
+    <col min="54" max="54" width="15.28515625" style="4" customWidth="1"/>
+    <col min="55" max="55" width="12.42578125" style="4" customWidth="1"/>
+    <col min="56" max="56" width="9.140625" style="4"/>
+    <col min="57" max="57" width="19.85546875" style="4" customWidth="1"/>
+    <col min="58" max="58" width="25.7109375" style="4" customWidth="1"/>
+    <col min="59" max="59" width="13.42578125" style="4" customWidth="1"/>
+    <col min="60" max="60" width="15" style="4" customWidth="1"/>
+    <col min="61" max="61" width="20.140625" style="4" customWidth="1"/>
+    <col min="62" max="62" width="21.7109375" style="4" customWidth="1"/>
+    <col min="63" max="63" width="17.28515625" style="4" customWidth="1"/>
+    <col min="64" max="64" width="17.85546875" style="4" customWidth="1"/>
+    <col min="65" max="65" width="32.5703125" style="4" customWidth="1"/>
+    <col min="66" max="66" width="24.7109375" style="4" customWidth="1"/>
+    <col min="67" max="67" width="26.5703125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="32.7109375" style="4" customWidth="1"/>
+    <col min="69" max="69" width="18.42578125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="17.85546875" style="4" customWidth="1"/>
+    <col min="71" max="71" width="17.140625" style="4" customWidth="1"/>
+    <col min="72" max="72" width="18.5703125" style="4" customWidth="1"/>
+    <col min="73" max="73" width="18.42578125" style="4" customWidth="1"/>
+    <col min="74" max="75" width="17.85546875" style="4" customWidth="1"/>
+    <col min="76" max="78" width="25.28515625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="17.28515625" style="4" customWidth="1"/>
+    <col min="80" max="80" width="19.28515625" style="4" customWidth="1"/>
+    <col min="81" max="81" width="24.140625" style="4" customWidth="1"/>
+    <col min="82" max="82" width="16.28515625" style="4" customWidth="1"/>
+    <col min="83" max="83" width="16" style="4" customWidth="1"/>
+    <col min="84" max="84" width="19.42578125" style="4" customWidth="1"/>
+    <col min="85" max="85" width="19.85546875" style="4" customWidth="1"/>
+    <col min="86" max="86" width="17.5703125" style="4" customWidth="1"/>
+    <col min="87" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:86" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -8811,82 +8792,82 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="18.42578125"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="22" customWidth="true" style="4" width="24.0"/>
-    <col min="23" max="23" customWidth="true" style="4" width="15.7109375"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="4" width="12.0"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
-    <col min="27" max="27" customWidth="true" style="4" width="22.42578125"/>
-    <col min="28" max="28" customWidth="true" style="4" width="25.42578125"/>
-    <col min="29" max="29" customWidth="true" style="4" width="17.85546875"/>
-    <col min="30" max="30" customWidth="true" style="4" width="16.7109375"/>
-    <col min="31" max="32" customWidth="true" style="4" width="27.5703125"/>
-    <col min="33" max="33" customWidth="true" style="4" width="16.7109375"/>
-    <col min="34" max="34" customWidth="true" style="4" width="11.140625"/>
-    <col min="35" max="35" customWidth="true" style="4" width="24.5703125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="17.7109375"/>
-    <col min="37" max="38" customWidth="true" style="4" width="19.42578125"/>
-    <col min="39" max="40" customWidth="true" style="5" width="34.42578125"/>
-    <col min="41" max="41" customWidth="true" style="4" width="21.7109375"/>
-    <col min="42" max="42" customWidth="true" style="4" width="24.140625"/>
-    <col min="43" max="43" customWidth="true" style="4" width="26.7109375"/>
-    <col min="44" max="45" customWidth="true" style="4" width="19.140625"/>
-    <col min="46" max="46" customWidth="true" style="4" width="16.5703125"/>
-    <col min="47" max="47" customWidth="true" style="4" width="21.42578125"/>
-    <col min="48" max="48" customWidth="true" style="4" width="12.85546875"/>
-    <col min="49" max="49" customWidth="true" style="4" width="30.7109375"/>
-    <col min="50" max="50" customWidth="true" style="4" width="35.28515625"/>
-    <col min="51" max="51" customWidth="true" style="4" width="10.5703125"/>
-    <col min="52" max="52" customWidth="true" style="4" width="13.0"/>
-    <col min="53" max="53" customWidth="true" style="4" width="13.28515625"/>
-    <col min="54" max="54" customWidth="true" style="4" width="15.28515625"/>
-    <col min="55" max="55" customWidth="true" style="4" width="12.42578125"/>
-    <col min="56" max="56" style="4" width="9.140625"/>
-    <col min="57" max="57" customWidth="true" style="4" width="19.85546875"/>
-    <col min="58" max="58" customWidth="true" style="4" width="19.140625"/>
-    <col min="59" max="59" customWidth="true" style="4" width="17.5703125"/>
-    <col min="60" max="60" customWidth="true" style="4" width="15.0"/>
-    <col min="61" max="61" customWidth="true" style="4" width="20.140625"/>
-    <col min="62" max="62" customWidth="true" style="4" width="21.7109375"/>
-    <col min="63" max="63" customWidth="true" style="4" width="17.28515625"/>
-    <col min="64" max="64" customWidth="true" style="4" width="17.85546875"/>
-    <col min="65" max="65" customWidth="true" style="4" width="32.5703125"/>
-    <col min="66" max="66" customWidth="true" style="4" width="24.7109375"/>
-    <col min="67" max="67" customWidth="true" style="4" width="26.5703125"/>
-    <col min="68" max="68" customWidth="true" style="4" width="32.7109375"/>
-    <col min="69" max="69" customWidth="true" style="4" width="18.42578125"/>
-    <col min="70" max="70" customWidth="true" style="4" width="17.85546875"/>
-    <col min="71" max="71" customWidth="true" style="4" width="17.140625"/>
-    <col min="72" max="72" customWidth="true" style="4" width="18.5703125"/>
-    <col min="73" max="73" customWidth="true" style="4" width="18.42578125"/>
-    <col min="74" max="74" customWidth="true" style="4" width="17.85546875"/>
-    <col min="75" max="75" customWidth="true" style="4" width="17.28515625"/>
-    <col min="76" max="76" customWidth="true" style="4" width="19.28515625"/>
-    <col min="77" max="77" customWidth="true" style="4" width="24.140625"/>
-    <col min="78" max="78" customWidth="true" style="4" width="16.28515625"/>
-    <col min="79" max="79" customWidth="true" style="4" width="16.0"/>
-    <col min="80" max="80" customWidth="true" style="4" width="19.42578125"/>
-    <col min="81" max="81" customWidth="true" style="4" width="19.85546875"/>
-    <col min="82" max="82" customWidth="true" style="4" width="17.5703125"/>
-    <col min="83" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="22" width="24" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="25.42578125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="4" customWidth="1"/>
+    <col min="31" max="32" width="27.5703125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="17.7109375" style="4" customWidth="1"/>
+    <col min="37" max="38" width="19.42578125" style="4" customWidth="1"/>
+    <col min="39" max="40" width="34.42578125" style="5" customWidth="1"/>
+    <col min="41" max="41" width="21.7109375" style="4" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" style="4" customWidth="1"/>
+    <col min="43" max="43" width="26.7109375" style="4" customWidth="1"/>
+    <col min="44" max="45" width="19.140625" style="4" customWidth="1"/>
+    <col min="46" max="46" width="16.5703125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="21.42578125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="12.85546875" style="4" customWidth="1"/>
+    <col min="49" max="49" width="30.7109375" style="4" customWidth="1"/>
+    <col min="50" max="50" width="35.28515625" style="4" customWidth="1"/>
+    <col min="51" max="51" width="10.5703125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="13" style="4" customWidth="1"/>
+    <col min="53" max="53" width="13.28515625" style="4" customWidth="1"/>
+    <col min="54" max="54" width="15.28515625" style="4" customWidth="1"/>
+    <col min="55" max="55" width="12.42578125" style="4" customWidth="1"/>
+    <col min="56" max="56" width="9.140625" style="4"/>
+    <col min="57" max="57" width="19.85546875" style="4" customWidth="1"/>
+    <col min="58" max="58" width="19.140625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="17.5703125" style="4" customWidth="1"/>
+    <col min="60" max="60" width="15" style="4" customWidth="1"/>
+    <col min="61" max="61" width="20.140625" style="4" customWidth="1"/>
+    <col min="62" max="62" width="21.7109375" style="4" customWidth="1"/>
+    <col min="63" max="63" width="17.28515625" style="4" customWidth="1"/>
+    <col min="64" max="64" width="17.85546875" style="4" customWidth="1"/>
+    <col min="65" max="65" width="32.5703125" style="4" customWidth="1"/>
+    <col min="66" max="66" width="24.7109375" style="4" customWidth="1"/>
+    <col min="67" max="67" width="26.5703125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="32.7109375" style="4" customWidth="1"/>
+    <col min="69" max="69" width="18.42578125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="17.85546875" style="4" customWidth="1"/>
+    <col min="71" max="71" width="17.140625" style="4" customWidth="1"/>
+    <col min="72" max="72" width="18.5703125" style="4" customWidth="1"/>
+    <col min="73" max="73" width="18.42578125" style="4" customWidth="1"/>
+    <col min="74" max="74" width="17.85546875" style="4" customWidth="1"/>
+    <col min="75" max="75" width="17.28515625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="19.28515625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="24.140625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="16.28515625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="16" style="4" customWidth="1"/>
+    <col min="80" max="80" width="19.42578125" style="4" customWidth="1"/>
+    <col min="81" max="81" width="19.85546875" style="4" customWidth="1"/>
+    <col min="82" max="82" width="17.5703125" style="4" customWidth="1"/>
+    <col min="83" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:82" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -9377,88 +9358,88 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AU18" sqref="AU18"/>
+    <sheetView topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="AR14" sqref="AR14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="18.42578125"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="23" customWidth="true" style="4" width="24.0"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.7109375"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="4" width="12.0"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
-    <col min="28" max="28" customWidth="true" style="4" width="22.42578125"/>
-    <col min="29" max="29" customWidth="true" style="4" width="25.42578125"/>
-    <col min="30" max="30" customWidth="true" style="4" width="17.85546875"/>
-    <col min="31" max="31" customWidth="true" style="4" width="16.7109375"/>
-    <col min="32" max="33" customWidth="true" style="4" width="27.5703125"/>
-    <col min="34" max="34" customWidth="true" style="4" width="16.7109375"/>
-    <col min="35" max="35" customWidth="true" style="4" width="11.140625"/>
-    <col min="36" max="36" customWidth="true" style="4" width="24.5703125"/>
-    <col min="37" max="37" customWidth="true" style="4" width="17.7109375"/>
-    <col min="38" max="39" customWidth="true" style="4" width="19.42578125"/>
-    <col min="40" max="41" customWidth="true" style="5" width="34.42578125"/>
-    <col min="42" max="42" customWidth="true" style="4" width="21.7109375"/>
-    <col min="43" max="43" customWidth="true" style="4" width="24.140625"/>
-    <col min="44" max="45" customWidth="true" style="4" width="26.7109375"/>
-    <col min="46" max="47" customWidth="true" style="4" width="19.140625"/>
-    <col min="48" max="48" customWidth="true" style="4" width="16.5703125"/>
-    <col min="49" max="49" customWidth="true" style="4" width="21.42578125"/>
-    <col min="50" max="50" customWidth="true" style="4" width="12.85546875"/>
-    <col min="51" max="51" customWidth="true" style="4" width="30.7109375"/>
-    <col min="52" max="52" customWidth="true" style="4" width="32.140625"/>
-    <col min="53" max="53" customWidth="true" style="4" width="10.5703125"/>
-    <col min="54" max="54" customWidth="true" style="4" width="13.0"/>
-    <col min="55" max="55" customWidth="true" style="4" width="13.28515625"/>
-    <col min="56" max="56" customWidth="true" style="4" width="15.28515625"/>
-    <col min="57" max="57" customWidth="true" style="4" width="12.42578125"/>
-    <col min="58" max="58" style="4" width="9.140625"/>
-    <col min="59" max="59" customWidth="true" style="4" width="19.85546875"/>
-    <col min="60" max="60" customWidth="true" style="4" width="25.7109375"/>
-    <col min="61" max="61" customWidth="true" style="4" width="13.42578125"/>
-    <col min="62" max="62" customWidth="true" style="4" width="15.0"/>
-    <col min="63" max="63" customWidth="true" style="4" width="20.140625"/>
-    <col min="64" max="64" customWidth="true" style="4" width="21.7109375"/>
-    <col min="65" max="65" customWidth="true" style="4" width="17.28515625"/>
-    <col min="66" max="66" customWidth="true" style="4" width="17.85546875"/>
-    <col min="67" max="67" customWidth="true" style="4" width="32.5703125"/>
-    <col min="68" max="68" customWidth="true" style="4" width="24.7109375"/>
-    <col min="69" max="69" customWidth="true" style="4" width="26.5703125"/>
-    <col min="70" max="70" customWidth="true" style="4" width="32.7109375"/>
-    <col min="71" max="71" customWidth="true" style="4" width="18.42578125"/>
-    <col min="72" max="72" customWidth="true" style="4" width="17.85546875"/>
-    <col min="73" max="73" customWidth="true" style="4" width="17.140625"/>
-    <col min="74" max="74" customWidth="true" style="4" width="18.5703125"/>
-    <col min="75" max="75" customWidth="true" style="4" width="18.42578125"/>
-    <col min="76" max="76" customWidth="true" style="4" width="17.85546875"/>
-    <col min="77" max="77" customWidth="true" style="4" width="17.28515625"/>
-    <col min="78" max="78" customWidth="true" style="4" width="19.28515625"/>
-    <col min="79" max="79" customWidth="true" style="4" width="24.140625"/>
-    <col min="80" max="80" customWidth="true" style="4" width="16.28515625"/>
-    <col min="81" max="81" customWidth="true" style="4" width="16.0"/>
-    <col min="82" max="82" customWidth="true" style="4" width="19.42578125"/>
-    <col min="83" max="83" customWidth="true" style="4" width="19.85546875"/>
-    <col min="84" max="84" customWidth="true" style="4" width="17.5703125"/>
-    <col min="85" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="23" width="24" style="4" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="4" customWidth="1"/>
+    <col min="25" max="25" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="22.42578125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="25.42578125" style="4" customWidth="1"/>
+    <col min="30" max="30" width="17.85546875" style="4" customWidth="1"/>
+    <col min="31" max="31" width="16.7109375" style="4" customWidth="1"/>
+    <col min="32" max="33" width="27.5703125" style="4" customWidth="1"/>
+    <col min="34" max="34" width="16.7109375" style="4" customWidth="1"/>
+    <col min="35" max="35" width="11.140625" style="4" customWidth="1"/>
+    <col min="36" max="36" width="24.5703125" style="4" customWidth="1"/>
+    <col min="37" max="37" width="17.7109375" style="4" customWidth="1"/>
+    <col min="38" max="39" width="19.42578125" style="4" customWidth="1"/>
+    <col min="40" max="41" width="34.42578125" style="5" customWidth="1"/>
+    <col min="42" max="42" width="21.7109375" style="4" customWidth="1"/>
+    <col min="43" max="43" width="24.140625" style="4" customWidth="1"/>
+    <col min="44" max="45" width="26.7109375" style="4" customWidth="1"/>
+    <col min="46" max="47" width="19.140625" style="4" customWidth="1"/>
+    <col min="48" max="48" width="16.5703125" style="4" customWidth="1"/>
+    <col min="49" max="49" width="21.42578125" style="4" customWidth="1"/>
+    <col min="50" max="50" width="12.85546875" style="4" customWidth="1"/>
+    <col min="51" max="51" width="30.7109375" style="4" customWidth="1"/>
+    <col min="52" max="52" width="32.140625" style="4" customWidth="1"/>
+    <col min="53" max="53" width="10.5703125" style="4" customWidth="1"/>
+    <col min="54" max="54" width="13" style="4" customWidth="1"/>
+    <col min="55" max="55" width="13.28515625" style="4" customWidth="1"/>
+    <col min="56" max="56" width="15.28515625" style="4" customWidth="1"/>
+    <col min="57" max="57" width="12.42578125" style="4" customWidth="1"/>
+    <col min="58" max="58" width="9.140625" style="4"/>
+    <col min="59" max="59" width="19.85546875" style="4" customWidth="1"/>
+    <col min="60" max="60" width="25.7109375" style="4" customWidth="1"/>
+    <col min="61" max="61" width="13.42578125" style="4" customWidth="1"/>
+    <col min="62" max="62" width="15" style="4" customWidth="1"/>
+    <col min="63" max="63" width="20.140625" style="4" customWidth="1"/>
+    <col min="64" max="64" width="21.7109375" style="4" customWidth="1"/>
+    <col min="65" max="65" width="17.28515625" style="4" customWidth="1"/>
+    <col min="66" max="66" width="17.85546875" style="4" customWidth="1"/>
+    <col min="67" max="67" width="32.5703125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="24.7109375" style="4" customWidth="1"/>
+    <col min="69" max="69" width="26.5703125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="32.7109375" style="4" customWidth="1"/>
+    <col min="71" max="71" width="18.42578125" style="4" customWidth="1"/>
+    <col min="72" max="72" width="17.85546875" style="4" customWidth="1"/>
+    <col min="73" max="73" width="17.140625" style="4" customWidth="1"/>
+    <col min="74" max="74" width="18.5703125" style="4" customWidth="1"/>
+    <col min="75" max="75" width="18.42578125" style="4" customWidth="1"/>
+    <col min="76" max="76" width="17.85546875" style="4" customWidth="1"/>
+    <col min="77" max="77" width="17.28515625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="19.28515625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="24.140625" style="4" customWidth="1"/>
+    <col min="80" max="80" width="16.28515625" style="4" customWidth="1"/>
+    <col min="81" max="81" width="16" style="4" customWidth="1"/>
+    <col min="82" max="82" width="19.42578125" style="4" customWidth="1"/>
+    <col min="83" max="83" width="19.85546875" style="4" customWidth="1"/>
+    <col min="84" max="84" width="17.5703125" style="4" customWidth="1"/>
+    <col min="85" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:84" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -9961,83 +9942,83 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="18.42578125"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="22" customWidth="true" style="4" width="24.0"/>
-    <col min="23" max="23" customWidth="true" style="4" width="15.7109375"/>
-    <col min="24" max="24" customWidth="true" style="4" width="14.5703125"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
-    <col min="27" max="27" customWidth="true" style="4" width="22.42578125"/>
-    <col min="28" max="28" customWidth="true" style="4" width="25.42578125"/>
-    <col min="29" max="29" customWidth="true" style="4" width="17.85546875"/>
-    <col min="30" max="30" customWidth="true" style="4" width="16.7109375"/>
-    <col min="31" max="32" customWidth="true" style="4" width="27.5703125"/>
-    <col min="33" max="33" customWidth="true" style="4" width="16.7109375"/>
-    <col min="34" max="34" customWidth="true" style="4" width="11.140625"/>
-    <col min="35" max="35" customWidth="true" style="4" width="24.5703125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="17.7109375"/>
-    <col min="37" max="38" customWidth="true" style="4" width="19.42578125"/>
-    <col min="39" max="40" customWidth="true" style="5" width="34.42578125"/>
-    <col min="41" max="41" customWidth="true" style="4" width="21.7109375"/>
-    <col min="42" max="42" customWidth="true" style="4" width="24.140625"/>
-    <col min="43" max="44" customWidth="true" style="4" width="26.7109375"/>
-    <col min="45" max="46" customWidth="true" style="4" width="19.140625"/>
-    <col min="47" max="47" customWidth="true" style="4" width="16.5703125"/>
-    <col min="48" max="48" customWidth="true" style="4" width="21.42578125"/>
-    <col min="49" max="49" customWidth="true" style="4" width="12.85546875"/>
-    <col min="50" max="50" customWidth="true" style="4" width="30.7109375"/>
-    <col min="51" max="51" customWidth="true" style="4" width="32.140625"/>
-    <col min="52" max="52" customWidth="true" style="4" width="10.5703125"/>
-    <col min="53" max="53" customWidth="true" style="4" width="13.0"/>
-    <col min="54" max="54" customWidth="true" style="4" width="13.28515625"/>
-    <col min="55" max="55" customWidth="true" style="4" width="15.28515625"/>
-    <col min="56" max="56" customWidth="true" style="4" width="12.42578125"/>
-    <col min="57" max="57" style="4" width="9.140625"/>
-    <col min="58" max="58" customWidth="true" style="4" width="32.140625"/>
-    <col min="59" max="59" customWidth="true" style="4" width="25.7109375"/>
-    <col min="60" max="60" customWidth="true" style="4" width="13.42578125"/>
-    <col min="61" max="61" customWidth="true" style="4" width="15.0"/>
-    <col min="62" max="62" customWidth="true" style="4" width="20.140625"/>
-    <col min="63" max="63" customWidth="true" style="4" width="21.140625"/>
-    <col min="64" max="64" customWidth="true" style="4" width="26.140625"/>
-    <col min="65" max="65" customWidth="true" style="4" width="19.0"/>
-    <col min="66" max="66" customWidth="true" style="4" width="17.85546875"/>
-    <col min="67" max="67" customWidth="true" style="4" width="32.5703125"/>
-    <col min="68" max="68" customWidth="true" style="4" width="24.7109375"/>
-    <col min="69" max="69" customWidth="true" style="4" width="26.5703125"/>
-    <col min="70" max="70" customWidth="true" style="4" width="32.7109375"/>
-    <col min="71" max="71" customWidth="true" style="4" width="18.42578125"/>
-    <col min="72" max="72" customWidth="true" style="4" width="17.85546875"/>
-    <col min="73" max="73" customWidth="true" style="4" width="17.140625"/>
-    <col min="74" max="74" customWidth="true" style="4" width="18.5703125"/>
-    <col min="75" max="75" customWidth="true" style="4" width="18.42578125"/>
-    <col min="76" max="76" customWidth="true" style="4" width="17.85546875"/>
-    <col min="77" max="77" customWidth="true" style="4" width="17.28515625"/>
-    <col min="78" max="78" customWidth="true" style="4" width="19.28515625"/>
-    <col min="79" max="79" customWidth="true" style="4" width="24.140625"/>
-    <col min="80" max="80" customWidth="true" style="4" width="16.28515625"/>
-    <col min="81" max="81" customWidth="true" style="4" width="16.0"/>
-    <col min="82" max="82" customWidth="true" style="4" width="19.42578125"/>
-    <col min="83" max="83" customWidth="true" style="4" width="19.85546875"/>
-    <col min="84" max="84" customWidth="true" style="4" width="17.5703125"/>
-    <col min="85" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="22" width="24" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="25.42578125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="4" customWidth="1"/>
+    <col min="31" max="32" width="27.5703125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="17.7109375" style="4" customWidth="1"/>
+    <col min="37" max="38" width="19.42578125" style="4" customWidth="1"/>
+    <col min="39" max="40" width="34.42578125" style="5" customWidth="1"/>
+    <col min="41" max="41" width="21.7109375" style="4" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" style="4" customWidth="1"/>
+    <col min="43" max="44" width="26.7109375" style="4" customWidth="1"/>
+    <col min="45" max="46" width="19.140625" style="4" customWidth="1"/>
+    <col min="47" max="47" width="16.5703125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="21.42578125" style="4" customWidth="1"/>
+    <col min="49" max="49" width="12.85546875" style="4" customWidth="1"/>
+    <col min="50" max="50" width="30.7109375" style="4" customWidth="1"/>
+    <col min="51" max="51" width="32.140625" style="4" customWidth="1"/>
+    <col min="52" max="52" width="10.5703125" style="4" customWidth="1"/>
+    <col min="53" max="53" width="13" style="4" customWidth="1"/>
+    <col min="54" max="54" width="13.28515625" style="4" customWidth="1"/>
+    <col min="55" max="55" width="15.28515625" style="4" customWidth="1"/>
+    <col min="56" max="56" width="12.42578125" style="4" customWidth="1"/>
+    <col min="57" max="57" width="9.140625" style="4"/>
+    <col min="58" max="58" width="32.140625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="25.7109375" style="4" customWidth="1"/>
+    <col min="60" max="60" width="13.42578125" style="4" customWidth="1"/>
+    <col min="61" max="61" width="15" style="4" customWidth="1"/>
+    <col min="62" max="62" width="20.140625" style="4" customWidth="1"/>
+    <col min="63" max="63" width="21.140625" style="4" customWidth="1"/>
+    <col min="64" max="64" width="26.140625" style="4" customWidth="1"/>
+    <col min="65" max="65" width="19" style="4" customWidth="1"/>
+    <col min="66" max="66" width="17.85546875" style="4" customWidth="1"/>
+    <col min="67" max="67" width="32.5703125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="24.7109375" style="4" customWidth="1"/>
+    <col min="69" max="69" width="26.5703125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="32.7109375" style="4" customWidth="1"/>
+    <col min="71" max="71" width="18.42578125" style="4" customWidth="1"/>
+    <col min="72" max="72" width="17.85546875" style="4" customWidth="1"/>
+    <col min="73" max="73" width="17.140625" style="4" customWidth="1"/>
+    <col min="74" max="74" width="18.5703125" style="4" customWidth="1"/>
+    <col min="75" max="75" width="18.42578125" style="4" customWidth="1"/>
+    <col min="76" max="76" width="17.85546875" style="4" customWidth="1"/>
+    <col min="77" max="77" width="17.28515625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="19.28515625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="24.140625" style="4" customWidth="1"/>
+    <col min="80" max="80" width="16.28515625" style="4" customWidth="1"/>
+    <col min="81" max="81" width="16" style="4" customWidth="1"/>
+    <col min="82" max="82" width="19.42578125" style="4" customWidth="1"/>
+    <col min="83" max="83" width="19.85546875" style="4" customWidth="1"/>
+    <col min="84" max="84" width="17.5703125" style="4" customWidth="1"/>
+    <col min="85" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:84" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -10554,84 +10535,84 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.140625"/>
-    <col min="2" max="2" customWidth="true" style="4" width="14.28515625"/>
-    <col min="3" max="3" customWidth="true" style="4" width="12.85546875"/>
-    <col min="4" max="4" customWidth="true" style="4" width="12.7109375"/>
-    <col min="5" max="5" customWidth="true" style="4" width="14.7109375"/>
-    <col min="6" max="6" customWidth="true" style="4" width="14.28515625"/>
-    <col min="7" max="7" customWidth="true" style="4" width="12.28515625"/>
-    <col min="8" max="8" customWidth="true" style="4" width="14.7109375"/>
-    <col min="9" max="9" customWidth="true" style="4" width="21.5703125"/>
-    <col min="10" max="10" customWidth="true" style="4" width="34.7109375"/>
-    <col min="11" max="11" customWidth="true" style="4" width="11.85546875"/>
-    <col min="12" max="12" customWidth="true" style="4" width="12.0"/>
-    <col min="13" max="13" customWidth="true" style="4" width="12.28515625"/>
-    <col min="14" max="14" customWidth="true" style="4" width="25.0"/>
-    <col min="15" max="15" customWidth="true" style="4" width="17.5703125"/>
-    <col min="16" max="16" customWidth="true" style="4" width="30.7109375"/>
-    <col min="17" max="17" customWidth="true" style="4" width="12.85546875"/>
-    <col min="18" max="18" customWidth="true" style="4" width="16.85546875"/>
-    <col min="19" max="23" customWidth="true" style="4" width="24.0"/>
-    <col min="24" max="24" customWidth="true" style="4" width="15.7109375"/>
-    <col min="25" max="25" customWidth="true" style="4" width="20.85546875"/>
-    <col min="26" max="26" customWidth="true" style="4" width="36.28515625"/>
-    <col min="27" max="27" customWidth="true" style="4" width="29.140625"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="4" width="14.5703125"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="4" width="14.7109375"/>
-    <col min="30" max="30" customWidth="true" style="4" width="22.42578125"/>
-    <col min="31" max="31" customWidth="true" style="4" width="25.42578125"/>
-    <col min="32" max="32" customWidth="true" style="4" width="17.85546875"/>
-    <col min="33" max="33" customWidth="true" style="4" width="16.7109375"/>
-    <col min="34" max="35" customWidth="true" style="4" width="27.5703125"/>
-    <col min="36" max="36" customWidth="true" style="4" width="16.7109375"/>
-    <col min="37" max="37" customWidth="true" style="4" width="11.140625"/>
-    <col min="38" max="38" customWidth="true" style="4" width="24.5703125"/>
-    <col min="39" max="39" customWidth="true" style="4" width="17.7109375"/>
-    <col min="40" max="41" customWidth="true" style="4" width="19.42578125"/>
-    <col min="42" max="43" customWidth="true" style="5" width="34.42578125"/>
-    <col min="44" max="44" customWidth="true" style="4" width="21.7109375"/>
-    <col min="45" max="45" customWidth="true" style="4" width="24.140625"/>
-    <col min="46" max="46" customWidth="true" style="4" width="26.7109375"/>
-    <col min="47" max="48" customWidth="true" style="4" width="19.140625"/>
-    <col min="49" max="49" customWidth="true" style="4" width="16.5703125"/>
-    <col min="50" max="50" customWidth="true" style="4" width="21.42578125"/>
-    <col min="51" max="51" customWidth="true" style="4" width="12.85546875"/>
-    <col min="52" max="53" customWidth="true" style="4" width="30.7109375"/>
-    <col min="54" max="54" customWidth="true" style="4" width="10.5703125"/>
-    <col min="55" max="55" customWidth="true" style="4" width="13.0"/>
-    <col min="56" max="56" customWidth="true" style="4" width="13.28515625"/>
-    <col min="57" max="57" customWidth="true" style="4" width="15.28515625"/>
-    <col min="58" max="58" customWidth="true" style="4" width="12.42578125"/>
-    <col min="59" max="59" style="4" width="9.140625"/>
-    <col min="60" max="60" customWidth="true" style="4" width="19.85546875"/>
-    <col min="61" max="61" customWidth="true" style="4" width="25.7109375"/>
-    <col min="62" max="62" customWidth="true" style="4" width="13.42578125"/>
-    <col min="63" max="63" customWidth="true" style="4" width="15.0"/>
-    <col min="64" max="64" customWidth="true" style="4" width="20.140625"/>
-    <col min="65" max="65" customWidth="true" style="4" width="21.7109375"/>
-    <col min="66" max="66" customWidth="true" style="4" width="17.28515625"/>
-    <col min="67" max="67" customWidth="true" style="4" width="17.85546875"/>
-    <col min="68" max="68" customWidth="true" style="4" width="32.5703125"/>
-    <col min="69" max="69" customWidth="true" style="4" width="24.7109375"/>
-    <col min="70" max="70" customWidth="true" style="4" width="26.5703125"/>
-    <col min="71" max="71" customWidth="true" style="4" width="32.7109375"/>
-    <col min="72" max="72" customWidth="true" style="4" width="18.42578125"/>
-    <col min="73" max="73" customWidth="true" style="4" width="17.85546875"/>
-    <col min="74" max="74" customWidth="true" style="4" width="17.140625"/>
-    <col min="75" max="75" customWidth="true" style="4" width="18.5703125"/>
-    <col min="76" max="76" customWidth="true" style="4" width="18.42578125"/>
-    <col min="77" max="78" customWidth="true" style="4" width="17.85546875"/>
-    <col min="79" max="81" customWidth="true" style="4" width="25.28515625"/>
-    <col min="82" max="82" customWidth="true" style="4" width="17.28515625"/>
-    <col min="83" max="83" customWidth="true" style="4" width="19.28515625"/>
-    <col min="84" max="84" customWidth="true" style="4" width="24.140625"/>
-    <col min="85" max="85" customWidth="true" style="4" width="16.28515625"/>
-    <col min="86" max="86" customWidth="true" style="4" width="16.0"/>
-    <col min="87" max="87" customWidth="true" style="4" width="19.42578125"/>
-    <col min="88" max="88" customWidth="true" style="4" width="19.85546875"/>
-    <col min="89" max="89" customWidth="true" style="4" width="17.5703125"/>
-    <col min="90" max="16384" style="4" width="9.140625"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="23" width="24" style="4" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="4" customWidth="1"/>
+    <col min="25" max="25" width="20.85546875" style="4" customWidth="1"/>
+    <col min="26" max="26" width="36.28515625" style="4" customWidth="1"/>
+    <col min="27" max="27" width="29.140625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.42578125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="25.42578125" style="4" customWidth="1"/>
+    <col min="32" max="32" width="17.85546875" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="35" width="27.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="16.7109375" style="4" customWidth="1"/>
+    <col min="37" max="37" width="11.140625" style="4" customWidth="1"/>
+    <col min="38" max="38" width="24.5703125" style="4" customWidth="1"/>
+    <col min="39" max="39" width="17.7109375" style="4" customWidth="1"/>
+    <col min="40" max="41" width="19.42578125" style="4" customWidth="1"/>
+    <col min="42" max="43" width="34.42578125" style="5" customWidth="1"/>
+    <col min="44" max="44" width="21.7109375" style="4" customWidth="1"/>
+    <col min="45" max="45" width="24.140625" style="4" customWidth="1"/>
+    <col min="46" max="46" width="26.7109375" style="4" customWidth="1"/>
+    <col min="47" max="48" width="19.140625" style="4" customWidth="1"/>
+    <col min="49" max="49" width="16.5703125" style="4" customWidth="1"/>
+    <col min="50" max="50" width="21.42578125" style="4" customWidth="1"/>
+    <col min="51" max="51" width="12.85546875" style="4" customWidth="1"/>
+    <col min="52" max="53" width="30.7109375" style="4" customWidth="1"/>
+    <col min="54" max="54" width="10.5703125" style="4" customWidth="1"/>
+    <col min="55" max="55" width="13" style="4" customWidth="1"/>
+    <col min="56" max="56" width="13.28515625" style="4" customWidth="1"/>
+    <col min="57" max="57" width="15.28515625" style="4" customWidth="1"/>
+    <col min="58" max="58" width="12.42578125" style="4" customWidth="1"/>
+    <col min="59" max="59" width="9.140625" style="4"/>
+    <col min="60" max="60" width="19.85546875" style="4" customWidth="1"/>
+    <col min="61" max="61" width="25.7109375" style="4" customWidth="1"/>
+    <col min="62" max="62" width="13.42578125" style="4" customWidth="1"/>
+    <col min="63" max="63" width="15" style="4" customWidth="1"/>
+    <col min="64" max="64" width="20.140625" style="4" customWidth="1"/>
+    <col min="65" max="65" width="21.7109375" style="4" customWidth="1"/>
+    <col min="66" max="66" width="17.28515625" style="4" customWidth="1"/>
+    <col min="67" max="67" width="17.85546875" style="4" customWidth="1"/>
+    <col min="68" max="68" width="32.5703125" style="4" customWidth="1"/>
+    <col min="69" max="69" width="24.7109375" style="4" customWidth="1"/>
+    <col min="70" max="70" width="26.5703125" style="4" customWidth="1"/>
+    <col min="71" max="71" width="32.7109375" style="4" customWidth="1"/>
+    <col min="72" max="72" width="18.42578125" style="4" customWidth="1"/>
+    <col min="73" max="73" width="17.85546875" style="4" customWidth="1"/>
+    <col min="74" max="74" width="17.140625" style="4" customWidth="1"/>
+    <col min="75" max="75" width="18.5703125" style="4" customWidth="1"/>
+    <col min="76" max="76" width="18.42578125" style="4" customWidth="1"/>
+    <col min="77" max="78" width="17.85546875" style="4" customWidth="1"/>
+    <col min="79" max="81" width="25.28515625" style="4" customWidth="1"/>
+    <col min="82" max="82" width="17.28515625" style="4" customWidth="1"/>
+    <col min="83" max="83" width="19.28515625" style="4" customWidth="1"/>
+    <col min="84" max="84" width="24.140625" style="4" customWidth="1"/>
+    <col min="85" max="85" width="16.28515625" style="4" customWidth="1"/>
+    <col min="86" max="86" width="16" style="4" customWidth="1"/>
+    <col min="87" max="87" width="19.42578125" style="4" customWidth="1"/>
+    <col min="88" max="88" width="19.85546875" style="4" customWidth="1"/>
+    <col min="89" max="89" width="17.5703125" style="4" customWidth="1"/>
+    <col min="90" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:89" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Script for Kotak Smart Home Product
</commit_message>
<xml_diff>
--- a/KMBAutomation/TestData/TestData_LeadDetails.xlsx
+++ b/KMBAutomation/TestData/TestData_LeadDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="7470" tabRatio="847" firstSheet="11" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="7470" tabRatio="847"/>
   </bookViews>
   <sheets>
     <sheet name="TestScenario" sheetId="3" r:id="rId1"/>
@@ -23,15 +23,18 @@
     <sheet name="HLDAPOnlyTopUpSalariedNRI" sheetId="15" r:id="rId14"/>
     <sheet name="HLDAPOnlyTopUpIndividual" sheetId="18" r:id="rId15"/>
     <sheet name="HLDAPOnlyTopUpNonIndividual" sheetId="19" r:id="rId16"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId17"/>
-    <sheet name="Output" sheetId="2" r:id="rId18"/>
+    <sheet name="HLDAPKotakSmartHomeSalIndian" sheetId="20" r:id="rId17"/>
+    <sheet name="HLDAPKotakSmartHomeSalNRI" sheetId="21" r:id="rId18"/>
+    <sheet name="HLDAPKotakSmartHomeIndividual" sheetId="22" r:id="rId19"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId20"/>
+    <sheet name="Output" sheetId="2" r:id="rId21"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2348" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2783" uniqueCount="367">
   <si>
     <t>Username</t>
   </si>
@@ -1090,10 +1093,49 @@
     <t>HLDAPBalanceTransferNonIndividual</t>
   </si>
   <si>
-    <t>00104844</t>
-  </si>
-  <si>
-    <t>28/06/2022 12:32 PM</t>
+    <t>9879879705</t>
+  </si>
+  <si>
+    <t>00104922</t>
+  </si>
+  <si>
+    <t>29/06/2022 3:55 PM</t>
+  </si>
+  <si>
+    <t>TC15</t>
+  </si>
+  <si>
+    <t>HLDAPKotakSmartHomeSalariedIndian</t>
+  </si>
+  <si>
+    <t>TC16</t>
+  </si>
+  <si>
+    <t>HLDAPKotakSmartHomeSalariedNRI</t>
+  </si>
+  <si>
+    <t>TC17</t>
+  </si>
+  <si>
+    <t>HLDAPKotakSmartHomeIndividual</t>
+  </si>
+  <si>
+    <t>Kotak Smart Home</t>
+  </si>
+  <si>
+    <t>Senior Manager</t>
+  </si>
+  <si>
+    <t>9879879704</t>
+  </si>
+  <si>
+    <t>00104952</t>
+  </si>
+  <si>
+    <t>30/06/2022 5:11 PM</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1193,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1200,6 +1242,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1240,7 +1288,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1277,7 +1325,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1301,13 +1348,15 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1634,10 +1683,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1667,7 +1716,7 @@
       <c r="A2" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="38" t="s">
         <v>256</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -1679,7 +1728,7 @@
       <c r="A3" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="39" t="s">
         <v>258</v>
       </c>
       <c r="C3" s="22" t="s">
@@ -1691,7 +1740,7 @@
       <c r="A4" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="37" t="s">
         <v>344</v>
       </c>
       <c r="C4" s="22" t="s">
@@ -1703,7 +1752,7 @@
       <c r="A5" s="22" t="s">
         <v>270</v>
       </c>
-      <c r="B5" s="39" t="s">
+      <c r="B5" s="37" t="s">
         <v>345</v>
       </c>
       <c r="C5" s="22" t="s">
@@ -1715,7 +1764,7 @@
       <c r="A6" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="28" t="s">
         <v>346</v>
       </c>
       <c r="C6" s="22" t="s">
@@ -1727,7 +1776,7 @@
       <c r="A7" s="22" t="s">
         <v>287</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="28" t="s">
         <v>347</v>
       </c>
       <c r="C7" s="22" t="s">
@@ -1736,92 +1785,138 @@
       <c r="D7" s="22"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="43" t="s">
         <v>348</v>
       </c>
       <c r="C8" s="22" t="s">
         <v>100</v>
       </c>
+      <c r="D8" s="22"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="43" t="s">
         <v>349</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>100</v>
       </c>
+      <c r="D9" s="22"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="22" t="s">
         <v>319</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="43" t="s">
         <v>350</v>
       </c>
       <c r="C10" s="22" t="s">
         <v>100</v>
       </c>
+      <c r="D10" s="22"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="22" t="s">
         <v>329</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="43" t="s">
         <v>351</v>
       </c>
       <c r="C11" s="22" t="s">
         <v>100</v>
       </c>
+      <c r="D11" s="22"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="22" t="s">
         <v>330</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="44" t="s">
         <v>342</v>
       </c>
-      <c r="C12" s="42" t="s">
+      <c r="C12" s="40" t="s">
         <v>100</v>
       </c>
+      <c r="D12" s="22"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="22" t="s">
         <v>331</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="44" t="s">
         <v>343</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>100</v>
       </c>
+      <c r="D13" s="22"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="44" t="s">
         <v>340</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>21</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="D14" s="22"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="22" t="s">
         <v>333</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="44" t="s">
         <v>341</v>
       </c>
       <c r="C15" s="22" t="s">
         <v>100</v>
       </c>
+      <c r="D15" s="22"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="B16" s="45" t="s">
+        <v>356</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>358</v>
+      </c>
+      <c r="C17" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D17" s="22"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="22" t="s">
+        <v>359</v>
+      </c>
+      <c r="B18" s="45" t="s">
+        <v>360</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="D18" s="22"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
@@ -1838,7 +1933,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C18">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2197,19 +2292,19 @@
       <c r="CF1" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="CG1" s="43" t="s">
+      <c r="CG1" s="41" t="s">
         <v>264</v>
       </c>
-      <c r="CH1" s="44" t="s">
+      <c r="CH1" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="CI1" s="43" t="s">
+      <c r="CI1" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="CJ1" s="43" t="s">
+      <c r="CJ1" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="CK1" s="43" t="s">
+      <c r="CK1" s="41" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2217,7 +2312,7 @@
       <c r="A2" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>
@@ -2844,7 +2939,7 @@
       <c r="A2" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>
@@ -3468,7 +3563,7 @@
       <c r="A2" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>
@@ -4058,7 +4153,7 @@
       <c r="A2" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>
@@ -4631,7 +4726,7 @@
       <c r="A2" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>
@@ -4866,8 +4961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AD19" sqref="AD19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5199,7 +5294,7 @@
       <c r="A2" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>
@@ -5227,7 +5322,7 @@
         <v>166</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>167</v>
@@ -5396,16 +5491,16 @@
         <v>245</v>
       </c>
       <c r="BZ2" t="s">
-        <v>327</v>
+        <v>352</v>
       </c>
       <c r="CA2" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="CB2" t="s">
         <v>83</v>
       </c>
       <c r="CC2" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -5782,7 +5877,7 @@
       <c r="A2" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>
@@ -6025,968 +6120,1741 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:CH2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="CA1" workbookViewId="0">
+      <selection activeCell="CE3" sqref="CE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21.85546875" customWidth="1"/>
-    <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="22" width="24" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="25.42578125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="4" customWidth="1"/>
+    <col min="31" max="32" width="27.5703125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="17.7109375" style="4" customWidth="1"/>
+    <col min="37" max="38" width="19.42578125" style="4" customWidth="1"/>
+    <col min="39" max="40" width="34.42578125" style="5" customWidth="1"/>
+    <col min="41" max="41" width="21.7109375" style="4" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" style="4" customWidth="1"/>
+    <col min="43" max="43" width="26.7109375" style="4" customWidth="1"/>
+    <col min="44" max="45" width="19.140625" style="4" customWidth="1"/>
+    <col min="46" max="46" width="16.5703125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="21.42578125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="12.85546875" style="4" customWidth="1"/>
+    <col min="49" max="49" width="30.7109375" style="4" customWidth="1"/>
+    <col min="50" max="50" width="91.42578125" style="4" customWidth="1"/>
+    <col min="51" max="51" width="10.5703125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="13" style="4" customWidth="1"/>
+    <col min="53" max="53" width="13.28515625" style="4" customWidth="1"/>
+    <col min="54" max="54" width="15.28515625" style="4" customWidth="1"/>
+    <col min="55" max="55" width="12.42578125" style="4" customWidth="1"/>
+    <col min="56" max="56" width="9.140625" style="4"/>
+    <col min="57" max="57" width="19.85546875" style="4" customWidth="1"/>
+    <col min="58" max="58" width="25.7109375" style="4" customWidth="1"/>
+    <col min="59" max="59" width="13.42578125" style="4" customWidth="1"/>
+    <col min="60" max="60" width="15" style="4" customWidth="1"/>
+    <col min="61" max="61" width="20.140625" style="4" customWidth="1"/>
+    <col min="62" max="62" width="21.7109375" style="4" customWidth="1"/>
+    <col min="63" max="63" width="17.28515625" style="4" customWidth="1"/>
+    <col min="64" max="64" width="17.85546875" style="4" customWidth="1"/>
+    <col min="65" max="65" width="32.5703125" style="4" customWidth="1"/>
+    <col min="66" max="66" width="24.7109375" style="4" customWidth="1"/>
+    <col min="67" max="67" width="26.5703125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="32.7109375" style="4" customWidth="1"/>
+    <col min="69" max="69" width="18.42578125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="17.85546875" style="4" customWidth="1"/>
+    <col min="71" max="71" width="17.140625" style="4" customWidth="1"/>
+    <col min="72" max="72" width="18.5703125" style="4" customWidth="1"/>
+    <col min="73" max="73" width="18.42578125" style="4" customWidth="1"/>
+    <col min="74" max="75" width="17.85546875" style="4" customWidth="1"/>
+    <col min="76" max="78" width="25.28515625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="17.28515625" style="4" customWidth="1"/>
+    <col min="80" max="80" width="19.28515625" style="4" customWidth="1"/>
+    <col min="81" max="81" width="24.140625" style="4" customWidth="1"/>
+    <col min="82" max="82" width="16.28515625" style="4" customWidth="1"/>
+    <col min="83" max="83" width="16" style="4" customWidth="1"/>
+    <col min="84" max="84" width="19.42578125" style="4" customWidth="1"/>
+    <col min="85" max="85" width="19.85546875" style="4" customWidth="1"/>
+    <col min="86" max="86" width="17.5703125" style="4" customWidth="1"/>
+    <col min="87" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:86" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="O1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="AH1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP1" s="7" t="s">
         <v>47</v>
       </c>
+      <c r="AQ1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="CA1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="CB1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="CC1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>264</v>
+      </c>
+      <c r="CE1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="str">
-        <f ca="1">CONCATENATE("HLNew Lead"," ",RANDBETWEEN(1,999))</f>
-        <v>HLNew Lead 230</v>
-      </c>
-      <c r="B2" s="2">
-        <f ca="1">RANDBETWEEN(6789000000,9999999999)</f>
-        <v>9079859646</v>
-      </c>
-      <c r="C2" s="2" t="str">
-        <f ca="1">CONCATENATE(SUBSTITUTE($A2," ",""),"@gmail.com")</f>
-        <v>HLNewLead230@gmail.com</v>
-      </c>
-      <c r="D2" s="2" t="str">
-        <f ca="1">CONCATENATE(RANDBETWEEN(10,30),RANDBETWEEN(10,12),RANDBETWEEN(1951,2004))</f>
-        <v>13111982</v>
-      </c>
-      <c r="E2" s="2" t="str">
-        <f ca="1">CONCATENATE(CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),CHAR(RANDBETWEEN(65,90)))</f>
-        <v>STSFV1733Z</v>
-      </c>
-      <c r="F2" s="4" t="str">
-        <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Male","Female")</f>
-        <v>Female</v>
+    <row r="2" spans="1:86" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="U2" s="23">
+        <v>4200000</v>
+      </c>
+      <c r="V2" s="23"/>
+      <c r="W2" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AN2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ2" s="17"/>
+      <c r="AR2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AS2" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="AT2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV2" s="17"/>
+      <c r="AW2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX2" s="17"/>
+      <c r="AY2" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="AZ2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="BA2" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="BB2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="BD2" s="17"/>
+      <c r="BE2" s="17"/>
+      <c r="BF2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="BG2" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI2" s="17"/>
+      <c r="BJ2" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="BK2" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="BL2" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="BM2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BX2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="BY2" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="BZ2" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="CA2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="CB2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>363</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>364</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>83</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>365</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2">
+      <formula1>"January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
+      <formula1>"Buying new property,Buying resale property,Construction of property,Renovation of existing property"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="BE22" sqref="BE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" customWidth="1"/>
-    <col min="3" max="3" width="17" style="4" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="22" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="22" width="24" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="25.42578125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="4" customWidth="1"/>
+    <col min="31" max="32" width="27.5703125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="17.7109375" style="4" customWidth="1"/>
+    <col min="37" max="38" width="19.42578125" style="4" customWidth="1"/>
+    <col min="39" max="40" width="34.42578125" style="5" customWidth="1"/>
+    <col min="41" max="41" width="21.7109375" style="4" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" style="4" customWidth="1"/>
+    <col min="43" max="43" width="26.7109375" style="4" customWidth="1"/>
+    <col min="44" max="45" width="19.140625" style="4" customWidth="1"/>
+    <col min="46" max="46" width="16.5703125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="21.42578125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="12.85546875" style="4" customWidth="1"/>
+    <col min="49" max="49" width="30.7109375" style="4" customWidth="1"/>
+    <col min="50" max="50" width="35.28515625" style="4" customWidth="1"/>
+    <col min="51" max="51" width="10.5703125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="13" style="4" customWidth="1"/>
+    <col min="53" max="53" width="13.28515625" style="4" customWidth="1"/>
+    <col min="54" max="54" width="15.28515625" style="4" customWidth="1"/>
+    <col min="55" max="55" width="12.42578125" style="4" customWidth="1"/>
+    <col min="56" max="56" width="9.140625" style="4"/>
+    <col min="57" max="57" width="19.85546875" style="4" customWidth="1"/>
+    <col min="58" max="58" width="19.140625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="17.5703125" style="4" customWidth="1"/>
+    <col min="60" max="60" width="15" style="4" customWidth="1"/>
+    <col min="61" max="61" width="20.140625" style="4" customWidth="1"/>
+    <col min="62" max="62" width="21.7109375" style="4" customWidth="1"/>
+    <col min="63" max="63" width="17.28515625" style="4" customWidth="1"/>
+    <col min="64" max="64" width="17.85546875" style="4" customWidth="1"/>
+    <col min="65" max="65" width="32.5703125" style="4" customWidth="1"/>
+    <col min="66" max="66" width="24.7109375" style="4" customWidth="1"/>
+    <col min="67" max="67" width="26.5703125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="32.7109375" style="4" customWidth="1"/>
+    <col min="69" max="69" width="18.42578125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="17.85546875" style="4" customWidth="1"/>
+    <col min="71" max="71" width="17.140625" style="4" customWidth="1"/>
+    <col min="72" max="72" width="18.5703125" style="4" customWidth="1"/>
+    <col min="73" max="73" width="18.42578125" style="4" customWidth="1"/>
+    <col min="74" max="74" width="17.85546875" style="4" customWidth="1"/>
+    <col min="75" max="75" width="17.28515625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="19.28515625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="24.140625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="16.28515625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="16" style="4" customWidth="1"/>
+    <col min="80" max="80" width="19.42578125" style="4" customWidth="1"/>
+    <col min="81" max="81" width="19.85546875" style="4" customWidth="1"/>
+    <col min="82" max="82" width="17.5703125" style="4" customWidth="1"/>
+    <col min="83" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:82" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" s="4" t="s">
+      <c r="B1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="BZ1" t="s">
+        <v>264</v>
+      </c>
+      <c r="CA1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D1" t="s">
+      <c r="CB1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" t="s">
+      <c r="CC1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" t="s">
+      <c r="CD1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:82" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>357</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="23">
+        <v>4200000</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AN2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AS2" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="AT2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV2" s="17"/>
+      <c r="AW2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX2" s="17"/>
+      <c r="AY2" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="AZ2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="BA2" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="BB2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="BD2" s="17"/>
+      <c r="BE2" s="17"/>
+      <c r="BF2" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="BG2" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI2" s="17"/>
+      <c r="BJ2" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="BK2" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="BL2" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="BM2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="BX2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="BY2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>297</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>298</v>
+      </c>
+      <c r="CB2" t="s">
         <v>83</v>
       </c>
-      <c r="E2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D4" t="s">
-        <v>83</v>
-      </c>
-      <c r="E4" t="s">
-        <v>91</v>
-      </c>
-      <c r="F4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" t="s">
-        <v>93</v>
-      </c>
-      <c r="F5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B7" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D8" t="s">
-        <v>83</v>
-      </c>
-      <c r="E8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" t="s">
-        <v>117</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D11" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" t="s">
-        <v>83</v>
-      </c>
-      <c r="E12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" t="s">
-        <v>139</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="D13" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" t="s">
-        <v>141</v>
-      </c>
-      <c r="F13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>71</v>
-      </c>
-      <c r="B14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="D14" t="s">
-        <v>83</v>
-      </c>
-      <c r="E14" t="s">
-        <v>144</v>
-      </c>
-      <c r="F14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" t="s">
-        <v>146</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="D15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" t="s">
-        <v>149</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D16" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>99</v>
-      </c>
-      <c r="B17" t="s">
-        <v>149</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E17" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B18" t="s">
-        <v>157</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D18" t="s">
-        <v>83</v>
-      </c>
-      <c r="E18" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>99</v>
-      </c>
-      <c r="B19" t="s">
-        <v>157</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="D19" t="s">
-        <v>83</v>
-      </c>
-      <c r="E19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" t="s">
-        <v>173</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="D20" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" t="s">
-        <v>175</v>
-      </c>
-      <c r="F20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" t="s">
-        <v>173</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D21" t="s">
-        <v>178</v>
-      </c>
-      <c r="E21" t="s">
-        <v>176</v>
-      </c>
-      <c r="F21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>99</v>
-      </c>
-      <c r="B22" t="s">
-        <v>172</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D22" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>99</v>
-      </c>
-      <c r="B23" t="s">
-        <v>172</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D23" t="s">
-        <v>83</v>
-      </c>
-      <c r="E23" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B24" t="s">
-        <v>182</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D24" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" t="s">
-        <v>182</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D25" t="s">
-        <v>83</v>
-      </c>
-      <c r="E25" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B26" t="s">
-        <v>173</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D26" t="s">
-        <v>187</v>
-      </c>
-      <c r="E26" t="s">
-        <v>188</v>
-      </c>
-      <c r="F26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>99</v>
-      </c>
-      <c r="B27" t="s">
-        <v>182</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D27" t="s">
-        <v>83</v>
-      </c>
-      <c r="E27" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" t="s">
-        <v>182</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D28" t="s">
-        <v>83</v>
-      </c>
-      <c r="E28" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>192</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D29" t="s">
-        <v>83</v>
-      </c>
-      <c r="E29" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>192</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="D30" t="s">
-        <v>83</v>
-      </c>
-      <c r="E30" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" t="s">
-        <v>203</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E31" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>99</v>
-      </c>
-      <c r="B32" t="s">
-        <v>203</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="D32" t="s">
-        <v>83</v>
-      </c>
-      <c r="E32" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B33" t="s">
-        <v>231</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D33" t="s">
-        <v>83</v>
-      </c>
-      <c r="E33" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" t="s">
-        <v>231</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D34" t="s">
-        <v>83</v>
-      </c>
-      <c r="E34" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>99</v>
-      </c>
-      <c r="B35" t="s">
-        <v>231</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="D35" t="s">
-        <v>83</v>
-      </c>
-      <c r="E35" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>99</v>
-      </c>
-      <c r="B36" t="s">
-        <v>236</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="D36" t="s">
-        <v>83</v>
-      </c>
-      <c r="E36" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>99</v>
-      </c>
-      <c r="B37" t="s">
-        <v>236</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="D37" t="s">
-        <v>83</v>
-      </c>
-      <c r="E37" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>99</v>
-      </c>
-      <c r="B38" t="s">
-        <v>139</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="D38" t="s">
-        <v>83</v>
-      </c>
-      <c r="E38" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>99</v>
-      </c>
-      <c r="B39" t="s">
-        <v>139</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="D39" t="s">
-        <v>83</v>
-      </c>
-      <c r="E39" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>99</v>
-      </c>
-      <c r="B40" t="s">
-        <v>247</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D40" t="s">
-        <v>83</v>
-      </c>
-      <c r="E40" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>99</v>
-      </c>
-      <c r="B41" t="s">
-        <v>247</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="D41" t="s">
-        <v>83</v>
-      </c>
-      <c r="E41" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>99</v>
-      </c>
-      <c r="B42" t="s">
-        <v>251</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="D42" t="s">
-        <v>83</v>
-      </c>
-      <c r="E42" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>99</v>
-      </c>
-      <c r="B43" t="s">
-        <v>251</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="D43" t="s">
-        <v>83</v>
-      </c>
-      <c r="E43" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" s="4" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B44" s="4">
-        <v>9879879815</v>
-      </c>
-      <c r="C44" s="5" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>99</v>
-      </c>
-      <c r="B45" t="s">
-        <v>260</v>
-      </c>
-      <c r="C45" t="s">
-        <v>261</v>
-      </c>
-      <c r="D45" t="s">
-        <v>83</v>
-      </c>
-      <c r="E45" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>99</v>
-      </c>
-      <c r="B46" t="s">
-        <v>260</v>
-      </c>
-      <c r="C46" t="s">
-        <v>261</v>
-      </c>
-      <c r="D46" t="s">
-        <v>83</v>
-      </c>
-      <c r="E46" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>270</v>
-      </c>
-      <c r="B47" t="s">
-        <v>271</v>
-      </c>
-      <c r="C47" t="s">
-        <v>273</v>
-      </c>
-      <c r="D47" t="s">
-        <v>83</v>
-      </c>
-      <c r="E47" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>270</v>
-      </c>
-      <c r="B48" t="s">
-        <v>271</v>
-      </c>
-      <c r="C48" t="s">
-        <v>273</v>
-      </c>
-      <c r="D48" t="s">
-        <v>83</v>
-      </c>
-      <c r="E48" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>270</v>
-      </c>
-      <c r="B49" t="s">
-        <v>271</v>
-      </c>
-      <c r="C49" t="s">
-        <v>273</v>
-      </c>
-      <c r="D49" t="s">
-        <v>83</v>
-      </c>
-      <c r="E49" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>270</v>
-      </c>
-      <c r="B50" t="s">
-        <v>277</v>
-      </c>
-      <c r="C50" t="s">
-        <v>279</v>
-      </c>
-      <c r="D50" t="s">
-        <v>83</v>
-      </c>
-      <c r="E50" t="s">
-        <v>280</v>
+      <c r="CC2" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2">
+      <formula1>"January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
+      <formula1>"Buying new property,Buying resale property,Construction of property,Renovation of existing property"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CE2"/>
+  <sheetViews>
+    <sheetView topLeftCell="BQ1" workbookViewId="0">
+      <selection activeCell="BV18" sqref="BV18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="21" width="24" style="4" customWidth="1"/>
+    <col min="22" max="22" width="25.140625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="25.42578125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="4" customWidth="1"/>
+    <col min="31" max="32" width="27.5703125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="17.7109375" style="4" customWidth="1"/>
+    <col min="37" max="38" width="19.42578125" style="4" customWidth="1"/>
+    <col min="39" max="40" width="34.42578125" style="5" customWidth="1"/>
+    <col min="41" max="41" width="21.7109375" style="4" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" style="4" customWidth="1"/>
+    <col min="43" max="44" width="26.7109375" style="4" customWidth="1"/>
+    <col min="45" max="46" width="19.140625" style="4" customWidth="1"/>
+    <col min="47" max="47" width="16.5703125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="21.42578125" style="4" customWidth="1"/>
+    <col min="49" max="49" width="12.85546875" style="4" customWidth="1"/>
+    <col min="50" max="50" width="30.7109375" style="4" customWidth="1"/>
+    <col min="51" max="51" width="32.140625" style="4" customWidth="1"/>
+    <col min="52" max="52" width="10.5703125" style="4" customWidth="1"/>
+    <col min="53" max="53" width="13" style="4" customWidth="1"/>
+    <col min="54" max="54" width="13.28515625" style="4" customWidth="1"/>
+    <col min="55" max="55" width="15.28515625" style="4" customWidth="1"/>
+    <col min="56" max="56" width="12.42578125" style="4" customWidth="1"/>
+    <col min="57" max="57" width="9.140625" style="4"/>
+    <col min="58" max="58" width="19.85546875" style="4" customWidth="1"/>
+    <col min="59" max="59" width="25.7109375" style="4" customWidth="1"/>
+    <col min="60" max="60" width="13.42578125" style="4" customWidth="1"/>
+    <col min="61" max="61" width="15" style="4" customWidth="1"/>
+    <col min="62" max="62" width="20.140625" style="4" customWidth="1"/>
+    <col min="63" max="63" width="21.7109375" style="4" customWidth="1"/>
+    <col min="64" max="64" width="17.28515625" style="4" customWidth="1"/>
+    <col min="65" max="65" width="17.85546875" style="4" customWidth="1"/>
+    <col min="66" max="66" width="24.140625" style="4" customWidth="1"/>
+    <col min="67" max="67" width="24.7109375" style="4" customWidth="1"/>
+    <col min="68" max="68" width="29.5703125" style="4" customWidth="1"/>
+    <col min="69" max="69" width="32.7109375" style="4" customWidth="1"/>
+    <col min="70" max="70" width="18.42578125" style="4" customWidth="1"/>
+    <col min="71" max="71" width="17.85546875" style="4" customWidth="1"/>
+    <col min="72" max="72" width="17.140625" style="4" customWidth="1"/>
+    <col min="73" max="73" width="18.5703125" style="4" customWidth="1"/>
+    <col min="74" max="74" width="18.42578125" style="4" customWidth="1"/>
+    <col min="75" max="75" width="17.85546875" style="4" customWidth="1"/>
+    <col min="76" max="76" width="17.28515625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="19.28515625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="24.140625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="16.28515625" style="4" customWidth="1"/>
+    <col min="80" max="80" width="16" style="4" customWidth="1"/>
+    <col min="81" max="81" width="19.42578125" style="4" customWidth="1"/>
+    <col min="82" max="82" width="19.85546875" style="4" customWidth="1"/>
+    <col min="83" max="83" width="17.5703125" style="4" customWidth="1"/>
+    <col min="84" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:83" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AU1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AV1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="BM1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>264</v>
+      </c>
+      <c r="CB1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:83" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>260</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="23">
+        <v>4200000</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AN2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR2" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="AS2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AT2" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="AU2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AW2" s="17"/>
+      <c r="AX2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AY2" s="17"/>
+      <c r="AZ2" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="BA2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="BB2" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BD2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="BE2" s="17"/>
+      <c r="BF2" s="17"/>
+      <c r="BG2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="BH2" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="BI2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BJ2" s="17"/>
+      <c r="BK2" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="BL2" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="BM2" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="BX2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="BY2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="BZ2" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA2">
+      <formula1>"January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
+      <formula1>"Buying new property,Buying resale property,Construction of property,Renovation of existing property"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
+      <formula1>"Less than 3 years,3 or more years"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2">
+      <formula1>"Individual,Non-Individual"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BG2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BQ2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6995,7 +7863,7 @@
   <dimension ref="A1:BW3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7336,18 +8204,18 @@
       <c r="L2" s="10"/>
       <c r="M2" s="12" t="str">
         <f ca="1">Sheet1!A2</f>
-        <v>HLNew Lead 230</v>
+        <v>HLNew Lead 24</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>173</v>
       </c>
       <c r="O2" s="10" t="str">
         <f ca="1">Sheet1!C2</f>
-        <v>HLNewLead230@gmail.com</v>
+        <v>HLNewLead24@gmail.com</v>
       </c>
       <c r="P2" s="10" t="str">
         <f ca="1">Sheet1!D2</f>
-        <v>13111982</v>
+        <v>12111958</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>76</v>
@@ -7382,7 +8250,7 @@
       <c r="AC2" s="10"/>
       <c r="AD2" s="10" t="str">
         <f ca="1">Sheet1!E2</f>
-        <v>STSFV1733Z</v>
+        <v>UTMDU1742T</v>
       </c>
       <c r="AE2" s="10" t="s">
         <v>36</v>
@@ -7670,12 +8538,979 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.28515625" customWidth="1"/>
+    <col min="2" max="2" width="21.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="str">
+        <f ca="1">CONCATENATE("HLNew Lead"," ",RANDBETWEEN(1,999))</f>
+        <v>HLNew Lead 24</v>
+      </c>
+      <c r="B2" s="2">
+        <f ca="1">RANDBETWEEN(6789000000,9999999999)</f>
+        <v>7740625513</v>
+      </c>
+      <c r="C2" s="2" t="str">
+        <f ca="1">CONCATENATE(SUBSTITUTE($A2," ",""),"@gmail.com")</f>
+        <v>HLNewLead24@gmail.com</v>
+      </c>
+      <c r="D2" s="2" t="str">
+        <f ca="1">CONCATENATE(RANDBETWEEN(10,30),RANDBETWEEN(10,12),RANDBETWEEN(1951,2004))</f>
+        <v>12111958</v>
+      </c>
+      <c r="E2" s="2" t="str">
+        <f ca="1">CONCATENATE(CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),CHAR(RANDBETWEEN(65,90)))</f>
+        <v>UTMDU1742T</v>
+      </c>
+      <c r="F2" s="4" t="str">
+        <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Male","Female")</f>
+        <v>Female</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
+    <col min="3" max="3" width="17" style="4" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D6" t="s">
+        <v>83</v>
+      </c>
+      <c r="E6" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" t="s">
+        <v>141</v>
+      </c>
+      <c r="F13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" t="s">
+        <v>144</v>
+      </c>
+      <c r="F14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B16" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" t="s">
+        <v>157</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>71</v>
+      </c>
+      <c r="B20" t="s">
+        <v>173</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" t="s">
+        <v>175</v>
+      </c>
+      <c r="F20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>173</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D21" t="s">
+        <v>178</v>
+      </c>
+      <c r="E21" t="s">
+        <v>176</v>
+      </c>
+      <c r="F21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B22" t="s">
+        <v>172</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>173</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="D26" t="s">
+        <v>187</v>
+      </c>
+      <c r="E26" t="s">
+        <v>188</v>
+      </c>
+      <c r="F26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>182</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D27" t="s">
+        <v>83</v>
+      </c>
+      <c r="E27" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D29" t="s">
+        <v>83</v>
+      </c>
+      <c r="E29" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>203</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D31" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>203</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" t="s">
+        <v>231</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
+        <v>231</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D34" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
+        <v>231</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="D35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" t="s">
+        <v>236</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="D36" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" t="s">
+        <v>236</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="D37" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>99</v>
+      </c>
+      <c r="B38" t="s">
+        <v>139</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>99</v>
+      </c>
+      <c r="B39" t="s">
+        <v>139</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D39" t="s">
+        <v>83</v>
+      </c>
+      <c r="E39" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+      <c r="B40" t="s">
+        <v>247</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D40" t="s">
+        <v>83</v>
+      </c>
+      <c r="E40" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>99</v>
+      </c>
+      <c r="B41" t="s">
+        <v>247</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="D41" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" t="s">
+        <v>251</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="D42" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" t="s">
+        <v>251</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="D43" t="s">
+        <v>83</v>
+      </c>
+      <c r="E43" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" s="4" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B44" s="4">
+        <v>9879879815</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" t="s">
+        <v>260</v>
+      </c>
+      <c r="C45" t="s">
+        <v>261</v>
+      </c>
+      <c r="D45" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>99</v>
+      </c>
+      <c r="B46" t="s">
+        <v>260</v>
+      </c>
+      <c r="C46" t="s">
+        <v>261</v>
+      </c>
+      <c r="D46" t="s">
+        <v>83</v>
+      </c>
+      <c r="E46" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>270</v>
+      </c>
+      <c r="B47" t="s">
+        <v>271</v>
+      </c>
+      <c r="C47" t="s">
+        <v>273</v>
+      </c>
+      <c r="D47" t="s">
+        <v>83</v>
+      </c>
+      <c r="E47" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>270</v>
+      </c>
+      <c r="B48" t="s">
+        <v>271</v>
+      </c>
+      <c r="C48" t="s">
+        <v>273</v>
+      </c>
+      <c r="D48" t="s">
+        <v>83</v>
+      </c>
+      <c r="E48" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>270</v>
+      </c>
+      <c r="B49" t="s">
+        <v>271</v>
+      </c>
+      <c r="C49" t="s">
+        <v>273</v>
+      </c>
+      <c r="D49" t="s">
+        <v>83</v>
+      </c>
+      <c r="E49" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>270</v>
+      </c>
+      <c r="B50" t="s">
+        <v>277</v>
+      </c>
+      <c r="C50" t="s">
+        <v>279</v>
+      </c>
+      <c r="D50" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" t="s">
+        <v>280</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BK2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7966,18 +9801,18 @@
       <c r="M2" s="10"/>
       <c r="N2" s="12" t="str">
         <f ca="1">Sheet1!A2</f>
-        <v>HLNew Lead 230</v>
+        <v>HLNew Lead 24</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>173</v>
       </c>
       <c r="P2" s="10" t="str">
         <f ca="1">Sheet1!C2</f>
-        <v>HLNewLead230@gmail.com</v>
+        <v>HLNewLead24@gmail.com</v>
       </c>
       <c r="Q2" s="10" t="str">
         <f ca="1">Sheet1!D2</f>
-        <v>13111982</v>
+        <v>12111958</v>
       </c>
       <c r="R2" s="13" t="s">
         <v>76</v>
@@ -8012,7 +9847,7 @@
       <c r="AD2" s="10"/>
       <c r="AE2" s="10" t="str">
         <f ca="1">Sheet1!E2</f>
-        <v>STSFV1733Z</v>
+        <v>UTMDU1742T</v>
       </c>
       <c r="AF2" s="10" t="s">
         <v>36</v>
@@ -8098,89 +9933,89 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.7109375" style="33" customWidth="1"/>
-    <col min="2" max="2" width="21" style="37" customWidth="1"/>
-    <col min="3" max="3" width="14" style="33" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="33" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" style="33" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="33"/>
+    <col min="1" max="1" width="39.7109375" style="32" customWidth="1"/>
+    <col min="2" max="2" width="21" style="36" customWidth="1"/>
+    <col min="3" max="3" width="14" style="32" customWidth="1"/>
+    <col min="4" max="4" width="17.28515625" style="32" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="32" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="32"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>295</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="30" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>323</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="35" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>323</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="C3" s="36"/>
+      <c r="C3" s="35"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>323</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="C4" s="36"/>
+      <c r="C4" s="35"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="35" t="s">
         <v>323</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="35"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="35" t="s">
         <v>323</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="35"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="35" t="s">
         <v>323</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="C7" s="36"/>
+      <c r="C7" s="35"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="35" t="s">
         <v>323</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="35"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -8195,8 +10030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH2"/>
   <sheetViews>
-    <sheetView topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="AX21" sqref="AX21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8544,7 +10379,7 @@
       <c r="A2" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>
@@ -9122,7 +10957,7 @@
       <c r="A2" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>
@@ -9700,7 +11535,7 @@
       <c r="A2" s="17" t="s">
         <v>281</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>
@@ -10279,7 +12114,7 @@
       <c r="A2" s="17" t="s">
         <v>287</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>
@@ -10888,7 +12723,7 @@
       <c r="A2" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="29" t="s">
         <v>296</v>
       </c>
       <c r="C2" s="17"/>

</xml_diff>

<commit_message>
Added script for Add Financial CoApplicant
</commit_message>
<xml_diff>
--- a/KMBAutomation/TestData/TestData_LeadDetails.xlsx
+++ b/KMBAutomation/TestData/TestData_LeadDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="7470" tabRatio="847"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15030" windowHeight="7470" tabRatio="847" firstSheet="20" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="TestScenario" sheetId="3" r:id="rId1"/>
@@ -26,15 +26,19 @@
     <sheet name="HLDAPKotakSmartHomeSalIndian" sheetId="20" r:id="rId17"/>
     <sheet name="HLDAPKotakSmartHomeSalNRI" sheetId="21" r:id="rId18"/>
     <sheet name="HLDAPKotakSmartHomeIndividual" sheetId="22" r:id="rId19"/>
-    <sheet name="Sheet1" sheetId="4" r:id="rId20"/>
-    <sheet name="Output" sheetId="2" r:id="rId21"/>
+    <sheet name="HLDAPHomeLoanOverdraftSalIndian" sheetId="23" r:id="rId20"/>
+    <sheet name="HLDAPHomeLoanOverdraftIndividul" sheetId="24" r:id="rId21"/>
+    <sheet name="HLDAPHomeLoanOverdraftNonInd" sheetId="25" r:id="rId22"/>
+    <sheet name="HLDAPHLSalIndAddFinCOApp" sheetId="26" r:id="rId23"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId24"/>
+    <sheet name="Output" sheetId="2" r:id="rId25"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2783" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3418" uniqueCount="405">
   <si>
     <t>Username</t>
   </si>
@@ -1136,6 +1140,120 @@
   </si>
   <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>9879879820</t>
+  </si>
+  <si>
+    <t>9879879706</t>
+  </si>
+  <si>
+    <t>00105004</t>
+  </si>
+  <si>
+    <t>04/07/2022 11:46 AM</t>
+  </si>
+  <si>
+    <t>TC18</t>
+  </si>
+  <si>
+    <t>TC19</t>
+  </si>
+  <si>
+    <t>TC20</t>
+  </si>
+  <si>
+    <t>HLDAPHomeLoanOverdraftSalariedIndian</t>
+  </si>
+  <si>
+    <t>HLDAPHomeLoanOverdraftIndividual</t>
+  </si>
+  <si>
+    <t>HLDAPHomeLoanOverdraftNonIndividual</t>
+  </si>
+  <si>
+    <t>Home Loan Overdraft</t>
+  </si>
+  <si>
+    <t>9879879707</t>
+  </si>
+  <si>
+    <t>9879879821</t>
+  </si>
+  <si>
+    <t>4500000</t>
+  </si>
+  <si>
+    <t>4000000</t>
+  </si>
+  <si>
+    <t>4200000</t>
+  </si>
+  <si>
+    <t>06/07/2022 11:07 AM</t>
+  </si>
+  <si>
+    <t>FinCoAppName</t>
+  </si>
+  <si>
+    <t>FinCoAppMobile</t>
+  </si>
+  <si>
+    <t>FinCoAppEmail</t>
+  </si>
+  <si>
+    <t>FinCoAppRealtion</t>
+  </si>
+  <si>
+    <t>FinCoAppGender</t>
+  </si>
+  <si>
+    <t>Husband</t>
+  </si>
+  <si>
+    <t>8087537474</t>
+  </si>
+  <si>
+    <t>Amit Vibhute</t>
+  </si>
+  <si>
+    <t>amit@gmail.com</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>CoAppType</t>
+  </si>
+  <si>
+    <t>CoAppPAN</t>
+  </si>
+  <si>
+    <t>CoAppNetSalary</t>
+  </si>
+  <si>
+    <t>300000</t>
+  </si>
+  <si>
+    <t>TC21</t>
+  </si>
+  <si>
+    <t>HLDAPHomeLoanSalIndianAddFinCoApp</t>
+  </si>
+  <si>
+    <t>9879879711</t>
+  </si>
+  <si>
+    <t>00105248</t>
+  </si>
+  <si>
+    <t>12/07/2022 2:26 PM</t>
+  </si>
+  <si>
+    <t>CoAppResidentType</t>
+  </si>
+  <si>
+    <t>CoAppProfitAfterTax</t>
   </si>
 </sst>
 </file>
@@ -1193,7 +1311,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1248,6 +1366,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -1288,7 +1412,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1357,6 +1481,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1683,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1695,7 +1821,11 @@
     <col min="2" max="2" width="49.140625" style="25" customWidth="1"/>
     <col min="3" max="3" width="17.85546875" style="25" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" style="25" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="25"/>
+    <col min="5" max="5" width="17.5703125" style="25" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="25" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" style="25" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="25" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1746,7 +1876,9 @@
       <c r="C4" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D4" s="22"/>
+      <c r="D4" s="22" t="s">
+        <v>366</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
@@ -1888,7 +2020,7 @@
         <v>356</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>21</v>
+        <v>100</v>
       </c>
       <c r="D16" s="22" t="s">
         <v>366</v>
@@ -1916,7 +2048,63 @@
       <c r="C18" s="22" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="22"/>
+      <c r="D18" s="22" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="44" t="s">
+        <v>371</v>
+      </c>
+      <c r="B19" s="44" t="s">
+        <v>374</v>
+      </c>
+      <c r="C19" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="46"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="44" t="s">
+        <v>372</v>
+      </c>
+      <c r="B20" s="44" t="s">
+        <v>375</v>
+      </c>
+      <c r="C20" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="46" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="44" t="s">
+        <v>373</v>
+      </c>
+      <c r="B21" s="44" t="s">
+        <v>376</v>
+      </c>
+      <c r="C21" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="D21" s="46" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>399</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" t="s">
+        <v>366</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C1:C1048576">
@@ -3201,10 +3389,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CK2"/>
+  <dimension ref="A1:CL2"/>
   <sheetViews>
-    <sheetView topLeftCell="AY1" workbookViewId="0">
-      <selection activeCell="BF20" sqref="BF20"/>
+    <sheetView topLeftCell="BH1" workbookViewId="0">
+      <selection activeCell="BL3" sqref="BL3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3264,33 +3452,33 @@
     <col min="61" max="61" width="25.7109375" style="4" customWidth="1"/>
     <col min="62" max="62" width="13.42578125" style="4" customWidth="1"/>
     <col min="63" max="63" width="15" style="4" customWidth="1"/>
-    <col min="64" max="64" width="20.140625" style="4" customWidth="1"/>
-    <col min="65" max="65" width="21.7109375" style="4" customWidth="1"/>
-    <col min="66" max="66" width="17.28515625" style="4" customWidth="1"/>
-    <col min="67" max="67" width="17.85546875" style="4" customWidth="1"/>
-    <col min="68" max="68" width="32.5703125" style="4" customWidth="1"/>
-    <col min="69" max="69" width="24.7109375" style="4" customWidth="1"/>
-    <col min="70" max="70" width="26.5703125" style="4" customWidth="1"/>
-    <col min="71" max="71" width="32.7109375" style="4" customWidth="1"/>
-    <col min="72" max="72" width="18.42578125" style="4" customWidth="1"/>
-    <col min="73" max="73" width="17.85546875" style="4" customWidth="1"/>
-    <col min="74" max="74" width="17.140625" style="4" customWidth="1"/>
-    <col min="75" max="75" width="18.5703125" style="4" customWidth="1"/>
-    <col min="76" max="76" width="18.42578125" style="4" customWidth="1"/>
-    <col min="77" max="78" width="17.85546875" style="4" customWidth="1"/>
-    <col min="79" max="81" width="25.28515625" style="4" customWidth="1"/>
-    <col min="82" max="82" width="17.28515625" style="4" customWidth="1"/>
-    <col min="83" max="83" width="19.28515625" style="4" customWidth="1"/>
-    <col min="84" max="84" width="24.140625" style="4" customWidth="1"/>
-    <col min="85" max="85" width="16.28515625" style="4" customWidth="1"/>
-    <col min="86" max="86" width="16" style="4" customWidth="1"/>
-    <col min="87" max="87" width="19.42578125" style="4" customWidth="1"/>
-    <col min="88" max="88" width="19.85546875" style="4" customWidth="1"/>
-    <col min="89" max="89" width="17.5703125" style="4" customWidth="1"/>
-    <col min="90" max="16384" width="9.140625" style="4"/>
+    <col min="64" max="65" width="20.140625" style="4" customWidth="1"/>
+    <col min="66" max="66" width="30.28515625" style="4" customWidth="1"/>
+    <col min="67" max="67" width="17.28515625" style="4" customWidth="1"/>
+    <col min="68" max="68" width="17.85546875" style="4" customWidth="1"/>
+    <col min="69" max="69" width="32.5703125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="24.7109375" style="4" customWidth="1"/>
+    <col min="71" max="71" width="26.5703125" style="4" customWidth="1"/>
+    <col min="72" max="72" width="32.7109375" style="4" customWidth="1"/>
+    <col min="73" max="73" width="18.42578125" style="4" customWidth="1"/>
+    <col min="74" max="74" width="17.85546875" style="4" customWidth="1"/>
+    <col min="75" max="75" width="17.140625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="18.5703125" style="4" customWidth="1"/>
+    <col min="77" max="77" width="18.42578125" style="4" customWidth="1"/>
+    <col min="78" max="79" width="17.85546875" style="4" customWidth="1"/>
+    <col min="80" max="82" width="25.28515625" style="4" customWidth="1"/>
+    <col min="83" max="83" width="17.28515625" style="4" customWidth="1"/>
+    <col min="84" max="84" width="19.28515625" style="4" customWidth="1"/>
+    <col min="85" max="85" width="24.140625" style="4" customWidth="1"/>
+    <col min="86" max="86" width="16.28515625" style="4" customWidth="1"/>
+    <col min="87" max="87" width="16" style="4" customWidth="1"/>
+    <col min="88" max="88" width="19.42578125" style="4" customWidth="1"/>
+    <col min="89" max="89" width="19.85546875" style="4" customWidth="1"/>
+    <col min="90" max="90" width="17.5703125" style="4" customWidth="1"/>
+    <col min="91" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:89" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:90" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>74</v>
       </c>
@@ -3484,82 +3672,85 @@
         <v>142</v>
       </c>
       <c r="BM1" s="16" t="s">
-        <v>160</v>
+        <v>289</v>
       </c>
       <c r="BN1" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="BO1" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="BO1" s="16" t="s">
+      <c r="BP1" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BR1" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="CA1" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CB1" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CC1" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="CC1" s="3" t="s">
+      <c r="CD1" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="CD1" s="3" t="s">
+      <c r="CE1" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="CE1" s="3" t="s">
+      <c r="CF1" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="CF1" s="3" t="s">
+      <c r="CG1" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CH1" t="s">
         <v>264</v>
       </c>
-      <c r="CH1" s="4" t="s">
+      <c r="CI1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="CI1" t="s">
+      <c r="CJ1" t="s">
         <v>56</v>
       </c>
-      <c r="CJ1" t="s">
+      <c r="CK1" t="s">
         <v>57</v>
       </c>
-      <c r="CK1" t="s">
+      <c r="CL1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:89" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:90" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>319</v>
       </c>
@@ -3711,79 +3902,82 @@
       </c>
       <c r="BL2" s="17"/>
       <c r="BM2" s="17" t="s">
-        <v>161</v>
+        <v>380</v>
       </c>
       <c r="BN2" s="17" t="s">
-        <v>164</v>
+        <v>382</v>
       </c>
       <c r="BO2" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="BP2" s="4" t="s">
+      <c r="BP2" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BQ2" s="4" t="s">
+      <c r="BR2" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="BR2" s="4" t="s">
+      <c r="BS2" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="BS2" s="4" t="s">
+      <c r="BT2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="BT2" s="4" t="s">
+      <c r="BU2" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="BU2" s="4" t="s">
+      <c r="BV2" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="BV2" s="4" t="s">
+      <c r="BW2" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="BW2" s="4" t="s">
+      <c r="BX2" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="BX2" s="4" t="s">
+      <c r="BY2" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="BY2" s="4" t="s">
+      <c r="BZ2" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="BZ2" s="4" t="s">
+      <c r="CA2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="CA2" s="4" t="s">
+      <c r="CB2" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="CB2" s="4" t="s">
+      <c r="CC2" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="CC2" s="4" t="s">
+      <c r="CD2" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="CD2" s="4" t="s">
+      <c r="CE2" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="CE2" s="4" t="s">
+      <c r="CF2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="CF2" s="4" t="s">
+      <c r="CG2" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="CG2"/>
       <c r="CH2"/>
       <c r="CI2"/>
       <c r="CJ2"/>
+      <c r="CK2"/>
     </row>
   </sheetData>
   <dataValidations count="11">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="W2">
       <formula1>"Buying new property,Buying resale property,Construction of property,Renovation of existing property"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BR2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BS2">
       <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BS2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BT2">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL2">
@@ -3824,7 +4018,7 @@
   <dimension ref="A1:CC2"/>
   <sheetViews>
     <sheetView topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AR21" sqref="AR21"/>
+      <selection activeCell="AS21" sqref="AS21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4397,7 +4591,7 @@
   <dimension ref="A1:CC2"/>
   <sheetViews>
     <sheetView topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AS24" sqref="AS24"/>
+      <selection activeCell="AV24" sqref="AV24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5543,10 +5737,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CD2"/>
+  <dimension ref="A1:CE2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="BB1" workbookViewId="0">
+      <selection activeCell="BF1" sqref="BF1:BG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5599,33 +5793,33 @@
     <col min="53" max="54" width="25.7109375" style="4" customWidth="1"/>
     <col min="55" max="55" width="13.42578125" style="4" customWidth="1"/>
     <col min="56" max="56" width="15" style="4" customWidth="1"/>
-    <col min="57" max="57" width="20.140625" style="4" customWidth="1"/>
-    <col min="58" max="58" width="21.7109375" style="4" customWidth="1"/>
-    <col min="59" max="59" width="17.28515625" style="4" customWidth="1"/>
-    <col min="60" max="60" width="17.85546875" style="4" customWidth="1"/>
-    <col min="61" max="61" width="32.5703125" style="4" customWidth="1"/>
-    <col min="62" max="62" width="24.7109375" style="4" customWidth="1"/>
-    <col min="63" max="63" width="26.5703125" style="4" customWidth="1"/>
-    <col min="64" max="64" width="32.7109375" style="4" customWidth="1"/>
-    <col min="65" max="65" width="18.42578125" style="4" customWidth="1"/>
-    <col min="66" max="66" width="17.85546875" style="4" customWidth="1"/>
-    <col min="67" max="67" width="17.140625" style="4" customWidth="1"/>
-    <col min="68" max="68" width="18.5703125" style="4" customWidth="1"/>
-    <col min="69" max="69" width="18.42578125" style="4" customWidth="1"/>
-    <col min="70" max="71" width="17.85546875" style="4" customWidth="1"/>
-    <col min="72" max="74" width="25.28515625" style="4" customWidth="1"/>
-    <col min="75" max="75" width="17.28515625" style="4" customWidth="1"/>
-    <col min="76" max="76" width="19.28515625" style="4" customWidth="1"/>
-    <col min="77" max="77" width="24.140625" style="4" customWidth="1"/>
-    <col min="78" max="78" width="16.28515625" style="4" customWidth="1"/>
-    <col min="79" max="79" width="16" style="4" customWidth="1"/>
-    <col min="80" max="80" width="19.42578125" style="4" customWidth="1"/>
-    <col min="81" max="81" width="19.85546875" style="4" customWidth="1"/>
-    <col min="82" max="82" width="17.5703125" style="4" customWidth="1"/>
-    <col min="83" max="16384" width="9.140625" style="4"/>
+    <col min="57" max="58" width="20.140625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="25.28515625" style="4" customWidth="1"/>
+    <col min="60" max="60" width="17.28515625" style="4" customWidth="1"/>
+    <col min="61" max="61" width="17.85546875" style="4" customWidth="1"/>
+    <col min="62" max="62" width="32.5703125" style="4" customWidth="1"/>
+    <col min="63" max="63" width="24.7109375" style="4" customWidth="1"/>
+    <col min="64" max="64" width="26.5703125" style="4" customWidth="1"/>
+    <col min="65" max="65" width="32.7109375" style="4" customWidth="1"/>
+    <col min="66" max="66" width="18.42578125" style="4" customWidth="1"/>
+    <col min="67" max="67" width="17.85546875" style="4" customWidth="1"/>
+    <col min="68" max="68" width="17.140625" style="4" customWidth="1"/>
+    <col min="69" max="69" width="18.5703125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="18.42578125" style="4" customWidth="1"/>
+    <col min="71" max="72" width="17.85546875" style="4" customWidth="1"/>
+    <col min="73" max="75" width="25.28515625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="17.28515625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="19.28515625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="24.140625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="16.28515625" style="4" customWidth="1"/>
+    <col min="80" max="80" width="16" style="4" customWidth="1"/>
+    <col min="81" max="81" width="19.42578125" style="4" customWidth="1"/>
+    <col min="82" max="82" width="19.85546875" style="4" customWidth="1"/>
+    <col min="83" max="83" width="17.5703125" style="4" customWidth="1"/>
+    <col min="84" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:82" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>74</v>
       </c>
@@ -5798,82 +5992,85 @@
         <v>142</v>
       </c>
       <c r="BF1" s="16" t="s">
-        <v>160</v>
+        <v>289</v>
       </c>
       <c r="BG1" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="BH1" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="BH1" s="16" t="s">
+      <c r="BI1" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="BI1" s="3" t="s">
+      <c r="BJ1" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="BJ1" s="3" t="s">
+      <c r="BK1" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="BK1" s="3" t="s">
+      <c r="BL1" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="BL1" s="3" t="s">
+      <c r="BM1" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="BM1" s="3" t="s">
+      <c r="BN1" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="BN1" s="3" t="s">
+      <c r="BO1" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="BO1" s="3" t="s">
+      <c r="BP1" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="BP1" s="3" t="s">
+      <c r="BQ1" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BR1" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BS1" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="BT1" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="BU1" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="BV1" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="BW1" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="BX1" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="BZ1" t="s">
+      <c r="CA1" t="s">
         <v>264</v>
       </c>
-      <c r="CA1" s="4" t="s">
+      <c r="CB1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="CB1" t="s">
+      <c r="CC1" t="s">
         <v>56</v>
       </c>
-      <c r="CC1" t="s">
+      <c r="CD1" t="s">
         <v>57</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CE1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:82" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>319</v>
       </c>
@@ -6016,69 +6213,72 @@
       </c>
       <c r="BE2" s="17"/>
       <c r="BF2" s="17" t="s">
+        <v>380</v>
+      </c>
+      <c r="BG2" s="17" t="s">
+        <v>382</v>
+      </c>
+      <c r="BH2" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="BG2" s="17" t="s">
-        <v>164</v>
-      </c>
-      <c r="BH2" s="17" t="s">
+      <c r="BI2" s="17" t="s">
         <v>321</v>
       </c>
-      <c r="BI2" s="4" t="s">
+      <c r="BJ2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BJ2" s="4" t="s">
+      <c r="BK2" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="BK2" s="4" t="s">
+      <c r="BL2" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="BL2" s="4" t="s">
+      <c r="BM2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="BM2" s="4" t="s">
+      <c r="BN2" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="BN2" s="4" t="s">
+      <c r="BO2" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="BO2" s="4" t="s">
+      <c r="BP2" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="BP2" s="4" t="s">
+      <c r="BQ2" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="BQ2" s="4" t="s">
+      <c r="BR2" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="BR2" s="4" t="s">
+      <c r="BS2" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="BS2" s="4" t="s">
+      <c r="BT2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="BT2" s="4" t="s">
+      <c r="BU2" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="BU2" s="4" t="s">
+      <c r="BV2" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="BV2" s="4" t="s">
+      <c r="BW2" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="BW2" s="4" t="s">
+      <c r="BX2" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="BX2" s="4" t="s">
+      <c r="BY2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="BY2" s="4" t="s">
+      <c r="BZ2" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="BZ2"/>
       <c r="CA2"/>
       <c r="CB2"/>
       <c r="CC2"/>
+      <c r="CD2"/>
     </row>
   </sheetData>
   <dataValidations count="9">
@@ -6100,10 +6300,10 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2">
       <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BL2">
-      <formula1>"Yes,No"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK2">
       <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2">
@@ -6122,8 +6322,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CH2"/>
   <sheetViews>
-    <sheetView topLeftCell="CA1" workbookViewId="0">
-      <selection activeCell="CE3" sqref="CE3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6499,7 +6699,7 @@
         <v>166</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>167</v>
@@ -6715,8 +6915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CD2"/>
   <sheetViews>
-    <sheetView topLeftCell="AX1" workbookViewId="0">
-      <selection activeCell="BE22" sqref="BE22"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7287,8 +7487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CE2"/>
   <sheetViews>
-    <sheetView topLeftCell="BQ1" workbookViewId="0">
-      <selection activeCell="BV18" sqref="BV18"/>
+    <sheetView topLeftCell="BV1" workbookViewId="0">
+      <selection activeCell="CC14" sqref="CC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7625,7 +7825,7 @@
     </row>
     <row r="2" spans="1:83" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>281</v>
+        <v>359</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>296</v>
@@ -7655,7 +7855,7 @@
         <v>166</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>260</v>
+        <v>367</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>167</v>
@@ -7815,6 +8015,18 @@
       </c>
       <c r="BZ2" s="4" t="s">
         <v>245</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>367</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>369</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>83</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>370</v>
       </c>
     </row>
   </sheetData>
@@ -7862,8 +8074,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8204,18 +8416,18 @@
       <c r="L2" s="10"/>
       <c r="M2" s="12" t="str">
         <f ca="1">Sheet1!A2</f>
-        <v>HLNew Lead 24</v>
+        <v>HLNew Lead 48</v>
       </c>
       <c r="N2" s="12" t="s">
         <v>173</v>
       </c>
       <c r="O2" s="10" t="str">
         <f ca="1">Sheet1!C2</f>
-        <v>HLNewLead24@gmail.com</v>
+        <v>HLNewLead48@gmail.com</v>
       </c>
       <c r="P2" s="10" t="str">
         <f ca="1">Sheet1!D2</f>
-        <v>12111958</v>
+        <v>22111973</v>
       </c>
       <c r="Q2" s="13" t="s">
         <v>76</v>
@@ -8250,7 +8462,7 @@
       <c r="AC2" s="10"/>
       <c r="AD2" s="10" t="str">
         <f ca="1">Sheet1!E2</f>
-        <v>UTMDU1742T</v>
+        <v>PVDEE4386T</v>
       </c>
       <c r="AE2" s="10" t="s">
         <v>36</v>
@@ -8540,10 +8752,2432 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CH2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I21" sqref="I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="22" width="24" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="25.42578125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="4" customWidth="1"/>
+    <col min="31" max="32" width="27.5703125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="17.7109375" style="4" customWidth="1"/>
+    <col min="37" max="38" width="19.42578125" style="4" customWidth="1"/>
+    <col min="39" max="40" width="34.42578125" style="5" customWidth="1"/>
+    <col min="41" max="41" width="21.7109375" style="4" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" style="4" customWidth="1"/>
+    <col min="43" max="43" width="26.7109375" style="4" customWidth="1"/>
+    <col min="44" max="45" width="19.140625" style="4" customWidth="1"/>
+    <col min="46" max="46" width="16.5703125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="21.42578125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="12.85546875" style="4" customWidth="1"/>
+    <col min="49" max="49" width="30.7109375" style="4" customWidth="1"/>
+    <col min="50" max="50" width="91.42578125" style="4" customWidth="1"/>
+    <col min="51" max="51" width="10.5703125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="13" style="4" customWidth="1"/>
+    <col min="53" max="53" width="13.28515625" style="4" customWidth="1"/>
+    <col min="54" max="54" width="15.28515625" style="4" customWidth="1"/>
+    <col min="55" max="55" width="12.42578125" style="4" customWidth="1"/>
+    <col min="56" max="56" width="9.140625" style="4"/>
+    <col min="57" max="57" width="19.85546875" style="4" customWidth="1"/>
+    <col min="58" max="58" width="25.7109375" style="4" customWidth="1"/>
+    <col min="59" max="59" width="13.42578125" style="4" customWidth="1"/>
+    <col min="60" max="60" width="15" style="4" customWidth="1"/>
+    <col min="61" max="61" width="20.140625" style="4" customWidth="1"/>
+    <col min="62" max="62" width="21.7109375" style="4" customWidth="1"/>
+    <col min="63" max="63" width="17.28515625" style="4" customWidth="1"/>
+    <col min="64" max="64" width="17.85546875" style="4" customWidth="1"/>
+    <col min="65" max="65" width="32.5703125" style="4" customWidth="1"/>
+    <col min="66" max="66" width="24.7109375" style="4" customWidth="1"/>
+    <col min="67" max="67" width="26.5703125" style="4" customWidth="1"/>
+    <col min="68" max="68" width="32.7109375" style="4" customWidth="1"/>
+    <col min="69" max="69" width="18.42578125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="17.85546875" style="4" customWidth="1"/>
+    <col min="71" max="71" width="17.140625" style="4" customWidth="1"/>
+    <col min="72" max="72" width="18.5703125" style="4" customWidth="1"/>
+    <col min="73" max="73" width="18.42578125" style="4" customWidth="1"/>
+    <col min="74" max="75" width="17.85546875" style="4" customWidth="1"/>
+    <col min="76" max="78" width="25.28515625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="17.28515625" style="4" customWidth="1"/>
+    <col min="80" max="80" width="19.28515625" style="4" customWidth="1"/>
+    <col min="81" max="81" width="24.140625" style="4" customWidth="1"/>
+    <col min="82" max="82" width="16.28515625" style="4" customWidth="1"/>
+    <col min="83" max="83" width="16" style="4" customWidth="1"/>
+    <col min="84" max="84" width="19.42578125" style="4" customWidth="1"/>
+    <col min="85" max="85" width="19.85546875" style="4" customWidth="1"/>
+    <col min="86" max="86" width="17.5703125" style="4" customWidth="1"/>
+    <col min="87" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:86" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="CA1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="CB1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="CC1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>264</v>
+      </c>
+      <c r="CE1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="CF1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CG1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CH1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:86" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="U2" s="23">
+        <v>4200000</v>
+      </c>
+      <c r="V2" s="23"/>
+      <c r="W2" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AN2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ2" s="17"/>
+      <c r="AR2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AS2" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="AT2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV2" s="17"/>
+      <c r="AW2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX2" s="17"/>
+      <c r="AY2" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="AZ2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="BA2" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="BB2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="BD2" s="17"/>
+      <c r="BE2" s="17"/>
+      <c r="BF2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="BG2" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI2" s="17"/>
+      <c r="BJ2" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="BK2" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="BL2" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="BM2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BX2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="BY2" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="BZ2" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="CA2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="CB2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="CD2"/>
+      <c r="CE2"/>
+      <c r="CF2"/>
+      <c r="CG2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
+      <formula1>"Buying new property,Buying resale property,Construction of property,Renovation of existing property"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2">
+      <formula1>"January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CE2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="BZ24" sqref="BZ24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="21" width="24" style="4" customWidth="1"/>
+    <col min="22" max="22" width="25.140625" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="25.42578125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="4" customWidth="1"/>
+    <col min="31" max="32" width="27.5703125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="17.7109375" style="4" customWidth="1"/>
+    <col min="37" max="38" width="19.42578125" style="4" customWidth="1"/>
+    <col min="39" max="40" width="34.42578125" style="5" customWidth="1"/>
+    <col min="41" max="41" width="21.7109375" style="4" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" style="4" customWidth="1"/>
+    <col min="43" max="44" width="26.7109375" style="4" customWidth="1"/>
+    <col min="45" max="46" width="19.140625" style="4" customWidth="1"/>
+    <col min="47" max="47" width="16.5703125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="21.42578125" style="4" customWidth="1"/>
+    <col min="49" max="49" width="12.85546875" style="4" customWidth="1"/>
+    <col min="50" max="50" width="30.7109375" style="4" customWidth="1"/>
+    <col min="51" max="51" width="32.140625" style="4" customWidth="1"/>
+    <col min="52" max="52" width="10.5703125" style="4" customWidth="1"/>
+    <col min="53" max="53" width="13" style="4" customWidth="1"/>
+    <col min="54" max="54" width="13.28515625" style="4" customWidth="1"/>
+    <col min="55" max="55" width="15.28515625" style="4" customWidth="1"/>
+    <col min="56" max="56" width="12.42578125" style="4" customWidth="1"/>
+    <col min="57" max="57" width="9.140625" style="4"/>
+    <col min="58" max="58" width="19.85546875" style="4" customWidth="1"/>
+    <col min="59" max="59" width="25.7109375" style="4" customWidth="1"/>
+    <col min="60" max="60" width="13.42578125" style="4" customWidth="1"/>
+    <col min="61" max="61" width="15" style="4" customWidth="1"/>
+    <col min="62" max="62" width="20.140625" style="4" customWidth="1"/>
+    <col min="63" max="63" width="21.7109375" style="4" customWidth="1"/>
+    <col min="64" max="64" width="17.28515625" style="4" customWidth="1"/>
+    <col min="65" max="65" width="17.85546875" style="4" customWidth="1"/>
+    <col min="66" max="66" width="24.140625" style="4" customWidth="1"/>
+    <col min="67" max="67" width="24.7109375" style="4" customWidth="1"/>
+    <col min="68" max="68" width="29.5703125" style="4" customWidth="1"/>
+    <col min="69" max="69" width="32.7109375" style="4" customWidth="1"/>
+    <col min="70" max="70" width="18.42578125" style="4" customWidth="1"/>
+    <col min="71" max="71" width="17.85546875" style="4" customWidth="1"/>
+    <col min="72" max="72" width="17.140625" style="4" customWidth="1"/>
+    <col min="73" max="73" width="18.5703125" style="4" customWidth="1"/>
+    <col min="74" max="74" width="18.42578125" style="4" customWidth="1"/>
+    <col min="75" max="75" width="17.85546875" style="4" customWidth="1"/>
+    <col min="76" max="76" width="17.28515625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="19.28515625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="24.140625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="16.28515625" style="4" customWidth="1"/>
+    <col min="80" max="80" width="16" style="4" customWidth="1"/>
+    <col min="81" max="81" width="19.42578125" style="4" customWidth="1"/>
+    <col min="82" max="82" width="19.85546875" style="4" customWidth="1"/>
+    <col min="83" max="83" width="17.5703125" style="4" customWidth="1"/>
+    <col min="84" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:83" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AT1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AU1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AV1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AX1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="BM1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>264</v>
+      </c>
+      <c r="CB1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:83" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>379</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="23">
+        <v>4200000</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="V2" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AN2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ2" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="AR2" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="AS2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AT2" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="AU2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AW2" s="17"/>
+      <c r="AX2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AY2" s="17"/>
+      <c r="AZ2" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="BA2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="BB2" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BD2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="BE2" s="17"/>
+      <c r="BF2" s="17"/>
+      <c r="BG2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="BH2" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="BI2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BJ2" s="17"/>
+      <c r="BK2" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="BL2" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="BM2" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="BX2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="BY2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="BZ2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="CA2"/>
+      <c r="CB2"/>
+      <c r="CC2"/>
+      <c r="CD2"/>
+    </row>
+  </sheetData>
+  <dataValidations count="10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BQ2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BG2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AQ2">
+      <formula1>"Individual,Non-Individual"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR2">
+      <formula1>"Less than 3 years,3 or more years"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
+      <formula1>"Buying new property,Buying resale property,Construction of property,Renovation of existing property"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA2">
+      <formula1>"January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CE2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="34.7109375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="21" width="24" style="4" customWidth="1"/>
+    <col min="22" max="22" width="15.7109375" style="4" customWidth="1"/>
+    <col min="23" max="23" width="20.85546875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="29.140625" style="4" customWidth="1"/>
+    <col min="25" max="25" width="16.7109375" style="4" customWidth="1"/>
+    <col min="26" max="27" width="27.5703125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="16.7109375" style="4" customWidth="1"/>
+    <col min="29" max="29" width="11.140625" style="4" customWidth="1"/>
+    <col min="30" max="30" width="24.5703125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="17.7109375" style="4" customWidth="1"/>
+    <col min="32" max="33" width="19.42578125" style="4" customWidth="1"/>
+    <col min="34" max="35" width="34.42578125" style="5" customWidth="1"/>
+    <col min="36" max="36" width="21.7109375" style="4" customWidth="1"/>
+    <col min="37" max="37" width="24.140625" style="4" customWidth="1"/>
+    <col min="38" max="39" width="26.7109375" style="4" customWidth="1"/>
+    <col min="40" max="41" width="19.140625" style="4" customWidth="1"/>
+    <col min="42" max="42" width="16.5703125" style="4" customWidth="1"/>
+    <col min="43" max="43" width="21.42578125" style="4" customWidth="1"/>
+    <col min="44" max="44" width="12.85546875" style="4" customWidth="1"/>
+    <col min="45" max="45" width="30.7109375" style="4" customWidth="1"/>
+    <col min="46" max="46" width="35.42578125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="10.5703125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="13" style="4" customWidth="1"/>
+    <col min="49" max="49" width="13.28515625" style="4" customWidth="1"/>
+    <col min="50" max="50" width="15.28515625" style="4" customWidth="1"/>
+    <col min="51" max="51" width="12.42578125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="17.7109375" style="4" customWidth="1"/>
+    <col min="53" max="54" width="25.7109375" style="4" customWidth="1"/>
+    <col min="55" max="55" width="13.42578125" style="4" customWidth="1"/>
+    <col min="56" max="56" width="15" style="4" customWidth="1"/>
+    <col min="57" max="58" width="20.140625" style="4" customWidth="1"/>
+    <col min="59" max="59" width="27.140625" style="4" customWidth="1"/>
+    <col min="60" max="60" width="17.28515625" style="4" customWidth="1"/>
+    <col min="61" max="61" width="17.85546875" style="4" customWidth="1"/>
+    <col min="62" max="62" width="32.5703125" style="4" customWidth="1"/>
+    <col min="63" max="63" width="24.7109375" style="4" customWidth="1"/>
+    <col min="64" max="64" width="26.5703125" style="4" customWidth="1"/>
+    <col min="65" max="65" width="32.7109375" style="4" customWidth="1"/>
+    <col min="66" max="66" width="18.42578125" style="4" customWidth="1"/>
+    <col min="67" max="67" width="17.85546875" style="4" customWidth="1"/>
+    <col min="68" max="68" width="17.140625" style="4" customWidth="1"/>
+    <col min="69" max="69" width="18.5703125" style="4" customWidth="1"/>
+    <col min="70" max="70" width="18.42578125" style="4" customWidth="1"/>
+    <col min="71" max="72" width="17.85546875" style="4" customWidth="1"/>
+    <col min="73" max="75" width="25.28515625" style="4" customWidth="1"/>
+    <col min="76" max="76" width="17.28515625" style="4" customWidth="1"/>
+    <col min="77" max="77" width="19.28515625" style="4" customWidth="1"/>
+    <col min="78" max="78" width="24.140625" style="4" customWidth="1"/>
+    <col min="79" max="79" width="16.28515625" style="4" customWidth="1"/>
+    <col min="80" max="80" width="16" style="4" customWidth="1"/>
+    <col min="81" max="81" width="19.42578125" style="4" customWidth="1"/>
+    <col min="82" max="82" width="19.85546875" style="4" customWidth="1"/>
+    <col min="83" max="83" width="17.5703125" style="4" customWidth="1"/>
+    <col min="84" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:83" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AH1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AM1" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AP1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AQ1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AR1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AU1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="AV1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="AW1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="AX1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>289</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BJ1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="BK1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BL1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="CA1" t="s">
+        <v>264</v>
+      </c>
+      <c r="CB1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="CC1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CD1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CE1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:83" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="24" t="s">
+        <v>291</v>
+      </c>
+      <c r="U2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="V2" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="W2" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AB2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AE2" s="17"/>
+      <c r="AF2" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AH2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AI2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="AM2" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="AN2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AO2" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="AP2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AQ2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AR2" s="17"/>
+      <c r="AS2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AT2" s="17"/>
+      <c r="AU2" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="AW2" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="AX2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="AY2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ2" s="17"/>
+      <c r="BA2" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="BB2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="BD2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BE2" s="17"/>
+      <c r="BF2" s="17" t="s">
+        <v>380</v>
+      </c>
+      <c r="BG2" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="BH2" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="BI2" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="BJ2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BK2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="BL2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="BM2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="BX2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="BY2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="BZ2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>378</v>
+      </c>
+      <c r="CB2">
+        <v>105123</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>83</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV2">
+      <formula1>" January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BL2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BM2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U2">
+      <formula1>"Residential,Commercial"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
+      <formula1>"Less than 3 years,3 or more years"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CR2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="BN1" workbookViewId="0">
+      <selection activeCell="BQ22" sqref="BQ22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="14.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="14.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="12" style="4" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16" width="30.7109375" style="4" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" style="4" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" style="4" customWidth="1"/>
+    <col min="19" max="22" width="24" style="4" customWidth="1"/>
+    <col min="23" max="23" width="15.7109375" style="4" customWidth="1"/>
+    <col min="24" max="24" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="22.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="25.42578125" style="4" customWidth="1"/>
+    <col min="29" max="29" width="17.85546875" style="4" customWidth="1"/>
+    <col min="30" max="30" width="16.7109375" style="4" customWidth="1"/>
+    <col min="31" max="32" width="27.5703125" style="4" customWidth="1"/>
+    <col min="33" max="33" width="16.7109375" style="4" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="24.5703125" style="4" customWidth="1"/>
+    <col min="36" max="36" width="17.7109375" style="4" customWidth="1"/>
+    <col min="37" max="38" width="19.42578125" style="4" customWidth="1"/>
+    <col min="39" max="40" width="34.42578125" style="5" customWidth="1"/>
+    <col min="41" max="41" width="21.7109375" style="4" customWidth="1"/>
+    <col min="42" max="42" width="24.140625" style="4" customWidth="1"/>
+    <col min="43" max="43" width="26.7109375" style="4" customWidth="1"/>
+    <col min="44" max="45" width="19.140625" style="4" customWidth="1"/>
+    <col min="46" max="46" width="16.5703125" style="4" customWidth="1"/>
+    <col min="47" max="47" width="21.42578125" style="4" customWidth="1"/>
+    <col min="48" max="48" width="12.85546875" style="4" customWidth="1"/>
+    <col min="49" max="49" width="30.7109375" style="4" customWidth="1"/>
+    <col min="50" max="50" width="18.5703125" style="4" customWidth="1"/>
+    <col min="51" max="51" width="10.5703125" style="4" customWidth="1"/>
+    <col min="52" max="52" width="13" style="4" customWidth="1"/>
+    <col min="53" max="53" width="13.28515625" style="4" customWidth="1"/>
+    <col min="54" max="54" width="15.28515625" style="4" customWidth="1"/>
+    <col min="55" max="55" width="12.42578125" style="4" customWidth="1"/>
+    <col min="56" max="56" width="9.140625" style="4"/>
+    <col min="57" max="57" width="19.85546875" style="4" customWidth="1"/>
+    <col min="58" max="58" width="25.7109375" style="4" customWidth="1"/>
+    <col min="59" max="59" width="13.42578125" style="4" customWidth="1"/>
+    <col min="60" max="60" width="15" style="4" customWidth="1"/>
+    <col min="61" max="61" width="16.5703125" style="4" customWidth="1"/>
+    <col min="62" max="62" width="21.7109375" style="4" customWidth="1"/>
+    <col min="63" max="63" width="17.28515625" style="4" customWidth="1"/>
+    <col min="64" max="64" width="17.85546875" style="4" customWidth="1"/>
+    <col min="65" max="65" width="32.5703125" style="4" customWidth="1"/>
+    <col min="66" max="66" width="24.7109375" style="4" customWidth="1"/>
+    <col min="67" max="67" width="33" style="4" customWidth="1"/>
+    <col min="68" max="69" width="26.140625" style="4" customWidth="1"/>
+    <col min="70" max="70" width="20.28515625" style="4" customWidth="1"/>
+    <col min="71" max="71" width="16.140625" style="4" customWidth="1"/>
+    <col min="72" max="72" width="21.85546875" style="4" customWidth="1"/>
+    <col min="73" max="73" width="20.140625" style="4" customWidth="1"/>
+    <col min="74" max="76" width="18.5703125" style="4" customWidth="1"/>
+    <col min="77" max="77" width="22.5703125" style="4" customWidth="1"/>
+    <col min="78" max="78" width="27.85546875" style="4" customWidth="1"/>
+    <col min="79" max="79" width="18.42578125" style="4" customWidth="1"/>
+    <col min="80" max="80" width="17.85546875" style="4" customWidth="1"/>
+    <col min="81" max="81" width="17.140625" style="4" customWidth="1"/>
+    <col min="82" max="82" width="18.5703125" style="4" customWidth="1"/>
+    <col min="83" max="83" width="18.42578125" style="4" customWidth="1"/>
+    <col min="84" max="85" width="17.85546875" style="4" customWidth="1"/>
+    <col min="86" max="88" width="25.28515625" style="4" customWidth="1"/>
+    <col min="89" max="89" width="17.28515625" style="4" customWidth="1"/>
+    <col min="90" max="90" width="19.28515625" style="4" customWidth="1"/>
+    <col min="91" max="91" width="24.140625" style="4" customWidth="1"/>
+    <col min="92" max="92" width="16.28515625" style="4" customWidth="1"/>
+    <col min="93" max="93" width="16" style="4" customWidth="1"/>
+    <col min="94" max="94" width="19.42578125" style="4" customWidth="1"/>
+    <col min="95" max="95" width="19.85546875" style="4" customWidth="1"/>
+    <col min="96" max="96" width="17.5703125" style="4" customWidth="1"/>
+    <col min="97" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:96" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="AC1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AD1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="AF1" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="AG1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="AH1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="AJ1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN1" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="AO1" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AP1" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="AQ1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="AS1" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AU1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AV1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AW1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AX1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AY1" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="AZ1" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA1" s="16" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB1" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="BC1" s="16" t="s">
+        <v>129</v>
+      </c>
+      <c r="BD1" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="BE1" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="BF1" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG1" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="BH1" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="BI1" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="BJ1" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="BK1" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="BL1" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="BM1" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="BN1" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="BO1" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="BP1" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="BX1" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="BY1" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="BZ1" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="CA1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="CB1" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="CC1" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="CD1" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="CE1" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="CF1" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="CG1" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="CH1" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="CI1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="CJ1" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="CK1" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="CL1" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="CM1" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="CN1" t="s">
+        <v>264</v>
+      </c>
+      <c r="CO1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="CP1" t="s">
+        <v>56</v>
+      </c>
+      <c r="CQ1" t="s">
+        <v>57</v>
+      </c>
+      <c r="CR1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:96" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" s="29" t="s">
+        <v>296</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>400</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="T2" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="U2" s="23">
+        <v>4200000</v>
+      </c>
+      <c r="V2" s="23"/>
+      <c r="W2" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="X2" s="47"/>
+      <c r="Y2" s="17"/>
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="17"/>
+      <c r="AD2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="AL2" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="AM2" s="20" t="s">
+        <v>153</v>
+      </c>
+      <c r="AN2" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="AO2" s="17"/>
+      <c r="AP2" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="AQ2" s="17"/>
+      <c r="AR2" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="AS2" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="AT2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="AU2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="AV2" s="17"/>
+      <c r="AW2" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="AX2" s="17"/>
+      <c r="AY2" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="AZ2" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="BA2" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="BB2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="BC2" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="BD2" s="17"/>
+      <c r="BE2" s="17"/>
+      <c r="BF2" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="BG2" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="BH2" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="BI2" s="17"/>
+      <c r="BJ2" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="BK2" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="BL2" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="BM2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="BN2" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="BO2" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="BP2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="BS2" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="BT2" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="BV2" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="BX2" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="BY2" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="BZ2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="CA2" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="CB2" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="CC2" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="CD2" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="CE2" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="CF2" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="CG2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="CH2" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="CI2" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="CJ2" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="CK2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="CL2" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="CM2" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>400</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>401</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>83</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>402</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2">
+      <formula1>"Salaried, Self employed"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CM2 BU2">
+      <formula1>"Father, Mother, Husband, Wife, Son, Daughter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2">
+      <formula1>"January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V2">
+      <formula1>"Buying new property,Buying resale property,Construction of property,Renovation of existing property"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO2">
+      <formula1>"Continue to Sanction Letter,Add Financial CO-app,Intiate Loan Deviation, Intiate ROI Deviation"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BZ2">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2">
+      <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BF2">
+      <formula1>"Indian,NRI"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2">
+      <formula1>"RM,DST"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BQ2">
+      <formula1>"Indian, NRI"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="BT2" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8579,23 +11213,23 @@
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="str">
         <f ca="1">CONCATENATE("HLNew Lead"," ",RANDBETWEEN(1,999))</f>
-        <v>HLNew Lead 24</v>
+        <v>HLNew Lead 48</v>
       </c>
       <c r="B2" s="2">
         <f ca="1">RANDBETWEEN(6789000000,9999999999)</f>
-        <v>7740625513</v>
+        <v>8297524543</v>
       </c>
       <c r="C2" s="2" t="str">
         <f ca="1">CONCATENATE(SUBSTITUTE($A2," ",""),"@gmail.com")</f>
-        <v>HLNewLead24@gmail.com</v>
+        <v>HLNewLead48@gmail.com</v>
       </c>
       <c r="D2" s="2" t="str">
         <f ca="1">CONCATENATE(RANDBETWEEN(10,30),RANDBETWEEN(10,12),RANDBETWEEN(1951,2004))</f>
-        <v>12111958</v>
+        <v>22111973</v>
       </c>
       <c r="E2" s="2" t="str">
         <f ca="1">CONCATENATE(CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),CHAR(RANDBETWEEN(65,90)),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),RANDBETWEEN(0,9),CHAR(RANDBETWEEN(65,90)))</f>
-        <v>UTMDU1742T</v>
+        <v>PVDEE4386T</v>
       </c>
       <c r="F2" s="4" t="str">
         <f ca="1">CHOOSE(RANDBETWEEN(1,2),"Male","Female")</f>
@@ -8607,7 +11241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F50"/>
   <sheetViews>
@@ -9801,18 +12435,18 @@
       <c r="M2" s="10"/>
       <c r="N2" s="12" t="str">
         <f ca="1">Sheet1!A2</f>
-        <v>HLNew Lead 24</v>
+        <v>HLNew Lead 48</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>173</v>
       </c>
       <c r="P2" s="10" t="str">
         <f ca="1">Sheet1!C2</f>
-        <v>HLNewLead24@gmail.com</v>
+        <v>HLNewLead48@gmail.com</v>
       </c>
       <c r="Q2" s="10" t="str">
         <f ca="1">Sheet1!D2</f>
-        <v>12111958</v>
+        <v>22111973</v>
       </c>
       <c r="R2" s="13" t="s">
         <v>76</v>
@@ -9847,7 +12481,7 @@
       <c r="AD2" s="10"/>
       <c r="AE2" s="10" t="str">
         <f ca="1">Sheet1!E2</f>
-        <v>UTMDU1742T</v>
+        <v>PVDEE4386T</v>
       </c>
       <c r="AF2" s="10" t="s">
         <v>36</v>
@@ -10028,10 +12662,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CH2"/>
+  <dimension ref="A1:CP2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="AP1" workbookViewId="0">
+      <selection activeCell="AW2" sqref="AW2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10078,7 +12712,7 @@
     <col min="47" max="47" width="21.42578125" style="4" customWidth="1"/>
     <col min="48" max="48" width="12.85546875" style="4" customWidth="1"/>
     <col min="49" max="49" width="30.7109375" style="4" customWidth="1"/>
-    <col min="50" max="50" width="91.42578125" style="4" customWidth="1"/>
+    <col min="50" max="50" width="18.5703125" style="4" customWidth="1"/>
     <col min="51" max="51" width="10.5703125" style="4" customWidth="1"/>
     <col min="52" max="52" width="13" style="4" customWidth="1"/>
     <col min="53" max="53" width="13.28515625" style="4" customWidth="1"/>
@@ -10089,33 +12723,39 @@
     <col min="58" max="58" width="25.7109375" style="4" customWidth="1"/>
     <col min="59" max="59" width="13.42578125" style="4" customWidth="1"/>
     <col min="60" max="60" width="15" style="4" customWidth="1"/>
-    <col min="61" max="61" width="20.140625" style="4" customWidth="1"/>
+    <col min="61" max="61" width="16.5703125" style="4" customWidth="1"/>
     <col min="62" max="62" width="21.7109375" style="4" customWidth="1"/>
     <col min="63" max="63" width="17.28515625" style="4" customWidth="1"/>
     <col min="64" max="64" width="17.85546875" style="4" customWidth="1"/>
     <col min="65" max="65" width="32.5703125" style="4" customWidth="1"/>
     <col min="66" max="66" width="24.7109375" style="4" customWidth="1"/>
-    <col min="67" max="67" width="26.5703125" style="4" customWidth="1"/>
-    <col min="68" max="68" width="32.7109375" style="4" customWidth="1"/>
-    <col min="69" max="69" width="18.42578125" style="4" customWidth="1"/>
-    <col min="70" max="70" width="17.85546875" style="4" customWidth="1"/>
-    <col min="71" max="71" width="17.140625" style="4" customWidth="1"/>
-    <col min="72" max="72" width="18.5703125" style="4" customWidth="1"/>
-    <col min="73" max="73" width="18.42578125" style="4" customWidth="1"/>
-    <col min="74" max="75" width="17.85546875" style="4" customWidth="1"/>
-    <col min="76" max="78" width="25.28515625" style="4" customWidth="1"/>
-    <col min="79" max="79" width="17.28515625" style="4" customWidth="1"/>
-    <col min="80" max="80" width="19.28515625" style="4" customWidth="1"/>
-    <col min="81" max="81" width="24.140625" style="4" customWidth="1"/>
-    <col min="82" max="82" width="16.28515625" style="4" customWidth="1"/>
-    <col min="83" max="83" width="16" style="4" customWidth="1"/>
-    <col min="84" max="84" width="19.42578125" style="4" customWidth="1"/>
-    <col min="85" max="85" width="19.85546875" style="4" customWidth="1"/>
-    <col min="86" max="86" width="17.5703125" style="4" customWidth="1"/>
-    <col min="87" max="16384" width="9.140625" style="4"/>
+    <col min="67" max="67" width="33" style="4" customWidth="1"/>
+    <col min="68" max="68" width="26.140625" style="4" customWidth="1"/>
+    <col min="69" max="69" width="20.28515625" style="4" customWidth="1"/>
+    <col min="70" max="70" width="16.140625" style="4" customWidth="1"/>
+    <col min="71" max="71" width="21.85546875" style="4" customWidth="1"/>
+    <col min="72" max="72" width="20.140625" style="4" customWidth="1"/>
+    <col min="73" max="75" width="18.5703125" style="4" customWidth="1"/>
+    <col min="76" max="76" width="27.85546875" style="4" customWidth="1"/>
+    <col min="77" max="77" width="18.42578125" style="4" customWidth="1"/>
+    <col min="78" max="78" width="17.85546875" style="4" customWidth="1"/>
+    <col min="79" max="79" width="17.140625" style="4" customWidth="1"/>
+    <col min="80" max="80" width="18.5703125" style="4" customWidth="1"/>
+    <col min="81" max="81" width="18.42578125" style="4" customWidth="1"/>
+    <col min="82" max="83" width="17.85546875" style="4" customWidth="1"/>
+    <col min="84" max="86" width="25.28515625" style="4" customWidth="1"/>
+    <col min="87" max="87" width="17.28515625" style="4" customWidth="1"/>
+    <col min="88" max="88" width="19.28515625" style="4" customWidth="1"/>
+    <col min="89" max="89" width="24.140625" style="4" customWidth="1"/>
+    <col min="90" max="90" width="16.28515625" style="4" customWidth="1"/>
+    <col min="91" max="91" width="16" style="4" customWidth="1"/>
+    <col min="92" max="92" width="19.42578125" style="4" customWidth="1"/>
+    <col min="93" max="93" width="19.85546875" style="4" customWidth="1"/>
+    <col min="94" max="94" width="17.5703125" style="4" customWidth="1"/>
+    <col min="95" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:86" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:94" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>74</v>
       </c>
@@ -10318,64 +12958,88 @@
         <v>210</v>
       </c>
       <c r="BP1" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="BQ1" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="BR1" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="BS1" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="BT1" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="BU1" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="BV1" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="BW1" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="BX1" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="BQ1" s="3" t="s">
+      <c r="BY1" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="BR1" s="3" t="s">
+      <c r="BZ1" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="BS1" s="3" t="s">
+      <c r="CA1" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="BT1" s="3" t="s">
+      <c r="CB1" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="BU1" s="3" t="s">
+      <c r="CC1" s="3" t="s">
         <v>221</v>
       </c>
-      <c r="BV1" s="3" t="s">
+      <c r="CD1" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="BW1" s="3" t="s">
+      <c r="CE1" s="3" t="s">
         <v>300</v>
       </c>
-      <c r="BX1" s="3" t="s">
+      <c r="CF1" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="BY1" s="3" t="s">
+      <c r="CG1" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="BZ1" s="3" t="s">
+      <c r="CH1" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="CA1" s="3" t="s">
+      <c r="CI1" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="CB1" s="3" t="s">
+      <c r="CJ1" s="3" t="s">
         <v>229</v>
       </c>
-      <c r="CC1" s="3" t="s">
+      <c r="CK1" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="CD1" t="s">
+      <c r="CL1" t="s">
         <v>264</v>
       </c>
-      <c r="CE1" s="4" t="s">
+      <c r="CM1" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="CF1" t="s">
+      <c r="CN1" t="s">
         <v>56</v>
       </c>
-      <c r="CG1" t="s">
+      <c r="CO1" t="s">
         <v>57</v>
       </c>
-      <c r="CH1" t="s">
+      <c r="CP1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:86" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:94" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>101</v>
       </c>
@@ -10407,7 +13071,7 @@
         <v>166</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>327</v>
+        <v>400</v>
       </c>
       <c r="P2" s="19" t="s">
         <v>167</v>
@@ -10485,13 +13149,13 @@
       </c>
       <c r="AX2" s="17"/>
       <c r="AY2" s="17" t="s">
-        <v>155</v>
+        <v>265</v>
       </c>
       <c r="AZ2" s="17" t="s">
         <v>322</v>
       </c>
       <c r="BA2" s="17" t="s">
-        <v>156</v>
+        <v>266</v>
       </c>
       <c r="BB2" s="17" t="s">
         <v>128</v>
@@ -10530,62 +13194,83 @@
         <v>211</v>
       </c>
       <c r="BP2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="BQ2" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="BR2" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="BS2" s="29" t="s">
+        <v>392</v>
+      </c>
+      <c r="BT2" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="BU2" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="BW2" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="BX2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="BQ2" s="4" t="s">
+      <c r="BY2" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="BR2" s="4" t="s">
+      <c r="BZ2" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="BS2" s="4" t="s">
+      <c r="CA2" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="BT2" s="4" t="s">
+      <c r="CB2" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="BU2" s="4" t="s">
+      <c r="CC2" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="BV2" s="4" t="s">
+      <c r="CD2" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="BW2" s="4" t="s">
+      <c r="CE2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="BX2" s="4" t="s">
+      <c r="CF2" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="BY2" s="4" t="s">
+      <c r="CG2" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="BZ2" s="4" t="s">
+      <c r="CH2" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="CA2" s="4" t="s">
+      <c r="CI2" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="CB2" s="4" t="s">
+      <c r="CJ2" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="CC2" s="4" t="s">
+      <c r="CK2" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="CD2" t="s">
+      <c r="CL2" t="s">
         <v>324</v>
       </c>
-      <c r="CE2" t="s">
+      <c r="CM2" t="s">
         <v>325</v>
       </c>
-      <c r="CF2" t="s">
+      <c r="CN2" t="s">
         <v>83</v>
       </c>
-      <c r="CG2" t="s">
+      <c r="CO2" t="s">
         <v>326</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="10">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
       <formula1>"Home Loan,Balance Transfer/BT+Top up,Only Top up,Kotak Smart Home,Home Loan Overdraft"</formula1>
     </dataValidation>
@@ -10598,7 +13283,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AI2">
       <formula1>"Annual household income is less than Rs. 6 lacs,Annual household income is between Rs. 6 lacs to Rs.12 lacs,Annual household income is between Rs. 12 lacs to Rs.18 lacs"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX2">
       <formula1>"Yes,No"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO2">
@@ -10609,13 +13294,20 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AZ2">
       <formula1>"January , February , March , April,  May , June , July , August , September , October , November , December "</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CK2 BT2">
+      <formula1>"Father, Mother, Husband, Wife, Son, Daughter"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP2">
+      <formula1>"Salaried, Self employed"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="BS2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -11771,8 +14463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CF2"/>
   <sheetViews>
-    <sheetView topLeftCell="BB1" workbookViewId="0">
-      <selection activeCell="BH23" sqref="BH23"/>
+    <sheetView topLeftCell="BN1" workbookViewId="0">
+      <selection activeCell="BN15" sqref="BN15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12262,10 +14954,10 @@
         <v>292</v>
       </c>
       <c r="BM2" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="BN2" s="17" t="s">
-        <v>165</v>
+        <v>317</v>
       </c>
       <c r="BO2" s="4" t="s">
         <v>49</v>

</xml_diff>